<commit_message>
fix M1 run control file
</commit_message>
<xml_diff>
--- a/IO_M1/RunControl_M1.xlsx
+++ b/IO_M1/RunControl_M1.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\PenSim-Projects\Model_Main\IO_M1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\Model_Main\IO_M1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TOC" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="227">
   <si>
     <t>Sheet #</t>
   </si>
@@ -497,9 +497,6 @@
   </si>
   <si>
     <t>return_type</t>
-  </si>
-  <si>
-    <t>internal</t>
   </si>
   <si>
     <t>start</t>
@@ -846,7 +843,7 @@
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -892,19 +889,12 @@
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -913,10 +903,16 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1279,14 +1275,14 @@
       <selection pane="bottomRight" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.5546875"/>
-    <col min="2" max="2" width="16.6640625"/>
-    <col min="3" max="1025" width="8.5546875"/>
+    <col min="1" max="1" width="7.5703125"/>
+    <col min="2" max="2" width="16.7109375"/>
+    <col min="3" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1294,7 +1290,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1302,7 +1298,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -1310,7 +1306,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -1337,77 +1333,77 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1025" width="8.5546875"/>
+    <col min="1" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>21</v>
       </c>
@@ -1423,35 +1419,35 @@
   <dimension ref="A1:AQ31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="AC6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="U1" sqref="U1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="AK33" sqref="AK33"/>
+      <selection pane="bottomRight" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="54.44140625"/>
-    <col min="2" max="2" width="98.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="9" width="24.44140625"/>
-    <col min="10" max="11" width="17.44140625"/>
-    <col min="12" max="12" width="16.109375"/>
-    <col min="13" max="14" width="21.44140625"/>
-    <col min="15" max="15" width="24.5546875"/>
+    <col min="1" max="1" width="54.42578125"/>
+    <col min="2" max="2" width="98.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="9" width="24.42578125"/>
+    <col min="10" max="11" width="17.42578125"/>
+    <col min="12" max="12" width="16.140625"/>
+    <col min="13" max="14" width="21.42578125"/>
+    <col min="15" max="15" width="24.5703125"/>
     <col min="16" max="16" width="16"/>
-    <col min="17" max="21" width="12.6640625"/>
-    <col min="22" max="22" width="11.109375" customWidth="1"/>
-    <col min="23" max="32" width="12.6640625"/>
+    <col min="17" max="21" width="12.7109375"/>
+    <col min="22" max="22" width="11.140625" customWidth="1"/>
+    <col min="23" max="32" width="12.7109375"/>
     <col min="35" max="35" width="9" customWidth="1"/>
     <col min="37" max="37" width="12" customWidth="1"/>
-    <col min="38" max="38" width="12.6640625"/>
-    <col min="39" max="40" width="27.109375"/>
-    <col min="41" max="41" width="26.88671875"/>
+    <col min="38" max="38" width="12.7109375"/>
+    <col min="39" max="40" width="27.140625"/>
+    <col min="41" max="41" width="26.85546875"/>
     <col min="43" max="43" width="16"/>
-    <col min="44" max="1030" width="8.5546875"/>
+    <col min="44" max="1030" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:43" x14ac:dyDescent="0.25">
       <c r="AC1" s="1" t="s">
         <v>22</v>
       </c>
@@ -1462,7 +1458,7 @@
       <c r="AH1" s="1"/>
       <c r="AI1" s="1"/>
     </row>
-    <row r="2" spans="1:43" s="4" customFormat="1" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:43" s="4" customFormat="1" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>23</v>
       </c>
@@ -1524,13 +1520,13 @@
         <v>40</v>
       </c>
       <c r="AH2" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="AI2" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="AJ2" s="6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="AK2" s="6"/>
       <c r="AL2" s="4" t="s">
@@ -1543,7 +1539,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:43" ht="42" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:43" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>43</v>
       </c>
@@ -1578,7 +1574,7 @@
         <v>53</v>
       </c>
       <c r="AJ3" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="AK3" s="4"/>
       <c r="AN3" s="4" t="s">
@@ -1594,69 +1590,69 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:43" s="8" customFormat="1" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="29" t="s">
+    <row r="4" spans="1:43" s="8" customFormat="1" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="B4" s="29"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="30" t="s">
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="E4" s="30"/>
-      <c r="F4" s="31" t="s">
+      <c r="E4" s="33"/>
+      <c r="F4" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="G4" s="31"/>
-      <c r="H4" s="32" t="s">
+      <c r="G4" s="34"/>
+      <c r="H4" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="I4" s="32"/>
-      <c r="J4" s="33" t="s">
+      <c r="I4" s="29"/>
+      <c r="J4" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="K4" s="33"/>
-      <c r="L4" s="32" t="s">
+      <c r="K4" s="30"/>
+      <c r="L4" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="M4" s="32"/>
-      <c r="N4" s="32"/>
-      <c r="O4" s="32"/>
-      <c r="P4" s="32"/>
-      <c r="Q4" s="32"/>
-      <c r="R4" s="32"/>
-      <c r="S4" s="33" t="s">
+      <c r="M4" s="29"/>
+      <c r="N4" s="29"/>
+      <c r="O4" s="29"/>
+      <c r="P4" s="29"/>
+      <c r="Q4" s="29"/>
+      <c r="R4" s="29"/>
+      <c r="S4" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="T4" s="33"/>
-      <c r="U4" s="33"/>
-      <c r="V4" s="34" t="s">
+      <c r="T4" s="30"/>
+      <c r="U4" s="30"/>
+      <c r="V4" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="W4" s="34"/>
-      <c r="X4" s="34"/>
+      <c r="W4" s="28"/>
+      <c r="X4" s="28"/>
       <c r="Y4" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="Z4" s="29" t="s">
+      <c r="Z4" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="AA4" s="29"/>
-      <c r="AB4" s="29"/>
-      <c r="AC4" s="35" t="s">
+      <c r="AA4" s="31"/>
+      <c r="AB4" s="31"/>
+      <c r="AC4" s="32" t="s">
         <v>68</v>
       </c>
-      <c r="AD4" s="35"/>
-      <c r="AE4" s="35"/>
-      <c r="AF4" s="35"/>
+      <c r="AD4" s="32"/>
+      <c r="AE4" s="32"/>
+      <c r="AF4" s="32"/>
       <c r="AG4" s="17"/>
-      <c r="AH4" s="27"/>
+      <c r="AH4" s="26"/>
       <c r="AI4" s="23"/>
-      <c r="AJ4" s="34" t="s">
+      <c r="AJ4" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="AK4" s="34"/>
-      <c r="AL4" s="34"/>
+      <c r="AK4" s="28"/>
+      <c r="AL4" s="28"/>
       <c r="AM4" s="24" t="s">
         <v>70</v>
       </c>
@@ -1665,7 +1661,7 @@
       <c r="AP4" s="24"/>
       <c r="AQ4" s="24"/>
     </row>
-    <row r="5" spans="1:43" s="10" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:43" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>71</v>
       </c>
@@ -1763,19 +1759,19 @@
         <v>101</v>
       </c>
       <c r="AG5" s="9" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="AH5" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="AI5" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="AJ5" s="9" t="s">
         <v>106</v>
       </c>
       <c r="AK5" s="9" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="AL5" s="9" t="s">
         <v>102</v>
@@ -1796,16 +1792,15 @@
         <v>108</v>
       </c>
     </row>
-    <row r="6" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C6" s="11" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6" t="s">
         <v>109</v>
@@ -1823,7 +1818,7 @@
         <v>149</v>
       </c>
       <c r="I6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J6" s="12">
         <v>0</v>
@@ -1862,7 +1857,7 @@
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="V6" s="12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="W6" s="12">
         <v>7.4999999999999997E-2</v>
@@ -1874,7 +1869,7 @@
         <v>112</v>
       </c>
       <c r="Z6" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="AA6" s="2" t="s">
         <v>114</v>
@@ -1904,7 +1899,7 @@
         <v>0</v>
       </c>
       <c r="AJ6" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AK6" s="19">
         <v>1</v>
@@ -1928,16 +1923,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C7" s="11" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D7" t="s">
         <v>109</v>
@@ -1955,7 +1949,7 @@
         <v>149</v>
       </c>
       <c r="I7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J7" s="12">
         <v>0</v>
@@ -1993,8 +1987,8 @@
       <c r="U7" s="12">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="V7" t="s">
-        <v>159</v>
+      <c r="V7" s="12" t="s">
+        <v>158</v>
       </c>
       <c r="W7" s="12">
         <v>7.4999999999999997E-2</v>
@@ -2036,7 +2030,7 @@
         <v>0</v>
       </c>
       <c r="AJ7" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AK7" s="19">
         <v>1</v>
@@ -2060,16 +2054,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C8" s="11" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8" t="s">
         <v>109</v>
@@ -2087,7 +2080,7 @@
         <v>149</v>
       </c>
       <c r="I8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J8" s="12">
         <v>0</v>
@@ -2126,7 +2119,7 @@
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="V8" s="12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="W8" s="12">
         <v>7.4999999999999997E-2</v>
@@ -2168,7 +2161,7 @@
         <v>0</v>
       </c>
       <c r="AJ8" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AK8" s="19">
         <v>1</v>
@@ -2192,16 +2185,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C9" s="11" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9" t="s">
         <v>109</v>
@@ -2219,7 +2211,7 @@
         <v>149</v>
       </c>
       <c r="I9" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J9" s="12">
         <v>0</v>
@@ -2258,7 +2250,7 @@
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="V9" s="12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="W9" s="12">
         <v>7.4999999999999997E-2</v>
@@ -2273,7 +2265,7 @@
         <v>113</v>
       </c>
       <c r="AA9" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="AB9">
         <v>30</v>
@@ -2300,7 +2292,7 @@
         <v>0</v>
       </c>
       <c r="AJ9" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AK9" s="19">
         <v>1</v>
@@ -2324,12 +2316,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B10" s="22" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C10" s="11" t="b">
         <f>TRUE()</f>
@@ -2351,7 +2343,7 @@
         <v>149</v>
       </c>
       <c r="I10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J10" s="12">
         <v>0</v>
@@ -2389,8 +2381,8 @@
       <c r="U10" s="12">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="V10" s="25" t="s">
-        <v>156</v>
+      <c r="V10" s="12" t="s">
+        <v>158</v>
       </c>
       <c r="W10" s="12">
         <v>7.4999999999999997E-2</v>
@@ -2402,10 +2394,10 @@
         <v>112</v>
       </c>
       <c r="Z10" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="AA10" s="2" t="s">
         <v>163</v>
-      </c>
-      <c r="AA10" s="2" t="s">
-        <v>164</v>
       </c>
       <c r="AB10">
         <v>30</v>
@@ -2432,7 +2424,7 @@
         <v>0</v>
       </c>
       <c r="AJ10" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AK10" s="19">
         <v>1</v>
@@ -2456,12 +2448,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B11" s="22" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C11" s="11" t="b">
         <f>TRUE()</f>
@@ -2483,7 +2475,7 @@
         <v>149</v>
       </c>
       <c r="I11" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J11" s="12">
         <v>0</v>
@@ -2522,7 +2514,7 @@
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="V11" s="12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="W11" s="12">
         <v>7.4999999999999997E-2</v>
@@ -2534,10 +2526,10 @@
         <v>112</v>
       </c>
       <c r="Z11" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="AA11" s="2" t="s">
         <v>163</v>
-      </c>
-      <c r="AA11" s="2" t="s">
-        <v>164</v>
       </c>
       <c r="AB11">
         <v>30</v>
@@ -2564,7 +2556,7 @@
         <v>0</v>
       </c>
       <c r="AJ11" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AK11" s="19">
         <v>1</v>
@@ -2588,12 +2580,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C12" s="11" t="b">
         <f>TRUE()</f>
@@ -2615,7 +2607,7 @@
         <v>149</v>
       </c>
       <c r="I12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J12" s="12">
         <v>0</v>
@@ -2654,7 +2646,7 @@
         <v>5.5E-2</v>
       </c>
       <c r="V12" s="12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="W12" s="12">
         <v>7.4999999999999997E-2</v>
@@ -2666,10 +2658,10 @@
         <v>112</v>
       </c>
       <c r="Z12" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="AA12" s="2" t="s">
         <v>163</v>
-      </c>
-      <c r="AA12" s="2" t="s">
-        <v>164</v>
       </c>
       <c r="AB12">
         <v>30</v>
@@ -2696,7 +2688,7 @@
         <v>0</v>
       </c>
       <c r="AJ12" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AK12" s="19">
         <v>1</v>
@@ -2720,12 +2712,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B13" s="22" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C13" s="11" t="b">
         <f>TRUE()</f>
@@ -2747,7 +2739,7 @@
         <v>149</v>
       </c>
       <c r="I13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J13" s="12">
         <v>0</v>
@@ -2786,7 +2778,7 @@
         <v>5.5E-2</v>
       </c>
       <c r="V13" s="12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="W13" s="12">
         <v>5.5E-2</v>
@@ -2798,10 +2790,10 @@
         <v>112</v>
       </c>
       <c r="Z13" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="AA13" s="2" t="s">
         <v>163</v>
-      </c>
-      <c r="AA13" s="2" t="s">
-        <v>164</v>
       </c>
       <c r="AB13">
         <v>30</v>
@@ -2828,7 +2820,7 @@
         <v>0</v>
       </c>
       <c r="AJ13" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AK13" s="19">
         <v>1</v>
@@ -2852,21 +2844,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:43" x14ac:dyDescent="0.25">
       <c r="B14" s="22"/>
-      <c r="L14" s="28"/>
-      <c r="AF14" s="26"/>
+      <c r="L14" s="27"/>
+      <c r="AF14" s="25"/>
       <c r="AH14" s="21"/>
       <c r="AI14" s="21"/>
       <c r="AJ14" s="2"/>
       <c r="AK14" s="19"/>
     </row>
-    <row r="15" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>195</v>
+      </c>
+      <c r="B15" s="22" t="s">
         <v>196</v>
-      </c>
-      <c r="B15" s="22" t="s">
-        <v>197</v>
       </c>
       <c r="C15" s="11" t="b">
         <f>TRUE()</f>
@@ -2888,7 +2880,7 @@
         <v>149</v>
       </c>
       <c r="I15" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J15" s="12">
         <v>0</v>
@@ -2927,7 +2919,7 @@
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="V15" s="12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="W15" s="12">
         <v>7.4999999999999997E-2</v>
@@ -2939,7 +2931,7 @@
         <v>112</v>
       </c>
       <c r="Z15" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="AA15" s="2" t="s">
         <v>114</v>
@@ -2969,7 +2961,7 @@
         <v>0</v>
       </c>
       <c r="AJ15" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AK15" s="19">
         <v>0.75</v>
@@ -2993,12 +2985,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>197</v>
+      </c>
+      <c r="B16" s="22" t="s">
         <v>198</v>
-      </c>
-      <c r="B16" s="22" t="s">
-        <v>199</v>
       </c>
       <c r="C16" s="11" t="b">
         <f>TRUE()</f>
@@ -3020,7 +3012,7 @@
         <v>149</v>
       </c>
       <c r="I16" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J16" s="12">
         <v>0</v>
@@ -3058,8 +3050,8 @@
       <c r="U16" s="12">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="V16" t="s">
-        <v>159</v>
+      <c r="V16" s="12" t="s">
+        <v>158</v>
       </c>
       <c r="W16" s="12">
         <v>7.4999999999999997E-2</v>
@@ -3101,7 +3093,7 @@
         <v>0</v>
       </c>
       <c r="AJ16" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AK16" s="19">
         <v>0.75</v>
@@ -3125,12 +3117,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>199</v>
+      </c>
+      <c r="B17" s="22" t="s">
         <v>200</v>
-      </c>
-      <c r="B17" s="22" t="s">
-        <v>201</v>
       </c>
       <c r="C17" s="11" t="b">
         <f>TRUE()</f>
@@ -3152,7 +3144,7 @@
         <v>149</v>
       </c>
       <c r="I17" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J17" s="12">
         <v>0</v>
@@ -3191,7 +3183,7 @@
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="V17" s="12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="W17" s="12">
         <v>7.4999999999999997E-2</v>
@@ -3233,7 +3225,7 @@
         <v>0</v>
       </c>
       <c r="AJ17" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AK17" s="19">
         <v>0.75</v>
@@ -3257,12 +3249,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>201</v>
+      </c>
+      <c r="B18" s="22" t="s">
         <v>202</v>
-      </c>
-      <c r="B18" s="22" t="s">
-        <v>203</v>
       </c>
       <c r="C18" s="11" t="b">
         <f>TRUE()</f>
@@ -3284,7 +3276,7 @@
         <v>149</v>
       </c>
       <c r="I18" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J18" s="12">
         <v>0</v>
@@ -3323,7 +3315,7 @@
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="V18" s="12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="W18" s="12">
         <v>7.4999999999999997E-2</v>
@@ -3338,7 +3330,7 @@
         <v>113</v>
       </c>
       <c r="AA18" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="AB18">
         <v>30</v>
@@ -3365,7 +3357,7 @@
         <v>0</v>
       </c>
       <c r="AJ18" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AK18" s="19">
         <v>0.75</v>
@@ -3389,12 +3381,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>203</v>
+      </c>
+      <c r="B19" s="22" t="s">
         <v>204</v>
-      </c>
-      <c r="B19" s="22" t="s">
-        <v>205</v>
       </c>
       <c r="C19" s="11" t="b">
         <f>TRUE()</f>
@@ -3416,7 +3408,7 @@
         <v>149</v>
       </c>
       <c r="I19" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J19" s="12">
         <v>0</v>
@@ -3454,8 +3446,8 @@
       <c r="U19" s="12">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="V19" s="25" t="s">
-        <v>156</v>
+      <c r="V19" s="12" t="s">
+        <v>158</v>
       </c>
       <c r="W19" s="12">
         <v>7.4999999999999997E-2</v>
@@ -3467,10 +3459,10 @@
         <v>112</v>
       </c>
       <c r="Z19" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="AA19" s="2" t="s">
         <v>163</v>
-      </c>
-      <c r="AA19" s="2" t="s">
-        <v>164</v>
       </c>
       <c r="AB19">
         <v>30</v>
@@ -3497,7 +3489,7 @@
         <v>0</v>
       </c>
       <c r="AJ19" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AK19" s="19">
         <v>0.75</v>
@@ -3521,12 +3513,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>205</v>
+      </c>
+      <c r="B20" s="22" t="s">
         <v>206</v>
-      </c>
-      <c r="B20" s="22" t="s">
-        <v>207</v>
       </c>
       <c r="C20" s="11" t="b">
         <f>TRUE()</f>
@@ -3548,7 +3540,7 @@
         <v>149</v>
       </c>
       <c r="I20" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J20" s="12">
         <v>0</v>
@@ -3587,7 +3579,7 @@
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="V20" s="12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="W20" s="12">
         <v>7.4999999999999997E-2</v>
@@ -3599,10 +3591,10 @@
         <v>112</v>
       </c>
       <c r="Z20" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="AA20" s="2" t="s">
         <v>163</v>
-      </c>
-      <c r="AA20" s="2" t="s">
-        <v>164</v>
       </c>
       <c r="AB20">
         <v>30</v>
@@ -3629,7 +3621,7 @@
         <v>0</v>
       </c>
       <c r="AJ20" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AK20" s="19">
         <v>0.75</v>
@@ -3653,12 +3645,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>207</v>
+      </c>
+      <c r="B21" s="22" t="s">
         <v>208</v>
-      </c>
-      <c r="B21" s="22" t="s">
-        <v>209</v>
       </c>
       <c r="C21" s="11" t="b">
         <f>TRUE()</f>
@@ -3680,7 +3672,7 @@
         <v>149</v>
       </c>
       <c r="I21" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J21" s="12">
         <v>0</v>
@@ -3719,7 +3711,7 @@
         <v>5.5E-2</v>
       </c>
       <c r="V21" s="12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="W21" s="12">
         <v>7.4999999999999997E-2</v>
@@ -3731,10 +3723,10 @@
         <v>112</v>
       </c>
       <c r="Z21" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="AA21" s="2" t="s">
         <v>163</v>
-      </c>
-      <c r="AA21" s="2" t="s">
-        <v>164</v>
       </c>
       <c r="AB21">
         <v>30</v>
@@ -3761,7 +3753,7 @@
         <v>0</v>
       </c>
       <c r="AJ21" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AK21" s="19">
         <v>0.75</v>
@@ -3785,12 +3777,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>209</v>
+      </c>
+      <c r="B22" s="22" t="s">
         <v>210</v>
-      </c>
-      <c r="B22" s="22" t="s">
-        <v>211</v>
       </c>
       <c r="C22" s="11" t="b">
         <f>TRUE()</f>
@@ -3812,7 +3804,7 @@
         <v>149</v>
       </c>
       <c r="I22" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J22" s="12">
         <v>0</v>
@@ -3851,7 +3843,7 @@
         <v>5.5E-2</v>
       </c>
       <c r="V22" s="12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="W22" s="12">
         <v>5.5E-2</v>
@@ -3863,10 +3855,10 @@
         <v>112</v>
       </c>
       <c r="Z22" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="AA22" s="2" t="s">
         <v>163</v>
-      </c>
-      <c r="AA22" s="2" t="s">
-        <v>164</v>
       </c>
       <c r="AB22">
         <v>30</v>
@@ -3893,7 +3885,7 @@
         <v>0</v>
       </c>
       <c r="AJ22" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AK22" s="19">
         <v>0.75</v>
@@ -3917,12 +3909,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>211</v>
+      </c>
+      <c r="B24" s="22" t="s">
         <v>212</v>
-      </c>
-      <c r="B24" s="22" t="s">
-        <v>213</v>
       </c>
       <c r="C24" s="11" t="b">
         <f>TRUE()</f>
@@ -3944,7 +3936,7 @@
         <v>149</v>
       </c>
       <c r="I24" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J24" s="12">
         <v>0</v>
@@ -3983,7 +3975,7 @@
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="V24" s="12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="W24" s="12">
         <v>7.4999999999999997E-2</v>
@@ -3995,7 +3987,7 @@
         <v>112</v>
       </c>
       <c r="Z24" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="AA24" s="2" t="s">
         <v>114</v>
@@ -4025,7 +4017,7 @@
         <v>0</v>
       </c>
       <c r="AJ24" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AK24" s="19">
         <v>0.5</v>
@@ -4049,12 +4041,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>213</v>
+      </c>
+      <c r="B25" s="22" t="s">
         <v>214</v>
-      </c>
-      <c r="B25" s="22" t="s">
-        <v>215</v>
       </c>
       <c r="C25" s="11" t="b">
         <f>TRUE()</f>
@@ -4076,7 +4068,7 @@
         <v>149</v>
       </c>
       <c r="I25" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J25" s="12">
         <v>0</v>
@@ -4114,8 +4106,8 @@
       <c r="U25" s="12">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="V25" t="s">
-        <v>159</v>
+      <c r="V25" s="12" t="s">
+        <v>158</v>
       </c>
       <c r="W25" s="12">
         <v>7.4999999999999997E-2</v>
@@ -4157,7 +4149,7 @@
         <v>0</v>
       </c>
       <c r="AJ25" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AK25" s="19">
         <v>0.5</v>
@@ -4181,12 +4173,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>215</v>
+      </c>
+      <c r="B26" s="22" t="s">
         <v>216</v>
-      </c>
-      <c r="B26" s="22" t="s">
-        <v>217</v>
       </c>
       <c r="C26" s="11" t="b">
         <f>TRUE()</f>
@@ -4208,7 +4200,7 @@
         <v>149</v>
       </c>
       <c r="I26" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J26" s="12">
         <v>0</v>
@@ -4247,7 +4239,7 @@
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="V26" s="12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="W26" s="12">
         <v>7.4999999999999997E-2</v>
@@ -4289,7 +4281,7 @@
         <v>0</v>
       </c>
       <c r="AJ26" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AK26" s="19">
         <v>0.5</v>
@@ -4313,12 +4305,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>217</v>
+      </c>
+      <c r="B27" s="22" t="s">
         <v>218</v>
-      </c>
-      <c r="B27" s="22" t="s">
-        <v>219</v>
       </c>
       <c r="C27" s="11" t="b">
         <f>TRUE()</f>
@@ -4340,7 +4332,7 @@
         <v>149</v>
       </c>
       <c r="I27" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J27" s="12">
         <v>0</v>
@@ -4379,7 +4371,7 @@
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="V27" s="12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="W27" s="12">
         <v>7.4999999999999997E-2</v>
@@ -4394,7 +4386,7 @@
         <v>113</v>
       </c>
       <c r="AA27" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="AB27">
         <v>30</v>
@@ -4421,7 +4413,7 @@
         <v>0</v>
       </c>
       <c r="AJ27" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AK27" s="19">
         <v>0.5</v>
@@ -4445,12 +4437,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>219</v>
+      </c>
+      <c r="B28" s="22" t="s">
         <v>220</v>
-      </c>
-      <c r="B28" s="22" t="s">
-        <v>221</v>
       </c>
       <c r="C28" s="11" t="b">
         <f>TRUE()</f>
@@ -4472,7 +4464,7 @@
         <v>149</v>
       </c>
       <c r="I28" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J28" s="12">
         <v>0</v>
@@ -4510,8 +4502,8 @@
       <c r="U28" s="12">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="V28" s="25" t="s">
-        <v>156</v>
+      <c r="V28" s="12" t="s">
+        <v>158</v>
       </c>
       <c r="W28" s="12">
         <v>7.4999999999999997E-2</v>
@@ -4523,10 +4515,10 @@
         <v>112</v>
       </c>
       <c r="Z28" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="AA28" s="2" t="s">
         <v>163</v>
-      </c>
-      <c r="AA28" s="2" t="s">
-        <v>164</v>
       </c>
       <c r="AB28">
         <v>30</v>
@@ -4553,7 +4545,7 @@
         <v>0</v>
       </c>
       <c r="AJ28" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AK28" s="19">
         <v>0.5</v>
@@ -4577,12 +4569,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>221</v>
+      </c>
+      <c r="B29" s="22" t="s">
         <v>222</v>
-      </c>
-      <c r="B29" s="22" t="s">
-        <v>223</v>
       </c>
       <c r="C29" s="11" t="b">
         <f>TRUE()</f>
@@ -4604,7 +4596,7 @@
         <v>149</v>
       </c>
       <c r="I29" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J29" s="12">
         <v>0</v>
@@ -4643,7 +4635,7 @@
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="V29" s="12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="W29" s="12">
         <v>7.4999999999999997E-2</v>
@@ -4655,10 +4647,10 @@
         <v>112</v>
       </c>
       <c r="Z29" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="AA29" s="2" t="s">
         <v>163</v>
-      </c>
-      <c r="AA29" s="2" t="s">
-        <v>164</v>
       </c>
       <c r="AB29">
         <v>30</v>
@@ -4685,7 +4677,7 @@
         <v>0</v>
       </c>
       <c r="AJ29" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AK29" s="19">
         <v>0.5</v>
@@ -4709,12 +4701,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>223</v>
+      </c>
+      <c r="B30" s="22" t="s">
         <v>224</v>
-      </c>
-      <c r="B30" s="22" t="s">
-        <v>225</v>
       </c>
       <c r="C30" s="11" t="b">
         <f>TRUE()</f>
@@ -4736,7 +4728,7 @@
         <v>149</v>
       </c>
       <c r="I30" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J30" s="12">
         <v>0</v>
@@ -4775,7 +4767,7 @@
         <v>5.5E-2</v>
       </c>
       <c r="V30" s="12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="W30" s="12">
         <v>7.4999999999999997E-2</v>
@@ -4787,10 +4779,10 @@
         <v>112</v>
       </c>
       <c r="Z30" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="AA30" s="2" t="s">
         <v>163</v>
-      </c>
-      <c r="AA30" s="2" t="s">
-        <v>164</v>
       </c>
       <c r="AB30">
         <v>30</v>
@@ -4817,7 +4809,7 @@
         <v>0</v>
       </c>
       <c r="AJ30" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AK30" s="19">
         <v>0.5</v>
@@ -4841,12 +4833,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>225</v>
+      </c>
+      <c r="B31" s="22" t="s">
         <v>226</v>
-      </c>
-      <c r="B31" s="22" t="s">
-        <v>227</v>
       </c>
       <c r="C31" s="11" t="b">
         <f>TRUE()</f>
@@ -4868,7 +4860,7 @@
         <v>149</v>
       </c>
       <c r="I31" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J31" s="12">
         <v>0</v>
@@ -4907,7 +4899,7 @@
         <v>5.5E-2</v>
       </c>
       <c r="V31" s="12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="W31" s="12">
         <v>5.5E-2</v>
@@ -4919,10 +4911,10 @@
         <v>112</v>
       </c>
       <c r="Z31" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="AA31" s="2" t="s">
         <v>163</v>
-      </c>
-      <c r="AA31" s="2" t="s">
-        <v>164</v>
       </c>
       <c r="AB31">
         <v>30</v>
@@ -4949,7 +4941,7 @@
         <v>0</v>
       </c>
       <c r="AJ31" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AK31" s="19">
         <v>0.5</v>
@@ -4975,17 +4967,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="J4:K4"/>
     <mergeCell ref="AJ4:AL4"/>
     <mergeCell ref="L4:R4"/>
     <mergeCell ref="S4:U4"/>
     <mergeCell ref="Z4:AB4"/>
     <mergeCell ref="AC4:AF4"/>
     <mergeCell ref="V4:X4"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="J4:K4"/>
   </mergeCells>
   <dataValidations count="20">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AP6:AP13 AP15:AP22 AP24:AP31">
@@ -5004,7 +4996,7 @@
       <formula1>ConPolicy</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6:C13 K6:K13 C15:C22 K15:K22 C24:C31 K24:K31">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K24:K31 K6:K13 C15:C22 K15:K22 C24:C31 C6:C13">
       <formula1>"TRUE,FALSE"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -5052,7 +5044,7 @@
       <formula1>1</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="V6:V13 V15:V22 V24:V31"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="V15:V22 V6:V13 V24:V31"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AG6:AI22 AG24:AI31">
       <formula1>"TRUE, FALSE"</formula1>
     </dataValidation>
@@ -5064,11 +5056,6 @@
       <formula2>1.5</formula2>
     </dataValidation>
   </dataValidations>
-  <hyperlinks>
-    <hyperlink ref="V10" location="Returns!A1" display="internal"/>
-    <hyperlink ref="V19" location="Returns!A1" display="internal"/>
-    <hyperlink ref="V28" location="Returns!A1" display="internal"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <extLst>
@@ -5097,12 +5084,12 @@
   <dimension ref="A3:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>71</v>
       </c>
@@ -5116,9 +5103,9 @@
         <v>154</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B4" s="12">
         <v>7.4999999999999997E-2</v>
@@ -5130,9 +5117,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B5" s="12">
         <v>5.5E-2</v>
@@ -5144,9 +5131,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B6" s="12">
         <v>7.4999999999999997E-2</v>
@@ -5155,12 +5142,12 @@
         <v>0</v>
       </c>
       <c r="D6">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B7" s="12">
         <v>7.4999999999999997E-2</v>
@@ -5172,9 +5159,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B8" s="12">
         <v>5.5E-2</v>
@@ -5186,9 +5173,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B9" s="12">
         <v>7.4999999999999997E-2</v>
@@ -5197,12 +5184,12 @@
         <v>0</v>
       </c>
       <c r="D9">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B10" s="12">
         <v>7.4999999999999997E-2</v>
@@ -5214,9 +5201,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B11" s="12">
         <v>5.5E-2</v>
@@ -5228,9 +5215,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B12" s="12">
         <v>7.4999999999999997E-2</v>
@@ -5239,7 +5226,7 @@
         <v>0</v>
       </c>
       <c r="D12">
-        <v>65</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -5265,25 +5252,25 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>71</v>
       </c>
       <c r="B2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C2" t="s">
         <v>154</v>
       </c>
       <c r="D2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B3" s="18">
         <v>11</v>
@@ -5295,9 +5282,9 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B4" s="18">
         <v>11</v>
@@ -5309,9 +5296,9 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B5" s="18">
         <v>11</v>
@@ -5333,20 +5320,20 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1025" width="8.5546875"/>
+    <col min="1" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>120</v>
       </c>
@@ -5369,9 +5356,9 @@
         <v>126</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="B3">
         <v>1000</v>
@@ -5406,30 +5393,30 @@
       <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.44140625"/>
+    <col min="1" max="1" width="23.42578125"/>
     <col min="2" max="2" width="5"/>
-    <col min="3" max="3" width="85.44140625"/>
-    <col min="4" max="1025" width="8.5546875"/>
+    <col min="3" max="3" width="85.42578125"/>
+    <col min="4" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>127</v>
       </c>
       <c r="B1" s="3"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>129</v>
       </c>
@@ -5437,12 +5424,12 @@
         <v>130</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>112</v>
       </c>
@@ -5450,7 +5437,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>118</v>
       </c>
@@ -5458,7 +5445,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>133</v>
       </c>
@@ -5466,12 +5453,12 @@
         <v>134</v>
       </c>
     </row>
-    <row r="11" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>115</v>
       </c>
@@ -5479,7 +5466,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>136</v>
       </c>
@@ -5487,7 +5474,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>138</v>
       </c>
@@ -5495,12 +5482,12 @@
         <v>139</v>
       </c>
     </row>
-    <row r="16" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>109</v>
       </c>
@@ -5508,7 +5495,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>141</v>
       </c>
@@ -5516,12 +5503,12 @@
         <v>142</v>
       </c>
     </row>
-    <row r="20" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>109</v>
       </c>
@@ -5529,7 +5516,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>141</v>
       </c>
@@ -5537,12 +5524,12 @@
         <v>142</v>
       </c>
     </row>
-    <row r="24" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="16" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>109</v>
       </c>
@@ -5550,7 +5537,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>141</v>
       </c>
@@ -5558,12 +5545,12 @@
         <v>142</v>
       </c>
     </row>
-    <row r="28" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="16" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>109</v>
       </c>
@@ -5571,7 +5558,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>141</v>
       </c>
@@ -5579,12 +5566,12 @@
         <v>142</v>
       </c>
     </row>
-    <row r="32" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="16" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>117</v>
       </c>
@@ -5592,7 +5579,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>144</v>
       </c>
@@ -5600,12 +5587,12 @@
         <v>145</v>
       </c>
     </row>
-    <row r="36" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="16" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>110</v>
       </c>
@@ -5613,7 +5600,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>147</v>
       </c>
@@ -5621,7 +5608,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>149</v>
       </c>
@@ -5629,7 +5616,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>151</v>
       </c>
@@ -5637,17 +5624,17 @@
         <v>152</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.3">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="16" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>111</v>
       </c>
@@ -5655,14 +5642,14 @@
         <v>153</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>178</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>179</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add analysis of actuarial methods
</commit_message>
<xml_diff>
--- a/IO_M1/RunControl_M1.xlsx
+++ b/IO_M1/RunControl_M1.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\PenSim-Projects\Model_Main\IO_M1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\Model_Main\IO_M1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TOC" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="222">
   <si>
     <t>Sheet #</t>
   </si>
@@ -514,12 +514,6 @@
     <t>exCon</t>
   </si>
   <si>
-    <t>R5F1</t>
-  </si>
-  <si>
-    <t>R6F1</t>
-  </si>
-  <si>
     <t>open</t>
   </si>
   <si>
@@ -541,18 +535,6 @@
     <t>MA_0_pct</t>
   </si>
   <si>
-    <t>R5F3</t>
-  </si>
-  <si>
-    <t>R6F3</t>
-  </si>
-  <si>
-    <t>R5F2</t>
-  </si>
-  <si>
-    <t>R6F2</t>
-  </si>
-  <si>
     <t>EEC_fixed</t>
   </si>
   <si>
@@ -667,52 +649,52 @@
     <t>75% initial Funding; Full smoothing, DR 5.5%, ir 5.5%, sd 8%</t>
   </si>
   <si>
-    <t>M1-F50-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">50% initial Funding; No Smoothing </t>
-  </si>
-  <si>
-    <t>M1-F50-2</t>
-  </si>
-  <si>
-    <t>50% initial Funding; Closed 10-year cd</t>
-  </si>
-  <si>
-    <t>M1-F50-3</t>
-  </si>
-  <si>
-    <t>50% initial Funding; Closed 30-year cd</t>
-  </si>
-  <si>
-    <t>M1-F50-4</t>
-  </si>
-  <si>
-    <t>50% initial Funding; Closed 30-year cp</t>
-  </si>
-  <si>
-    <t>M1-F50-5</t>
-  </si>
-  <si>
-    <t>50% initial Funding; Open 30-year cp</t>
-  </si>
-  <si>
-    <t>M1-F50-6</t>
-  </si>
-  <si>
-    <t>50% initial Funding; Full smoothing:open 30 year cp; 5-year asset smoothing</t>
-  </si>
-  <si>
-    <t>M1-F50-7</t>
-  </si>
-  <si>
-    <t>50% initial Funding; Full smoothing, DR 5.5%, ir 7.5%, sd 12%</t>
-  </si>
-  <si>
-    <t>M1-F50-8</t>
-  </si>
-  <si>
-    <t>50% initial Funding; Full smoothing, DR 5.5%, ir 5.5%, sd 8%</t>
+    <t>M1-F100-BRP1</t>
+  </si>
+  <si>
+    <t>100% initial Funding; BRP: open 15-year cp; 5-year asset smoothing, DR 6.4%, ir 7.5%, sd 12%</t>
+  </si>
+  <si>
+    <t>100% initial Funding; BRP: open 15-year cp; 5-year asset smoothing, DR 6.4%, ir 6.4%, sd 8%</t>
+  </si>
+  <si>
+    <t>M1-F100-BRP2</t>
+  </si>
+  <si>
+    <t>M1-F100-BRP3</t>
+  </si>
+  <si>
+    <t>M1-F100-BRP4</t>
+  </si>
+  <si>
+    <t>100% initial Funding; BRP: open 15-year cp; 5-year asset smoothing, DR 7.5%, ir 7.5%, sd 12%</t>
+  </si>
+  <si>
+    <t>100% initial Funding; BRP: open 15-year cp; 5-year asset smoothing, DR 7.5%, ir 6.4%, sd 8%</t>
+  </si>
+  <si>
+    <t>M1-F75-BRP1</t>
+  </si>
+  <si>
+    <t>75% initial Funding; BRP: open 15-year cp; 5-year asset smoothing, DR 6.4%, ir 7.5%, sd 12%</t>
+  </si>
+  <si>
+    <t>M1-F75-BRP2</t>
+  </si>
+  <si>
+    <t>75% initial Funding; BRP: open 15-year cp; 5-year asset smoothing, DR 6.4%, ir 6.4%, sd 8%</t>
+  </si>
+  <si>
+    <t>M1-F75-BRP3</t>
+  </si>
+  <si>
+    <t>75% initial Funding; BRP: open 15-year cp; 5-year asset smoothing, DR 7.5%, ir 7.5%, sd 12%</t>
+  </si>
+  <si>
+    <t>M1-F75-BRP4</t>
+  </si>
+  <si>
+    <t>75% initial Funding; BRP: open 15-year cp; 5-year asset smoothing, DR 7.5%, ir 6.4%, sd 8%</t>
   </si>
 </sst>
 </file>
@@ -1279,14 +1261,14 @@
       <selection pane="bottomRight" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.5546875"/>
-    <col min="2" max="2" width="16.6640625"/>
-    <col min="3" max="1025" width="8.5546875"/>
+    <col min="1" max="1" width="7.5703125"/>
+    <col min="2" max="2" width="16.7109375"/>
+    <col min="3" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1294,7 +1276,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1302,7 +1284,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -1310,7 +1292,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -1337,77 +1319,77 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1025" width="8.5546875"/>
+    <col min="1" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>21</v>
       </c>
@@ -1420,38 +1402,38 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AQ31"/>
+  <dimension ref="A1:AQ30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="U1" sqref="U1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="C9" sqref="C9"/>
+      <selection pane="bottomRight" activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="54.44140625"/>
-    <col min="2" max="2" width="98.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="9" width="24.44140625"/>
-    <col min="10" max="11" width="17.44140625"/>
-    <col min="12" max="12" width="16.109375"/>
-    <col min="13" max="14" width="21.44140625"/>
-    <col min="15" max="15" width="24.5546875"/>
+    <col min="1" max="1" width="54.42578125"/>
+    <col min="2" max="2" width="98.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="9" width="24.42578125"/>
+    <col min="10" max="11" width="17.42578125"/>
+    <col min="12" max="12" width="16.140625"/>
+    <col min="13" max="14" width="21.42578125"/>
+    <col min="15" max="15" width="24.5703125"/>
     <col min="16" max="16" width="16"/>
-    <col min="17" max="21" width="12.6640625"/>
-    <col min="22" max="22" width="11.109375" customWidth="1"/>
-    <col min="23" max="32" width="12.6640625"/>
+    <col min="17" max="21" width="12.7109375"/>
+    <col min="22" max="22" width="11.140625" customWidth="1"/>
+    <col min="23" max="32" width="12.7109375"/>
     <col min="35" max="35" width="9" customWidth="1"/>
     <col min="37" max="37" width="12" customWidth="1"/>
-    <col min="38" max="38" width="12.6640625"/>
-    <col min="39" max="40" width="27.109375"/>
-    <col min="41" max="41" width="26.88671875"/>
+    <col min="38" max="38" width="12.7109375"/>
+    <col min="39" max="40" width="27.140625"/>
+    <col min="41" max="41" width="26.85546875"/>
     <col min="43" max="43" width="16"/>
-    <col min="44" max="1030" width="8.5546875"/>
+    <col min="44" max="1030" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:43" x14ac:dyDescent="0.25">
       <c r="AC1" s="1" t="s">
         <v>22</v>
       </c>
@@ -1462,7 +1444,7 @@
       <c r="AH1" s="1"/>
       <c r="AI1" s="1"/>
     </row>
-    <row r="2" spans="1:43" s="4" customFormat="1" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:43" s="4" customFormat="1" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>23</v>
       </c>
@@ -1524,13 +1506,13 @@
         <v>40</v>
       </c>
       <c r="AH2" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="AI2" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="AJ2" s="6" t="s">
         <v>165</v>
-      </c>
-      <c r="AI2" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="AJ2" s="6" t="s">
-        <v>167</v>
       </c>
       <c r="AK2" s="6"/>
       <c r="AL2" s="4" t="s">
@@ -1543,7 +1525,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:43" ht="42" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:43" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>43</v>
       </c>
@@ -1578,7 +1560,7 @@
         <v>53</v>
       </c>
       <c r="AJ3" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="AK3" s="4"/>
       <c r="AN3" s="4" t="s">
@@ -1594,7 +1576,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:43" s="8" customFormat="1" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:43" s="8" customFormat="1" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="32" t="s">
         <v>58</v>
       </c>
@@ -1665,7 +1647,7 @@
       <c r="AP4" s="24"/>
       <c r="AQ4" s="24"/>
     </row>
-    <row r="5" spans="1:43" s="10" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:43" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>71</v>
       </c>
@@ -1766,16 +1748,16 @@
         <v>160</v>
       </c>
       <c r="AH5" s="9" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="AI5" s="9" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="AJ5" s="9" t="s">
         <v>106</v>
       </c>
       <c r="AK5" s="9" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="AL5" s="9" t="s">
         <v>102</v>
@@ -1796,12 +1778,12 @@
         <v>108</v>
       </c>
     </row>
-    <row r="6" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="C6" s="11" t="b">
         <f>TRUE()</f>
@@ -1823,7 +1805,7 @@
         <v>149</v>
       </c>
       <c r="I6" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="J6" s="12">
         <v>0</v>
@@ -1874,7 +1856,7 @@
         <v>112</v>
       </c>
       <c r="Z6" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="AA6" s="2" t="s">
         <v>114</v>
@@ -1904,7 +1886,7 @@
         <v>0</v>
       </c>
       <c r="AJ6" s="2" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="AK6" s="19">
         <v>1</v>
@@ -1928,12 +1910,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="C7" s="11" t="b">
         <v>0</v>
@@ -1954,7 +1936,7 @@
         <v>149</v>
       </c>
       <c r="I7" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="J7" s="12">
         <v>0</v>
@@ -2035,7 +2017,7 @@
         <v>0</v>
       </c>
       <c r="AJ7" s="2" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="AK7" s="19">
         <v>1</v>
@@ -2059,12 +2041,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="C8" s="11" t="b">
         <v>0</v>
@@ -2085,7 +2067,7 @@
         <v>149</v>
       </c>
       <c r="I8" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="J8" s="12">
         <v>0</v>
@@ -2166,7 +2148,7 @@
         <v>0</v>
       </c>
       <c r="AJ8" s="2" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="AK8" s="19">
         <v>1</v>
@@ -2190,12 +2172,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="C9" s="11" t="b">
         <v>0</v>
@@ -2216,7 +2198,7 @@
         <v>149</v>
       </c>
       <c r="I9" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="J9" s="12">
         <v>0</v>
@@ -2270,7 +2252,7 @@
         <v>113</v>
       </c>
       <c r="AA9" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="AB9">
         <v>30</v>
@@ -2297,7 +2279,7 @@
         <v>0</v>
       </c>
       <c r="AJ9" s="2" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="AK9" s="19">
         <v>1</v>
@@ -2321,12 +2303,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="B10" s="22" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="C10" s="11" t="b">
         <v>0</v>
@@ -2347,7 +2329,7 @@
         <v>149</v>
       </c>
       <c r="I10" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="J10" s="12">
         <v>0</v>
@@ -2398,10 +2380,10 @@
         <v>112</v>
       </c>
       <c r="Z10" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="AA10" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="AB10">
         <v>30</v>
@@ -2428,7 +2410,7 @@
         <v>0</v>
       </c>
       <c r="AJ10" s="2" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="AK10" s="19">
         <v>1</v>
@@ -2452,12 +2434,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="B11" s="22" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="C11" s="11" t="b">
         <v>0</v>
@@ -2478,7 +2460,7 @@
         <v>149</v>
       </c>
       <c r="I11" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="J11" s="12">
         <v>0</v>
@@ -2529,10 +2511,10 @@
         <v>112</v>
       </c>
       <c r="Z11" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="AA11" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="AB11">
         <v>30</v>
@@ -2559,7 +2541,7 @@
         <v>0</v>
       </c>
       <c r="AJ11" s="2" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="AK11" s="19">
         <v>1</v>
@@ -2583,12 +2565,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="C12" s="11" t="b">
         <v>0</v>
@@ -2609,7 +2591,7 @@
         <v>149</v>
       </c>
       <c r="I12" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="J12" s="12">
         <v>0</v>
@@ -2660,10 +2642,10 @@
         <v>112</v>
       </c>
       <c r="Z12" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="AA12" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="AB12">
         <v>30</v>
@@ -2690,7 +2672,7 @@
         <v>0</v>
       </c>
       <c r="AJ12" s="2" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="AK12" s="19">
         <v>1</v>
@@ -2714,12 +2696,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="B13" s="22" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="C13" s="11" t="b">
         <v>0</v>
@@ -2740,7 +2722,7 @@
         <v>149</v>
       </c>
       <c r="I13" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="J13" s="12">
         <v>0</v>
@@ -2791,10 +2773,10 @@
         <v>112</v>
       </c>
       <c r="Z13" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="AA13" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="AB13">
         <v>30</v>
@@ -2821,7 +2803,7 @@
         <v>0</v>
       </c>
       <c r="AJ13" s="2" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="AK13" s="19">
         <v>1</v>
@@ -2845,24 +2827,143 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="B14" s="22"/>
-      <c r="C14" t="b">
-        <v>0</v>
-      </c>
-      <c r="L14" s="28"/>
-      <c r="AF14" s="26"/>
-      <c r="AH14" s="21"/>
-      <c r="AI14" s="21"/>
-      <c r="AJ14" s="2"/>
-      <c r="AK14" s="19"/>
-    </row>
-    <row r="15" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>206</v>
+      </c>
+      <c r="B14" s="22" t="s">
+        <v>207</v>
+      </c>
+      <c r="C14" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D14" t="s">
+        <v>109</v>
+      </c>
+      <c r="E14" t="s">
+        <v>109</v>
+      </c>
+      <c r="F14" t="s">
+        <v>109</v>
+      </c>
+      <c r="G14" t="s">
+        <v>109</v>
+      </c>
+      <c r="H14" t="s">
+        <v>149</v>
+      </c>
+      <c r="I14" t="s">
+        <v>172</v>
+      </c>
+      <c r="J14" s="12">
+        <v>0</v>
+      </c>
+      <c r="K14" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="L14" s="12">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="M14">
+        <v>3</v>
+      </c>
+      <c r="N14">
+        <v>65</v>
+      </c>
+      <c r="O14">
+        <v>65</v>
+      </c>
+      <c r="P14" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="Q14">
+        <v>10</v>
+      </c>
+      <c r="R14">
+        <v>10</v>
+      </c>
+      <c r="S14" s="12">
+        <v>0.03</v>
+      </c>
+      <c r="T14" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="U14" s="12">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="V14" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="W14" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="X14" s="12">
+        <v>0.12</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z14" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="AA14" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="AB14">
+        <v>15</v>
+      </c>
+      <c r="AC14" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="AD14" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="AE14" s="14">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AF14" s="14">
+        <v>0.05</v>
+      </c>
+      <c r="AG14" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="AH14" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="AI14" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ14" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="AK14" s="19">
+        <v>1</v>
+      </c>
+      <c r="AL14">
+        <v>200</v>
+      </c>
+      <c r="AM14" t="s">
+        <v>117</v>
+      </c>
+      <c r="AN14">
+        <v>5</v>
+      </c>
+      <c r="AO14">
+        <v>200</v>
+      </c>
+      <c r="AP14" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="AQ14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>196</v>
+        <v>209</v>
       </c>
       <c r="B15" s="22" t="s">
-        <v>197</v>
+        <v>208</v>
       </c>
       <c r="C15" s="11" t="b">
         <v>0</v>
@@ -2883,7 +2984,7 @@
         <v>149</v>
       </c>
       <c r="I15" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="J15" s="12">
         <v>0</v>
@@ -2919,28 +3020,28 @@
         <v>0.01</v>
       </c>
       <c r="U15" s="12">
-        <v>7.4999999999999997E-2</v>
+        <v>6.4000000000000001E-2</v>
       </c>
       <c r="V15" s="12" t="s">
         <v>159</v>
       </c>
       <c r="W15" s="12">
-        <v>7.4999999999999997E-2</v>
+        <v>6.4000000000000001E-2</v>
       </c>
       <c r="X15" s="12">
-        <v>0.12</v>
+        <v>0.08</v>
       </c>
       <c r="Y15" t="s">
         <v>112</v>
       </c>
       <c r="Z15" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="AA15" s="2" t="s">
-        <v>114</v>
+        <v>162</v>
       </c>
       <c r="AB15">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="AC15" s="2" t="s">
         <v>115</v>
@@ -2964,16 +3065,16 @@
         <v>0</v>
       </c>
       <c r="AJ15" s="2" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="AK15" s="19">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="AL15">
         <v>200</v>
       </c>
       <c r="AM15" t="s">
-        <v>144</v>
+        <v>117</v>
       </c>
       <c r="AN15">
         <v>5</v>
@@ -2988,12 +3089,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>198</v>
+        <v>210</v>
       </c>
       <c r="B16" s="22" t="s">
-        <v>199</v>
+        <v>212</v>
       </c>
       <c r="C16" s="11" t="b">
         <v>0</v>
@@ -3014,7 +3115,7 @@
         <v>149</v>
       </c>
       <c r="I16" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="J16" s="12">
         <v>0</v>
@@ -3052,7 +3153,7 @@
       <c r="U16" s="12">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="V16" t="s">
+      <c r="V16" s="12" t="s">
         <v>159</v>
       </c>
       <c r="W16" s="12">
@@ -3065,13 +3166,13 @@
         <v>112</v>
       </c>
       <c r="Z16" s="2" t="s">
-        <v>113</v>
+        <v>161</v>
       </c>
       <c r="AA16" s="2" t="s">
-        <v>114</v>
+        <v>162</v>
       </c>
       <c r="AB16">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="AC16" s="2" t="s">
         <v>115</v>
@@ -3095,16 +3196,16 @@
         <v>0</v>
       </c>
       <c r="AJ16" s="2" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="AK16" s="19">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="AL16">
         <v>200</v>
       </c>
       <c r="AM16" t="s">
-        <v>144</v>
+        <v>117</v>
       </c>
       <c r="AN16">
         <v>5</v>
@@ -3119,12 +3220,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>200</v>
+        <v>211</v>
       </c>
       <c r="B17" s="22" t="s">
-        <v>201</v>
+        <v>213</v>
       </c>
       <c r="C17" s="11" t="b">
         <v>0</v>
@@ -3145,7 +3246,7 @@
         <v>149</v>
       </c>
       <c r="I17" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="J17" s="12">
         <v>0</v>
@@ -3187,22 +3288,22 @@
         <v>159</v>
       </c>
       <c r="W17" s="12">
-        <v>7.4999999999999997E-2</v>
+        <v>6.4000000000000001E-2</v>
       </c>
       <c r="X17" s="12">
-        <v>0.12</v>
+        <v>0.08</v>
       </c>
       <c r="Y17" t="s">
         <v>112</v>
       </c>
       <c r="Z17" s="2" t="s">
-        <v>113</v>
+        <v>161</v>
       </c>
       <c r="AA17" s="2" t="s">
-        <v>114</v>
+        <v>162</v>
       </c>
       <c r="AB17">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="AC17" s="2" t="s">
         <v>115</v>
@@ -3226,16 +3327,16 @@
         <v>0</v>
       </c>
       <c r="AJ17" s="2" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="AK17" s="19">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="AL17">
         <v>200</v>
       </c>
       <c r="AM17" t="s">
-        <v>144</v>
+        <v>117</v>
       </c>
       <c r="AN17">
         <v>5</v>
@@ -3250,143 +3351,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>202</v>
-      </c>
-      <c r="B18" s="22" t="s">
-        <v>203</v>
-      </c>
-      <c r="C18" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="D18" t="s">
-        <v>109</v>
-      </c>
-      <c r="E18" t="s">
-        <v>109</v>
-      </c>
-      <c r="F18" t="s">
-        <v>109</v>
-      </c>
-      <c r="G18" t="s">
-        <v>109</v>
-      </c>
-      <c r="H18" t="s">
-        <v>149</v>
-      </c>
-      <c r="I18" t="s">
-        <v>178</v>
-      </c>
-      <c r="J18" s="12">
-        <v>0</v>
-      </c>
-      <c r="K18" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="L18" s="12">
-        <v>1.7999999999999999E-2</v>
-      </c>
-      <c r="M18">
-        <v>3</v>
-      </c>
-      <c r="N18">
-        <v>65</v>
-      </c>
-      <c r="O18">
-        <v>65</v>
-      </c>
-      <c r="P18" s="12">
-        <v>0.01</v>
-      </c>
-      <c r="Q18">
-        <v>10</v>
-      </c>
-      <c r="R18">
-        <v>10</v>
-      </c>
-      <c r="S18" s="12">
-        <v>0.03</v>
-      </c>
-      <c r="T18" s="12">
-        <v>0.01</v>
-      </c>
-      <c r="U18" s="12">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="V18" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="W18" s="12">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="X18" s="12">
-        <v>0.12</v>
-      </c>
-      <c r="Y18" t="s">
-        <v>112</v>
-      </c>
-      <c r="Z18" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="AA18" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="AB18">
-        <v>30</v>
-      </c>
-      <c r="AC18" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="AD18" s="14">
-        <v>0.25</v>
-      </c>
-      <c r="AE18" s="14">
-        <v>0.14499999999999999</v>
-      </c>
-      <c r="AF18" s="14">
-        <v>0.05</v>
-      </c>
-      <c r="AG18" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="AH18" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="AI18" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="AJ18" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="AK18" s="19">
-        <v>0.75</v>
-      </c>
-      <c r="AL18">
-        <v>200</v>
-      </c>
-      <c r="AM18" t="s">
-        <v>144</v>
-      </c>
-      <c r="AN18">
-        <v>5</v>
-      </c>
-      <c r="AO18">
-        <v>200</v>
-      </c>
-      <c r="AP18" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="AQ18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="B18" s="22"/>
+      <c r="L18" s="28"/>
+      <c r="AF18" s="26"/>
+      <c r="AH18" s="21"/>
+      <c r="AI18" s="21"/>
+      <c r="AJ18" s="2"/>
+      <c r="AK18" s="19"/>
+    </row>
+    <row r="19" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>204</v>
+        <v>190</v>
       </c>
       <c r="B19" s="22" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
       <c r="C19" s="11" t="b">
         <v>0</v>
@@ -3407,7 +3386,7 @@
         <v>149</v>
       </c>
       <c r="I19" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="J19" s="12">
         <v>0</v>
@@ -3445,8 +3424,8 @@
       <c r="U19" s="12">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="V19" s="25" t="s">
-        <v>156</v>
+      <c r="V19" s="12" t="s">
+        <v>159</v>
       </c>
       <c r="W19" s="12">
         <v>7.4999999999999997E-2</v>
@@ -3458,13 +3437,13 @@
         <v>112</v>
       </c>
       <c r="Z19" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="AA19" s="2" t="s">
-        <v>164</v>
+        <v>114</v>
       </c>
       <c r="AB19">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="AC19" s="2" t="s">
         <v>115</v>
@@ -3488,7 +3467,7 @@
         <v>0</v>
       </c>
       <c r="AJ19" s="2" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="AK19" s="19">
         <v>0.75</v>
@@ -3512,12 +3491,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>206</v>
+        <v>192</v>
       </c>
       <c r="B20" s="22" t="s">
-        <v>207</v>
+        <v>193</v>
       </c>
       <c r="C20" s="11" t="b">
         <v>0</v>
@@ -3538,7 +3517,7 @@
         <v>149</v>
       </c>
       <c r="I20" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="J20" s="12">
         <v>0</v>
@@ -3576,7 +3555,7 @@
       <c r="U20" s="12">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="V20" s="12" t="s">
+      <c r="V20" t="s">
         <v>159</v>
       </c>
       <c r="W20" s="12">
@@ -3589,13 +3568,13 @@
         <v>112</v>
       </c>
       <c r="Z20" s="2" t="s">
-        <v>163</v>
+        <v>113</v>
       </c>
       <c r="AA20" s="2" t="s">
-        <v>164</v>
+        <v>114</v>
       </c>
       <c r="AB20">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="AC20" s="2" t="s">
         <v>115</v>
@@ -3619,7 +3598,7 @@
         <v>0</v>
       </c>
       <c r="AJ20" s="2" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="AK20" s="19">
         <v>0.75</v>
@@ -3628,7 +3607,7 @@
         <v>200</v>
       </c>
       <c r="AM20" t="s">
-        <v>117</v>
+        <v>144</v>
       </c>
       <c r="AN20">
         <v>5</v>
@@ -3643,12 +3622,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>208</v>
+        <v>194</v>
       </c>
       <c r="B21" s="22" t="s">
-        <v>209</v>
+        <v>195</v>
       </c>
       <c r="C21" s="11" t="b">
         <v>0</v>
@@ -3669,7 +3648,7 @@
         <v>149</v>
       </c>
       <c r="I21" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="J21" s="12">
         <v>0</v>
@@ -3705,7 +3684,7 @@
         <v>0.01</v>
       </c>
       <c r="U21" s="12">
-        <v>5.5E-2</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="V21" s="12" t="s">
         <v>159</v>
@@ -3720,10 +3699,10 @@
         <v>112</v>
       </c>
       <c r="Z21" s="2" t="s">
-        <v>163</v>
+        <v>113</v>
       </c>
       <c r="AA21" s="2" t="s">
-        <v>164</v>
+        <v>114</v>
       </c>
       <c r="AB21">
         <v>30</v>
@@ -3750,7 +3729,7 @@
         <v>0</v>
       </c>
       <c r="AJ21" s="2" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="AK21" s="19">
         <v>0.75</v>
@@ -3759,7 +3738,7 @@
         <v>200</v>
       </c>
       <c r="AM21" t="s">
-        <v>117</v>
+        <v>144</v>
       </c>
       <c r="AN21">
         <v>5</v>
@@ -3774,12 +3753,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>210</v>
+        <v>196</v>
       </c>
       <c r="B22" s="22" t="s">
-        <v>211</v>
+        <v>197</v>
       </c>
       <c r="C22" s="11" t="b">
         <v>0</v>
@@ -3800,7 +3779,7 @@
         <v>149</v>
       </c>
       <c r="I22" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="J22" s="12">
         <v>0</v>
@@ -3836,25 +3815,25 @@
         <v>0.01</v>
       </c>
       <c r="U22" s="12">
-        <v>5.5E-2</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="V22" s="12" t="s">
         <v>159</v>
       </c>
       <c r="W22" s="12">
-        <v>5.5E-2</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="X22" s="12">
-        <v>0.08</v>
+        <v>0.12</v>
       </c>
       <c r="Y22" t="s">
         <v>112</v>
       </c>
       <c r="Z22" s="2" t="s">
-        <v>163</v>
+        <v>113</v>
       </c>
       <c r="AA22" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="AB22">
         <v>30</v>
@@ -3881,7 +3860,7 @@
         <v>0</v>
       </c>
       <c r="AJ22" s="2" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="AK22" s="19">
         <v>0.75</v>
@@ -3890,7 +3869,7 @@
         <v>200</v>
       </c>
       <c r="AM22" t="s">
-        <v>117</v>
+        <v>144</v>
       </c>
       <c r="AN22">
         <v>5</v>
@@ -3905,17 +3884,143 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="C23" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>198</v>
+      </c>
+      <c r="B23" s="22" t="s">
+        <v>199</v>
+      </c>
+      <c r="C23" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D23" t="s">
+        <v>109</v>
+      </c>
+      <c r="E23" t="s">
+        <v>109</v>
+      </c>
+      <c r="F23" t="s">
+        <v>109</v>
+      </c>
+      <c r="G23" t="s">
+        <v>109</v>
+      </c>
+      <c r="H23" t="s">
+        <v>149</v>
+      </c>
+      <c r="I23" t="s">
+        <v>172</v>
+      </c>
+      <c r="J23" s="12">
+        <v>0</v>
+      </c>
+      <c r="K23" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="L23" s="12">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="M23">
+        <v>3</v>
+      </c>
+      <c r="N23">
+        <v>65</v>
+      </c>
+      <c r="O23">
+        <v>65</v>
+      </c>
+      <c r="P23" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="Q23">
+        <v>10</v>
+      </c>
+      <c r="R23">
+        <v>10</v>
+      </c>
+      <c r="S23" s="12">
+        <v>0.03</v>
+      </c>
+      <c r="T23" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="U23" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="V23" s="25" t="s">
+        <v>156</v>
+      </c>
+      <c r="W23" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="X23" s="12">
+        <v>0.12</v>
+      </c>
+      <c r="Y23" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z23" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="AA23" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="AB23">
+        <v>30</v>
+      </c>
+      <c r="AC23" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="AD23" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="AE23" s="14">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AF23" s="14">
+        <v>0.05</v>
+      </c>
+      <c r="AG23" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="AH23" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="AI23" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ23" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="AK23" s="19">
+        <v>0.75</v>
+      </c>
+      <c r="AL23">
+        <v>200</v>
+      </c>
+      <c r="AM23" t="s">
+        <v>144</v>
+      </c>
+      <c r="AN23">
+        <v>5</v>
+      </c>
+      <c r="AO23">
+        <v>200</v>
+      </c>
+      <c r="AP23" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="AQ23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="B24" s="22" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="C24" s="11" t="b">
         <v>0</v>
@@ -3936,7 +4041,7 @@
         <v>149</v>
       </c>
       <c r="I24" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="J24" s="12">
         <v>0</v>
@@ -3987,13 +4092,13 @@
         <v>112</v>
       </c>
       <c r="Z24" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="AA24" s="2" t="s">
-        <v>114</v>
+        <v>162</v>
       </c>
       <c r="AB24">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="AC24" s="2" t="s">
         <v>115</v>
@@ -4017,16 +4122,16 @@
         <v>0</v>
       </c>
       <c r="AJ24" s="2" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="AK24" s="19">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="AL24">
         <v>200</v>
       </c>
       <c r="AM24" t="s">
-        <v>144</v>
+        <v>117</v>
       </c>
       <c r="AN24">
         <v>5</v>
@@ -4041,12 +4146,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>214</v>
+        <v>202</v>
       </c>
       <c r="B25" s="22" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="C25" s="11" t="b">
         <v>0</v>
@@ -4067,7 +4172,7 @@
         <v>149</v>
       </c>
       <c r="I25" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="J25" s="12">
         <v>0</v>
@@ -4103,9 +4208,9 @@
         <v>0.01</v>
       </c>
       <c r="U25" s="12">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="V25" t="s">
+        <v>5.5E-2</v>
+      </c>
+      <c r="V25" s="12" t="s">
         <v>159</v>
       </c>
       <c r="W25" s="12">
@@ -4118,13 +4223,13 @@
         <v>112</v>
       </c>
       <c r="Z25" s="2" t="s">
-        <v>113</v>
+        <v>161</v>
       </c>
       <c r="AA25" s="2" t="s">
-        <v>114</v>
+        <v>162</v>
       </c>
       <c r="AB25">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="AC25" s="2" t="s">
         <v>115</v>
@@ -4148,16 +4253,16 @@
         <v>0</v>
       </c>
       <c r="AJ25" s="2" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="AK25" s="19">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="AL25">
         <v>200</v>
       </c>
       <c r="AM25" t="s">
-        <v>144</v>
+        <v>117</v>
       </c>
       <c r="AN25">
         <v>5</v>
@@ -4172,12 +4277,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="B26" s="22" t="s">
-        <v>217</v>
+        <v>205</v>
       </c>
       <c r="C26" s="11" t="b">
         <v>0</v>
@@ -4198,7 +4303,7 @@
         <v>149</v>
       </c>
       <c r="I26" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="J26" s="12">
         <v>0</v>
@@ -4234,25 +4339,25 @@
         <v>0.01</v>
       </c>
       <c r="U26" s="12">
-        <v>7.4999999999999997E-2</v>
+        <v>5.5E-2</v>
       </c>
       <c r="V26" s="12" t="s">
         <v>159</v>
       </c>
       <c r="W26" s="12">
-        <v>7.4999999999999997E-2</v>
+        <v>5.5E-2</v>
       </c>
       <c r="X26" s="12">
-        <v>0.12</v>
+        <v>0.08</v>
       </c>
       <c r="Y26" t="s">
         <v>112</v>
       </c>
       <c r="Z26" s="2" t="s">
-        <v>113</v>
+        <v>161</v>
       </c>
       <c r="AA26" s="2" t="s">
-        <v>114</v>
+        <v>162</v>
       </c>
       <c r="AB26">
         <v>30</v>
@@ -4279,16 +4384,16 @@
         <v>0</v>
       </c>
       <c r="AJ26" s="2" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="AK26" s="19">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="AL26">
         <v>200</v>
       </c>
       <c r="AM26" t="s">
-        <v>144</v>
+        <v>117</v>
       </c>
       <c r="AN26">
         <v>5</v>
@@ -4303,12 +4408,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="B27" s="22" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="C27" s="11" t="b">
         <v>0</v>
@@ -4329,7 +4434,7 @@
         <v>149</v>
       </c>
       <c r="I27" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="J27" s="12">
         <v>0</v>
@@ -4365,7 +4470,7 @@
         <v>0.01</v>
       </c>
       <c r="U27" s="12">
-        <v>7.4999999999999997E-2</v>
+        <v>6.4000000000000001E-2</v>
       </c>
       <c r="V27" s="12" t="s">
         <v>159</v>
@@ -4380,13 +4485,13 @@
         <v>112</v>
       </c>
       <c r="Z27" s="2" t="s">
-        <v>113</v>
+        <v>161</v>
       </c>
       <c r="AA27" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="AB27">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="AC27" s="2" t="s">
         <v>115</v>
@@ -4410,16 +4515,16 @@
         <v>0</v>
       </c>
       <c r="AJ27" s="2" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="AK27" s="19">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="AL27">
         <v>200</v>
       </c>
       <c r="AM27" t="s">
-        <v>144</v>
+        <v>117</v>
       </c>
       <c r="AN27">
         <v>5</v>
@@ -4434,12 +4539,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="B28" s="22" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="C28" s="11" t="b">
         <v>0</v>
@@ -4460,7 +4565,7 @@
         <v>149</v>
       </c>
       <c r="I28" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="J28" s="12">
         <v>0</v>
@@ -4496,28 +4601,28 @@
         <v>0.01</v>
       </c>
       <c r="U28" s="12">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="V28" s="25" t="s">
-        <v>156</v>
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="V28" s="12" t="s">
+        <v>159</v>
       </c>
       <c r="W28" s="12">
-        <v>7.4999999999999997E-2</v>
+        <v>6.4000000000000001E-2</v>
       </c>
       <c r="X28" s="12">
-        <v>0.12</v>
+        <v>0.08</v>
       </c>
       <c r="Y28" t="s">
         <v>112</v>
       </c>
       <c r="Z28" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="AA28" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="AB28">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="AC28" s="2" t="s">
         <v>115</v>
@@ -4541,16 +4646,16 @@
         <v>0</v>
       </c>
       <c r="AJ28" s="2" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="AK28" s="19">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="AL28">
         <v>200</v>
       </c>
       <c r="AM28" t="s">
-        <v>144</v>
+        <v>117</v>
       </c>
       <c r="AN28">
         <v>5</v>
@@ -4565,12 +4670,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="B29" s="22" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="C29" s="11" t="b">
         <v>0</v>
@@ -4591,7 +4696,7 @@
         <v>149</v>
       </c>
       <c r="I29" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="J29" s="12">
         <v>0</v>
@@ -4642,13 +4747,13 @@
         <v>112</v>
       </c>
       <c r="Z29" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="AA29" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="AB29">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="AC29" s="2" t="s">
         <v>115</v>
@@ -4672,10 +4777,10 @@
         <v>0</v>
       </c>
       <c r="AJ29" s="2" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="AK29" s="19">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="AL29">
         <v>200</v>
@@ -4696,12 +4801,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="B30" s="22" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="C30" s="11" t="b">
         <v>0</v>
@@ -4722,7 +4827,7 @@
         <v>149</v>
       </c>
       <c r="I30" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="J30" s="12">
         <v>0</v>
@@ -4758,28 +4863,28 @@
         <v>0.01</v>
       </c>
       <c r="U30" s="12">
-        <v>5.5E-2</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="V30" s="12" t="s">
         <v>159</v>
       </c>
       <c r="W30" s="12">
-        <v>7.4999999999999997E-2</v>
+        <v>6.4000000000000001E-2</v>
       </c>
       <c r="X30" s="12">
-        <v>0.12</v>
+        <v>0.08</v>
       </c>
       <c r="Y30" t="s">
         <v>112</v>
       </c>
       <c r="Z30" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="AA30" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="AB30">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="AC30" s="2" t="s">
         <v>115</v>
@@ -4803,10 +4908,10 @@
         <v>0</v>
       </c>
       <c r="AJ30" s="2" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="AK30" s="19">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="AL30">
         <v>200</v>
@@ -4824,137 +4929,6 @@
         <v>116</v>
       </c>
       <c r="AQ30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>226</v>
-      </c>
-      <c r="B31" s="22" t="s">
-        <v>227</v>
-      </c>
-      <c r="C31" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="D31" t="s">
-        <v>109</v>
-      </c>
-      <c r="E31" t="s">
-        <v>109</v>
-      </c>
-      <c r="F31" t="s">
-        <v>109</v>
-      </c>
-      <c r="G31" t="s">
-        <v>109</v>
-      </c>
-      <c r="H31" t="s">
-        <v>149</v>
-      </c>
-      <c r="I31" t="s">
-        <v>178</v>
-      </c>
-      <c r="J31" s="12">
-        <v>0</v>
-      </c>
-      <c r="K31" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="L31" s="12">
-        <v>1.7999999999999999E-2</v>
-      </c>
-      <c r="M31">
-        <v>3</v>
-      </c>
-      <c r="N31">
-        <v>65</v>
-      </c>
-      <c r="O31">
-        <v>65</v>
-      </c>
-      <c r="P31" s="12">
-        <v>0.01</v>
-      </c>
-      <c r="Q31">
-        <v>10</v>
-      </c>
-      <c r="R31">
-        <v>10</v>
-      </c>
-      <c r="S31" s="12">
-        <v>0.03</v>
-      </c>
-      <c r="T31" s="12">
-        <v>0.01</v>
-      </c>
-      <c r="U31" s="12">
-        <v>5.5E-2</v>
-      </c>
-      <c r="V31" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="W31" s="12">
-        <v>5.5E-2</v>
-      </c>
-      <c r="X31" s="12">
-        <v>0.08</v>
-      </c>
-      <c r="Y31" t="s">
-        <v>112</v>
-      </c>
-      <c r="Z31" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="AA31" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="AB31">
-        <v>30</v>
-      </c>
-      <c r="AC31" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="AD31" s="14">
-        <v>0.25</v>
-      </c>
-      <c r="AE31" s="14">
-        <v>0.14499999999999999</v>
-      </c>
-      <c r="AF31" s="14">
-        <v>0.05</v>
-      </c>
-      <c r="AG31" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="AH31" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="AI31" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="AJ31" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="AK31" s="19">
-        <v>0.5</v>
-      </c>
-      <c r="AL31">
-        <v>200</v>
-      </c>
-      <c r="AM31" t="s">
-        <v>117</v>
-      </c>
-      <c r="AN31">
-        <v>5</v>
-      </c>
-      <c r="AO31">
-        <v>200</v>
-      </c>
-      <c r="AP31" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="AQ31">
         <v>1</v>
       </c>
     </row>
@@ -4973,89 +4947,88 @@
     <mergeCell ref="V4:X4"/>
   </mergeCells>
   <dataValidations count="20">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AP6:AP13 AP15:AP22 AP24:AP31">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AP19:AP30 AP6:AP17">
       <formula1>"MA,EAA"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA6:AA13 AA15:AA22 AA24:AA31">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA19:AA30 AA6:AA17">
       <formula1>"cd,cp,sl"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z6:Z13 Z15:Z22 Z24:Z31">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z19:Z30 Z6:Z17">
       <formula1>"open,closed"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AC6:AC13 AC15:AC22 AC24:AC31">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AC19:AC30 AC6:AC17">
       <formula1>ConPolicy</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6:C13 K6:K13 C15:C22 K15:K22 C24:C31 K24:K31">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K19:K30 C19:C30 K6:K17 C6:C17">
       <formula1>"TRUE,FALSE"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer 55 to 65, please" sqref="N6:N13 N15:N22 N24:N31">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer 55 to 65, please" sqref="N19:N30 N6:N17">
       <formula1>55</formula1>
       <formula2>65</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-10% please" sqref="P6:P13 T6:T13 P15:P22 T15:T22 P24:P31 T24:T31">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-10% please" sqref="T19:T30 P19:P30 T6:T17 P6:P17">
       <formula1>0</formula1>
       <formula2>0.1</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 0-15" sqref="Q6:R13 Q15:R22 Q24:R31">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 0-15" sqref="Q19:R30 Q6:R17">
       <formula1>0</formula1>
       <formula2>15</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="W6:W13 S6:S13 U6:U13 W15:W22 S15:S22 U15:U22 W24:W31 S24:S31 U24:U31">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="U19:U30 W19:W30 S19:S30 W6:W17 U6:U17 S6:S17">
       <formula1>0</formula1>
       <formula2>0.2</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 0 to 30, please" sqref="AB6:AB13 AB15:AB22 AB24:AB31">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 0 to 30, please" sqref="AB19:AB30 AB6:AB17">
       <formula1>0</formula1>
       <formula2>30</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-75%" sqref="AD6:AE13 AD15:AE22 AD24:AE31">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-75%" sqref="AD19:AE30 AD6:AE17">
       <formula1>0</formula1>
       <formula2>0.75</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-30%" sqref="AF6:AF13 AF15:AF22 AF24:AF31">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-30%" sqref="AF19:AF30 AF6:AF17">
       <formula1>0</formula1>
       <formula2>0.3</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-75% please" sqref="X6:X13 X15:X22 X24:X31">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-75% please" sqref="X19:X30 X6:X17">
       <formula1>0</formula1>
       <formula2>0.75</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 1 to 30" sqref="AN6:AN13 AN15:AN22 AN24:AN31">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 1 to 30" sqref="AN19:AN30 AN6:AN17">
       <formula1>1</formula1>
       <formula2>30</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AO6:AO13 AO15:AO22 AO24:AO31">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AO19:AO30 AO6:AO17">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AQ6:AQ13 AQ15:AQ22 AQ24:AQ31">
+    <dataValidation type="decimal" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AQ19:AQ30 AQ6:AQ17">
       <formula1>1</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="V6:V13 V15:V22 V24:V31"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AG6:AI22 AG24:AI31">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="V19:V30 V6:V17"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AG6:AI30">
       <formula1>"TRUE, FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AJ6:AJ22 AJ24:AJ31">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AJ6:AJ30">
       <formula1>"MA,AL,AL_pct"</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AK6:AK22 AK24:AK31">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AK6:AK30">
       <formula1>0</formula1>
       <formula2>1.5</formula2>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="V10" location="Returns!A1" display="internal"/>
-    <hyperlink ref="V19" location="Returns!A1" display="internal"/>
-    <hyperlink ref="V28" location="Returns!A1" display="internal"/>
+    <hyperlink ref="V23" location="Returns!A1" display="internal"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
@@ -5063,13 +5036,13 @@
           <x14:formula1>
             <xm:f>DropDowns!$A$37:$A$41</xm:f>
           </x14:formula1>
-          <xm:sqref>H6:H22 H24:H31</xm:sqref>
+          <xm:sqref>H6:H30</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DropDowns!$A$44:$A$46</xm:f>
           </x14:formula1>
-          <xm:sqref>I6:I22 I24:I31</xm:sqref>
+          <xm:sqref>I6:I30</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -5082,12 +5055,12 @@
   <dimension ref="A3:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="A4" sqref="A4:D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>71</v>
       </c>
@@ -5101,131 +5074,41 @@
         <v>154</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>161</v>
-      </c>
-      <c r="B4" s="12">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="C4" s="12">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>161</v>
-      </c>
-      <c r="B5" s="12">
-        <v>5.5E-2</v>
-      </c>
-      <c r="C5" s="12">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>161</v>
-      </c>
-      <c r="B6" s="12">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="C6" s="12">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>172</v>
-      </c>
-      <c r="B7" s="12">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="C7" s="12">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>172</v>
-      </c>
-      <c r="B8" s="12">
-        <v>5.5E-2</v>
-      </c>
-      <c r="C8" s="12">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>172</v>
-      </c>
-      <c r="B9" s="12">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="C9" s="12">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>170</v>
-      </c>
-      <c r="B10" s="12">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="C10" s="12">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>170</v>
-      </c>
-      <c r="B11" s="12">
-        <v>5.5E-2</v>
-      </c>
-      <c r="C11" s="12">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>170</v>
-      </c>
-      <c r="B12" s="12">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="C12" s="12">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>65</v>
-      </c>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
     </row>
   </sheetData>
   <dataValidations count="2">
@@ -5247,12 +5130,12 @@
   <dimension ref="A2:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="A3" sqref="A3:D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>71</v>
       </c>
@@ -5266,47 +5149,20 @@
         <v>158</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>162</v>
-      </c>
-      <c r="B3" s="18">
-        <v>11</v>
-      </c>
-      <c r="C3" s="18">
-        <v>5</v>
-      </c>
-      <c r="D3" s="19">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>173</v>
-      </c>
-      <c r="B4" s="18">
-        <v>11</v>
-      </c>
-      <c r="C4" s="18">
-        <v>5</v>
-      </c>
-      <c r="D4" s="19">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>171</v>
-      </c>
-      <c r="B5" s="18">
-        <v>11</v>
-      </c>
-      <c r="C5" s="18">
-        <v>5</v>
-      </c>
-      <c r="D5" s="19">
-        <v>0.2</v>
-      </c>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="19"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="19"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="18"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5321,17 +5177,17 @@
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1025" width="8.5546875"/>
+    <col min="1" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>120</v>
       </c>
@@ -5354,7 +5210,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>80</v>
       </c>
@@ -5391,30 +5247,30 @@
       <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.44140625"/>
+    <col min="1" max="1" width="23.42578125"/>
     <col min="2" max="2" width="5"/>
-    <col min="3" max="3" width="85.44140625"/>
-    <col min="4" max="1025" width="8.5546875"/>
+    <col min="3" max="3" width="85.42578125"/>
+    <col min="4" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>127</v>
       </c>
       <c r="B1" s="3"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>129</v>
       </c>
@@ -5422,12 +5278,12 @@
         <v>130</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>112</v>
       </c>
@@ -5435,7 +5291,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>118</v>
       </c>
@@ -5443,7 +5299,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>133</v>
       </c>
@@ -5451,12 +5307,12 @@
         <v>134</v>
       </c>
     </row>
-    <row r="11" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>115</v>
       </c>
@@ -5464,7 +5320,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>136</v>
       </c>
@@ -5472,7 +5328,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>138</v>
       </c>
@@ -5480,12 +5336,12 @@
         <v>139</v>
       </c>
     </row>
-    <row r="16" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>109</v>
       </c>
@@ -5493,7 +5349,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>141</v>
       </c>
@@ -5501,12 +5357,12 @@
         <v>142</v>
       </c>
     </row>
-    <row r="20" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>109</v>
       </c>
@@ -5514,7 +5370,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>141</v>
       </c>
@@ -5522,12 +5378,12 @@
         <v>142</v>
       </c>
     </row>
-    <row r="24" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="16" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>109</v>
       </c>
@@ -5535,7 +5391,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>141</v>
       </c>
@@ -5543,12 +5399,12 @@
         <v>142</v>
       </c>
     </row>
-    <row r="28" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="16" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>109</v>
       </c>
@@ -5556,7 +5412,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>141</v>
       </c>
@@ -5564,12 +5420,12 @@
         <v>142</v>
       </c>
     </row>
-    <row r="32" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="16" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>117</v>
       </c>
@@ -5577,7 +5433,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>144</v>
       </c>
@@ -5585,12 +5441,12 @@
         <v>145</v>
       </c>
     </row>
-    <row r="36" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="16" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>110</v>
       </c>
@@ -5598,7 +5454,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>147</v>
       </c>
@@ -5606,7 +5462,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>149</v>
       </c>
@@ -5614,7 +5470,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>151</v>
       </c>
@@ -5622,17 +5478,17 @@
         <v>152</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.3">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="16" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>111</v>
       </c>
@@ -5640,14 +5496,14 @@
         <v>153</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changes in M1 control file
</commit_message>
<xml_diff>
--- a/IO_M1/RunControl_M1.xlsx
+++ b/IO_M1/RunControl_M1.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="800" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="704" uniqueCount="214">
   <si>
     <t>Sheet #</t>
   </si>
@@ -613,9 +613,6 @@
     <t>B1F100-1</t>
   </si>
   <si>
-    <t>B1F100-2</t>
-  </si>
-  <si>
     <t>B2F100-0</t>
   </si>
   <si>
@@ -625,15 +622,6 @@
     <t>B2F100-2</t>
   </si>
   <si>
-    <t>B3F100-0</t>
-  </si>
-  <si>
-    <t>B3F100-1</t>
-  </si>
-  <si>
-    <t>B3F100-2</t>
-  </si>
-  <si>
     <t>A1F075-0</t>
   </si>
   <si>
@@ -661,9 +649,6 @@
     <t>B1F075-1</t>
   </si>
   <si>
-    <t>B1F075-2</t>
-  </si>
-  <si>
     <t>B2F075-0</t>
   </si>
   <si>
@@ -673,15 +658,6 @@
     <t>B2F075-2</t>
   </si>
   <si>
-    <t>B3F075-0</t>
-  </si>
-  <si>
-    <t>B3F075-1</t>
-  </si>
-  <si>
-    <t>B3F075-2</t>
-  </si>
-  <si>
     <t>A1F075-1c</t>
   </si>
   <si>
@@ -689,6 +665,12 @@
   </si>
   <si>
     <t>A1F075-3c</t>
+  </si>
+  <si>
+    <t>A1F100-7</t>
+  </si>
+  <si>
+    <t>A1F075-7</t>
   </si>
 </sst>
 </file>
@@ -1395,13 +1377,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AQ51"/>
+  <dimension ref="A1:AQ42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="5" topLeftCell="B30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="U1" sqref="U1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="F52" sqref="F52"/>
+      <selection pane="bottomRight" activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1780,7 +1762,7 @@
         <v>173</v>
       </c>
       <c r="C6" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6" t="s">
         <v>109</v>
@@ -1911,7 +1893,7 @@
         <v>174</v>
       </c>
       <c r="C7" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D7" t="s">
         <v>109</v>
@@ -2042,7 +2024,7 @@
         <v>175</v>
       </c>
       <c r="C8" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8" t="s">
         <v>109</v>
@@ -2173,7 +2155,7 @@
         <v>176</v>
       </c>
       <c r="C9" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9" t="s">
         <v>109</v>
@@ -2304,7 +2286,7 @@
         <v>174</v>
       </c>
       <c r="C10" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D10" t="s">
         <v>109</v>
@@ -2435,7 +2417,7 @@
         <v>175</v>
       </c>
       <c r="C11" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D11" t="s">
         <v>109</v>
@@ -2566,7 +2548,7 @@
         <v>176</v>
       </c>
       <c r="C12" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D12" t="s">
         <v>109</v>
@@ -2697,7 +2679,7 @@
         <v>178</v>
       </c>
       <c r="C13" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D13" t="s">
         <v>109</v>
@@ -2918,7 +2900,7 @@
         <v>117</v>
       </c>
       <c r="AG14">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="AH14">
         <v>200</v>
@@ -2959,7 +2941,7 @@
         <v>177</v>
       </c>
       <c r="C15" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D15" t="s">
         <v>109</v>
@@ -3083,154 +3065,154 @@
       </c>
     </row>
     <row r="16" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="B16" s="22"/>
-      <c r="L16" s="27"/>
-      <c r="AC16" s="2"/>
-      <c r="AD16" s="19"/>
-      <c r="AN16" s="25"/>
-      <c r="AP16" s="21"/>
-      <c r="AQ16" s="21"/>
+      <c r="A16" t="s">
+        <v>212</v>
+      </c>
+      <c r="B16" s="22" t="s">
+        <v>177</v>
+      </c>
+      <c r="C16" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>109</v>
+      </c>
+      <c r="E16" t="s">
+        <v>109</v>
+      </c>
+      <c r="F16" t="s">
+        <v>109</v>
+      </c>
+      <c r="G16" t="s">
+        <v>109</v>
+      </c>
+      <c r="H16" t="s">
+        <v>149</v>
+      </c>
+      <c r="I16" t="s">
+        <v>171</v>
+      </c>
+      <c r="J16" s="12">
+        <v>0</v>
+      </c>
+      <c r="K16" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="L16" s="12">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="M16">
+        <v>3</v>
+      </c>
+      <c r="N16">
+        <v>65</v>
+      </c>
+      <c r="O16">
+        <v>65</v>
+      </c>
+      <c r="P16" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="Q16">
+        <v>10</v>
+      </c>
+      <c r="R16">
+        <v>10</v>
+      </c>
+      <c r="S16" s="12">
+        <v>0.03</v>
+      </c>
+      <c r="T16" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="U16" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="V16" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="W16" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="X16" s="12">
+        <v>0.12</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z16" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="AA16" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="AB16">
+        <v>30</v>
+      </c>
+      <c r="AC16" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="AD16" s="19">
+        <v>1</v>
+      </c>
+      <c r="AE16">
+        <v>200</v>
+      </c>
+      <c r="AF16" t="s">
+        <v>117</v>
+      </c>
+      <c r="AG16">
+        <v>10</v>
+      </c>
+      <c r="AH16">
+        <v>200</v>
+      </c>
+      <c r="AI16" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="AJ16">
+        <v>1</v>
+      </c>
+      <c r="AK16" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="AL16" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="AM16" s="14">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AN16" s="14">
+        <v>0.05</v>
+      </c>
+      <c r="AO16" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP16" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="AQ16" s="21" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>201</v>
-      </c>
-      <c r="B17" s="22" t="s">
-        <v>173</v>
-      </c>
-      <c r="C17" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="D17" t="s">
-        <v>109</v>
-      </c>
-      <c r="E17" t="s">
-        <v>109</v>
-      </c>
-      <c r="F17" t="s">
-        <v>109</v>
-      </c>
-      <c r="G17" t="s">
-        <v>109</v>
-      </c>
-      <c r="H17" t="s">
-        <v>149</v>
-      </c>
-      <c r="I17" t="s">
-        <v>171</v>
-      </c>
-      <c r="J17" s="12">
-        <v>0</v>
-      </c>
-      <c r="K17" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="L17" s="12">
-        <v>1.7999999999999999E-2</v>
-      </c>
-      <c r="M17">
-        <v>3</v>
-      </c>
-      <c r="N17">
-        <v>65</v>
-      </c>
-      <c r="O17">
-        <v>65</v>
-      </c>
-      <c r="P17" s="12">
-        <v>0.01</v>
-      </c>
-      <c r="Q17">
-        <v>10</v>
-      </c>
-      <c r="R17">
-        <v>10</v>
-      </c>
-      <c r="S17" s="12">
-        <v>0.03</v>
-      </c>
-      <c r="T17" s="12">
-        <v>0.01</v>
-      </c>
-      <c r="U17" s="12">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="V17" s="12" t="s">
-        <v>158</v>
-      </c>
-      <c r="W17" s="12">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="X17" s="12">
-        <v>0.12</v>
-      </c>
-      <c r="Y17" t="s">
-        <v>112</v>
-      </c>
-      <c r="Z17" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="AA17" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="AB17">
-        <v>1</v>
-      </c>
-      <c r="AC17" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="AD17" s="19">
-        <v>0.75</v>
-      </c>
-      <c r="AE17">
-        <v>200</v>
-      </c>
-      <c r="AF17" t="s">
-        <v>144</v>
-      </c>
-      <c r="AG17">
-        <v>5</v>
-      </c>
-      <c r="AH17">
-        <v>200</v>
-      </c>
-      <c r="AI17" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="AJ17">
-        <v>1</v>
-      </c>
-      <c r="AK17" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="AL17" s="14">
-        <v>0.25</v>
-      </c>
-      <c r="AM17" s="14">
-        <v>0.14499999999999999</v>
-      </c>
-      <c r="AN17" s="14">
-        <v>0.05</v>
-      </c>
-      <c r="AO17" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="AP17" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="AQ17" s="21" t="b">
-        <v>0</v>
-      </c>
+      <c r="B17" s="22"/>
+      <c r="L17" s="27"/>
+      <c r="AC17" s="2"/>
+      <c r="AD17" s="19"/>
+      <c r="AN17" s="25"/>
+      <c r="AP17" s="21"/>
+      <c r="AQ17" s="21"/>
     </row>
     <row r="18" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="B18" s="22" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C18" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D18" t="s">
         <v>109</v>
@@ -3286,7 +3268,7 @@
       <c r="U18" s="12">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="V18" t="s">
+      <c r="V18" s="12" t="s">
         <v>158</v>
       </c>
       <c r="W18" s="12">
@@ -3305,7 +3287,7 @@
         <v>114</v>
       </c>
       <c r="AB18">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="AC18" s="2" t="s">
         <v>169</v>
@@ -3355,13 +3337,13 @@
     </row>
     <row r="19" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="B19" s="22" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C19" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D19" t="s">
         <v>109</v>
@@ -3417,7 +3399,7 @@
       <c r="U19" s="12">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="V19" s="12" t="s">
+      <c r="V19" t="s">
         <v>158</v>
       </c>
       <c r="W19" s="12">
@@ -3436,7 +3418,7 @@
         <v>114</v>
       </c>
       <c r="AB19">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="AC19" s="2" t="s">
         <v>169</v>
@@ -3486,13 +3468,13 @@
     </row>
     <row r="20" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="B20" s="22" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C20" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D20" t="s">
         <v>109</v>
@@ -3564,7 +3546,7 @@
         <v>160</v>
       </c>
       <c r="AA20" s="2" t="s">
-        <v>161</v>
+        <v>114</v>
       </c>
       <c r="AB20">
         <v>30</v>
@@ -3617,13 +3599,13 @@
     </row>
     <row r="21" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>217</v>
+        <v>200</v>
       </c>
       <c r="B21" s="22" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C21" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D21" t="s">
         <v>109</v>
@@ -3679,7 +3661,7 @@
       <c r="U21" s="12">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="V21" t="s">
+      <c r="V21" s="12" t="s">
         <v>158</v>
       </c>
       <c r="W21" s="12">
@@ -3692,13 +3674,13 @@
         <v>112</v>
       </c>
       <c r="Z21" s="2" t="s">
-        <v>113</v>
+        <v>160</v>
       </c>
       <c r="AA21" s="2" t="s">
-        <v>114</v>
+        <v>161</v>
       </c>
       <c r="AB21">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="AC21" s="2" t="s">
         <v>169</v>
@@ -3748,13 +3730,13 @@
     </row>
     <row r="22" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="B22" s="22" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C22" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D22" t="s">
         <v>109</v>
@@ -3810,7 +3792,7 @@
       <c r="U22" s="12">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="V22" s="12" t="s">
+      <c r="V22" t="s">
         <v>158</v>
       </c>
       <c r="W22" s="12">
@@ -3829,7 +3811,7 @@
         <v>114</v>
       </c>
       <c r="AB22">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="AC22" s="2" t="s">
         <v>169</v>
@@ -3879,13 +3861,13 @@
     </row>
     <row r="23" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="B23" s="22" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C23" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D23" t="s">
         <v>109</v>
@@ -3957,7 +3939,7 @@
         <v>113</v>
       </c>
       <c r="AA23" s="2" t="s">
-        <v>161</v>
+        <v>114</v>
       </c>
       <c r="AB23">
         <v>30</v>
@@ -4010,13 +3992,13 @@
     </row>
     <row r="24" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="B24" s="22" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C24" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D24" t="s">
         <v>109</v>
@@ -4085,13 +4067,13 @@
         <v>112</v>
       </c>
       <c r="Z24" s="2" t="s">
-        <v>160</v>
+        <v>113</v>
       </c>
       <c r="AA24" s="2" t="s">
-        <v>114</v>
+        <v>161</v>
       </c>
       <c r="AB24">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="AC24" s="2" t="s">
         <v>169</v>
@@ -4103,7 +4085,7 @@
         <v>200</v>
       </c>
       <c r="AF24" t="s">
-        <v>117</v>
+        <v>144</v>
       </c>
       <c r="AG24">
         <v>5</v>
@@ -4141,13 +4123,13 @@
     </row>
     <row r="25" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="B25" s="22" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C25" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D25" t="s">
         <v>109</v>
@@ -4272,7 +4254,7 @@
     </row>
     <row r="26" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="B26" s="22" t="s">
         <v>177</v>
@@ -4350,10 +4332,10 @@
         <v>160</v>
       </c>
       <c r="AA26" s="2" t="s">
-        <v>161</v>
+        <v>114</v>
       </c>
       <c r="AB26">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="AC26" s="2" t="s">
         <v>169</v>
@@ -4368,7 +4350,7 @@
         <v>117</v>
       </c>
       <c r="AG26">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="AH26">
         <v>200</v>
@@ -4402,194 +4384,299 @@
       </c>
     </row>
     <row r="27" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="B27" s="22"/>
-      <c r="C27" s="11"/>
-      <c r="J27" s="12"/>
-      <c r="K27" s="21"/>
-      <c r="L27" s="12"/>
-      <c r="P27" s="12"/>
-      <c r="S27" s="12"/>
-      <c r="T27" s="12"/>
-      <c r="U27" s="12"/>
-      <c r="V27" s="12"/>
-      <c r="W27" s="12"/>
-      <c r="X27" s="12"/>
-      <c r="Z27" s="2"/>
-      <c r="AA27" s="2"/>
-      <c r="AC27" s="2"/>
-      <c r="AD27" s="19"/>
-      <c r="AI27" s="2"/>
-      <c r="AK27" s="2"/>
-      <c r="AL27" s="14"/>
-      <c r="AM27" s="14"/>
-      <c r="AN27" s="14"/>
-      <c r="AO27" s="21"/>
-      <c r="AP27" s="21"/>
-      <c r="AQ27" s="21"/>
+      <c r="A27" t="s">
+        <v>203</v>
+      </c>
+      <c r="B27" s="22" t="s">
+        <v>177</v>
+      </c>
+      <c r="C27" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D27" t="s">
+        <v>109</v>
+      </c>
+      <c r="E27" t="s">
+        <v>109</v>
+      </c>
+      <c r="F27" t="s">
+        <v>109</v>
+      </c>
+      <c r="G27" t="s">
+        <v>109</v>
+      </c>
+      <c r="H27" t="s">
+        <v>149</v>
+      </c>
+      <c r="I27" t="s">
+        <v>171</v>
+      </c>
+      <c r="J27" s="12">
+        <v>0</v>
+      </c>
+      <c r="K27" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="L27" s="12">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="M27">
+        <v>3</v>
+      </c>
+      <c r="N27">
+        <v>65</v>
+      </c>
+      <c r="O27">
+        <v>65</v>
+      </c>
+      <c r="P27" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="Q27">
+        <v>10</v>
+      </c>
+      <c r="R27">
+        <v>10</v>
+      </c>
+      <c r="S27" s="12">
+        <v>0.03</v>
+      </c>
+      <c r="T27" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="U27" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="V27" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="W27" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="X27" s="12">
+        <v>0.12</v>
+      </c>
+      <c r="Y27" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z27" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="AA27" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="AB27">
+        <v>30</v>
+      </c>
+      <c r="AC27" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="AD27" s="19">
+        <v>0.75</v>
+      </c>
+      <c r="AE27">
+        <v>200</v>
+      </c>
+      <c r="AF27" t="s">
+        <v>117</v>
+      </c>
+      <c r="AG27">
+        <v>5</v>
+      </c>
+      <c r="AH27">
+        <v>200</v>
+      </c>
+      <c r="AI27" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="AJ27">
+        <v>1</v>
+      </c>
+      <c r="AK27" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="AL27" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="AM27" s="14">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AN27" s="14">
+        <v>0.05</v>
+      </c>
+      <c r="AO27" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP27" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="AQ27" s="21" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="28" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="B28" s="22"/>
-      <c r="C28" s="11"/>
-      <c r="J28" s="12"/>
-      <c r="K28" s="21"/>
-      <c r="L28" s="12"/>
-      <c r="P28" s="12"/>
-      <c r="S28" s="12"/>
-      <c r="T28" s="12"/>
-      <c r="U28" s="12"/>
-      <c r="V28" s="12"/>
-      <c r="W28" s="12"/>
-      <c r="X28" s="12"/>
-      <c r="Z28" s="2"/>
-      <c r="AA28" s="2"/>
-      <c r="AC28" s="2"/>
-      <c r="AD28" s="19"/>
-      <c r="AI28" s="2"/>
-      <c r="AK28" s="2"/>
-      <c r="AL28" s="14"/>
-      <c r="AM28" s="14"/>
-      <c r="AN28" s="14"/>
-      <c r="AO28" s="21"/>
-      <c r="AP28" s="21"/>
-      <c r="AQ28" s="21"/>
-    </row>
-    <row r="29" spans="1:43" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="A28" t="s">
+        <v>213</v>
+      </c>
+      <c r="B28" s="22" t="s">
+        <v>177</v>
+      </c>
+      <c r="C28" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="D28" t="s">
+        <v>109</v>
+      </c>
+      <c r="E28" t="s">
+        <v>109</v>
+      </c>
+      <c r="F28" t="s">
+        <v>109</v>
+      </c>
+      <c r="G28" t="s">
+        <v>109</v>
+      </c>
+      <c r="H28" t="s">
+        <v>149</v>
+      </c>
+      <c r="I28" t="s">
+        <v>171</v>
+      </c>
+      <c r="J28" s="12">
+        <v>0</v>
+      </c>
+      <c r="K28" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="L28" s="12">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="M28">
+        <v>3</v>
+      </c>
+      <c r="N28">
+        <v>65</v>
+      </c>
+      <c r="O28">
+        <v>65</v>
+      </c>
+      <c r="P28" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="Q28">
+        <v>10</v>
+      </c>
+      <c r="R28">
+        <v>10</v>
+      </c>
+      <c r="S28" s="12">
+        <v>0.03</v>
+      </c>
+      <c r="T28" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="U28" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="V28" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="W28" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="X28" s="12">
+        <v>0.12</v>
+      </c>
+      <c r="Y28" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z28" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="AA28" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="AB28">
+        <v>30</v>
+      </c>
+      <c r="AC28" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="AD28" s="19">
+        <v>0.75</v>
+      </c>
+      <c r="AE28">
+        <v>200</v>
+      </c>
+      <c r="AF28" t="s">
+        <v>117</v>
+      </c>
+      <c r="AG28">
+        <v>10</v>
+      </c>
+      <c r="AH28">
+        <v>200</v>
+      </c>
+      <c r="AI28" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="AJ28">
+        <v>1</v>
+      </c>
+      <c r="AK28" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="AL28" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="AM28" s="14">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AN28" s="14">
+        <v>0.05</v>
+      </c>
+      <c r="AO28" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP28" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="AQ28" s="21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="B29" s="22"/>
+      <c r="C29" s="11"/>
+      <c r="J29" s="12"/>
+      <c r="K29" s="21"/>
+      <c r="L29" s="12"/>
+      <c r="P29" s="12"/>
+      <c r="S29" s="12"/>
+      <c r="T29" s="12"/>
+      <c r="U29" s="12"/>
+      <c r="V29" s="12"/>
+      <c r="W29" s="12"/>
+      <c r="X29" s="12"/>
+      <c r="Z29" s="2"/>
+      <c r="AA29" s="2"/>
+      <c r="AC29" s="2"/>
+      <c r="AD29" s="19"/>
+      <c r="AI29" s="2"/>
+      <c r="AK29" s="2"/>
+      <c r="AL29" s="14"/>
+      <c r="AM29" s="14"/>
+      <c r="AN29" s="14"/>
+      <c r="AO29" s="21"/>
+      <c r="AP29" s="21"/>
+      <c r="AQ29" s="21"/>
+    </row>
+    <row r="30" spans="1:43" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>192</v>
       </c>
-      <c r="B29" s="22" t="s">
+      <c r="B30" s="22" t="s">
         <v>180</v>
-      </c>
-      <c r="C29" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="D29" t="s">
-        <v>109</v>
-      </c>
-      <c r="E29" t="s">
-        <v>109</v>
-      </c>
-      <c r="F29" t="s">
-        <v>109</v>
-      </c>
-      <c r="G29" t="s">
-        <v>109</v>
-      </c>
-      <c r="H29" t="s">
-        <v>149</v>
-      </c>
-      <c r="I29" t="s">
-        <v>171</v>
-      </c>
-      <c r="J29" s="12">
-        <v>0</v>
-      </c>
-      <c r="K29" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="L29" s="12">
-        <v>1.7999999999999999E-2</v>
-      </c>
-      <c r="M29">
-        <v>3</v>
-      </c>
-      <c r="N29">
-        <v>65</v>
-      </c>
-      <c r="O29">
-        <v>65</v>
-      </c>
-      <c r="P29" s="12">
-        <v>0.01</v>
-      </c>
-      <c r="Q29">
-        <v>10</v>
-      </c>
-      <c r="R29">
-        <v>10</v>
-      </c>
-      <c r="S29" s="12">
-        <v>0.03</v>
-      </c>
-      <c r="T29" s="12">
-        <v>0.01</v>
-      </c>
-      <c r="U29" s="12">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="V29" s="12" t="s">
-        <v>158</v>
-      </c>
-      <c r="W29" s="12">
-        <v>8.2199999999999995E-2</v>
-      </c>
-      <c r="X29" s="12">
-        <v>0.12</v>
-      </c>
-      <c r="Y29" t="s">
-        <v>112</v>
-      </c>
-      <c r="Z29" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="AA29" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="AB29">
-        <v>30</v>
-      </c>
-      <c r="AC29" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="AD29" s="19">
-        <v>1</v>
-      </c>
-      <c r="AE29">
-        <v>200</v>
-      </c>
-      <c r="AF29" t="s">
-        <v>117</v>
-      </c>
-      <c r="AG29">
-        <v>5</v>
-      </c>
-      <c r="AH29">
-        <v>200</v>
-      </c>
-      <c r="AI29" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="AJ29">
-        <v>1</v>
-      </c>
-      <c r="AK29" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="AL29" s="14">
-        <v>0.25</v>
-      </c>
-      <c r="AM29" s="14">
-        <v>0.14499999999999999</v>
-      </c>
-      <c r="AN29" s="14">
-        <v>0.05</v>
-      </c>
-      <c r="AO29" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="AP29" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="AQ29" s="21" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>193</v>
-      </c>
-      <c r="B30" s="22" t="s">
-        <v>179</v>
       </c>
       <c r="C30" s="11" t="b">
         <v>1</v>
@@ -4652,7 +4739,7 @@
         <v>158</v>
       </c>
       <c r="W30" s="12">
-        <v>8.2199999999999995E-2</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="X30" s="12">
         <v>0.12</v>
@@ -4667,7 +4754,7 @@
         <v>161</v>
       </c>
       <c r="AB30">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="AC30" s="2" t="s">
         <v>169</v>
@@ -4717,10 +4804,10 @@
     </row>
     <row r="31" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B31" s="22" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C31" s="11" t="b">
         <v>1</v>
@@ -4777,13 +4864,13 @@
         <v>0.01</v>
       </c>
       <c r="U31" s="12">
-        <v>6.4000000000000001E-2</v>
+        <v>6.7799999999999999E-2</v>
       </c>
       <c r="V31" s="12" t="s">
         <v>158</v>
       </c>
       <c r="W31" s="12">
-        <v>8.2199999999999995E-2</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="X31" s="12">
         <v>0.12</v>
@@ -4846,9 +4933,35 @@
         <v>0</v>
       </c>
     </row>
+    <row r="32" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="B32" s="22"/>
+      <c r="C32" s="11"/>
+      <c r="J32" s="12"/>
+      <c r="K32" s="21"/>
+      <c r="L32" s="12"/>
+      <c r="P32" s="12"/>
+      <c r="S32" s="12"/>
+      <c r="T32" s="12"/>
+      <c r="U32" s="12"/>
+      <c r="V32" s="12"/>
+      <c r="W32" s="12"/>
+      <c r="X32" s="12"/>
+      <c r="Z32" s="2"/>
+      <c r="AA32" s="2"/>
+      <c r="AC32" s="2"/>
+      <c r="AD32" s="19"/>
+      <c r="AI32" s="2"/>
+      <c r="AK32" s="2"/>
+      <c r="AL32" s="14"/>
+      <c r="AM32" s="14"/>
+      <c r="AN32" s="14"/>
+      <c r="AO32" s="21"/>
+      <c r="AP32" s="21"/>
+      <c r="AQ32" s="21"/>
+    </row>
     <row r="33" spans="1:43" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B33" s="22" t="s">
         <v>180</v>
@@ -4914,10 +5027,10 @@
         <v>158</v>
       </c>
       <c r="W33" s="12">
-        <v>7.4999999999999997E-2</v>
+        <v>6.4000000000000001E-2</v>
       </c>
       <c r="X33" s="12">
-        <v>0.12</v>
+        <v>0.08</v>
       </c>
       <c r="Y33" t="s">
         <v>112</v>
@@ -4979,7 +5092,7 @@
     </row>
     <row r="34" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B34" s="22" t="s">
         <v>179</v>
@@ -5045,10 +5158,10 @@
         <v>158</v>
       </c>
       <c r="W34" s="12">
-        <v>7.4999999999999997E-2</v>
+        <v>6.4000000000000001E-2</v>
       </c>
       <c r="X34" s="12">
-        <v>0.12</v>
+        <v>0.08</v>
       </c>
       <c r="Y34" t="s">
         <v>112</v>
@@ -5110,7 +5223,7 @@
     </row>
     <row r="35" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B35" s="22" t="s">
         <v>181</v>
@@ -5176,10 +5289,10 @@
         <v>158</v>
       </c>
       <c r="W35" s="12">
-        <v>7.4999999999999997E-2</v>
+        <v>6.4000000000000001E-2</v>
       </c>
       <c r="X35" s="12">
-        <v>0.12</v>
+        <v>0.08</v>
       </c>
       <c r="Y35" t="s">
         <v>112</v>
@@ -5241,7 +5354,7 @@
     </row>
     <row r="37" spans="1:43" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="B37" s="22" t="s">
         <v>180</v>
@@ -5307,10 +5420,10 @@
         <v>158</v>
       </c>
       <c r="W37" s="12">
-        <v>6.4000000000000001E-2</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="X37" s="12">
-        <v>0.08</v>
+        <v>0.12</v>
       </c>
       <c r="Y37" t="s">
         <v>112</v>
@@ -5328,7 +5441,7 @@
         <v>169</v>
       </c>
       <c r="AD37" s="19">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="AE37">
         <v>200</v>
@@ -5372,7 +5485,7 @@
     </row>
     <row r="38" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="B38" s="22" t="s">
         <v>179</v>
@@ -5432,16 +5545,16 @@
         <v>0.01</v>
       </c>
       <c r="U38" s="12">
-        <v>7.4999999999999997E-2</v>
+        <v>6.7799999999999999E-2</v>
       </c>
       <c r="V38" s="12" t="s">
         <v>158</v>
       </c>
       <c r="W38" s="12">
-        <v>6.4000000000000001E-2</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="X38" s="12">
-        <v>0.08</v>
+        <v>0.12</v>
       </c>
       <c r="Y38" t="s">
         <v>112</v>
@@ -5459,7 +5572,7 @@
         <v>169</v>
       </c>
       <c r="AD38" s="19">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="AE38">
         <v>200</v>
@@ -5502,142 +5615,168 @@
       </c>
     </row>
     <row r="39" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="B39" s="22"/>
+      <c r="C39" s="11"/>
+      <c r="J39" s="12"/>
+      <c r="K39" s="21"/>
+      <c r="L39" s="12"/>
+      <c r="P39" s="12"/>
+      <c r="S39" s="12"/>
+      <c r="T39" s="12"/>
+      <c r="U39" s="12"/>
+      <c r="V39" s="12"/>
+      <c r="W39" s="12"/>
+      <c r="X39" s="12"/>
+      <c r="Z39" s="2"/>
+      <c r="AA39" s="2"/>
+      <c r="AC39" s="2"/>
+      <c r="AD39" s="19"/>
+      <c r="AI39" s="2"/>
+      <c r="AK39" s="2"/>
+      <c r="AL39" s="14"/>
+      <c r="AM39" s="14"/>
+      <c r="AN39" s="14"/>
+      <c r="AO39" s="21"/>
+      <c r="AP39" s="21"/>
+      <c r="AQ39" s="21"/>
+    </row>
+    <row r="40" spans="1:43" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>206</v>
+      </c>
+      <c r="B40" s="22" t="s">
+        <v>180</v>
+      </c>
+      <c r="C40" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="D40" t="s">
+        <v>109</v>
+      </c>
+      <c r="E40" t="s">
+        <v>109</v>
+      </c>
+      <c r="F40" t="s">
+        <v>109</v>
+      </c>
+      <c r="G40" t="s">
+        <v>109</v>
+      </c>
+      <c r="H40" t="s">
+        <v>149</v>
+      </c>
+      <c r="I40" t="s">
+        <v>171</v>
+      </c>
+      <c r="J40" s="12">
+        <v>0</v>
+      </c>
+      <c r="K40" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="L40" s="12">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="M40">
+        <v>3</v>
+      </c>
+      <c r="N40">
+        <v>65</v>
+      </c>
+      <c r="O40">
+        <v>65</v>
+      </c>
+      <c r="P40" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="Q40">
+        <v>10</v>
+      </c>
+      <c r="R40">
+        <v>10</v>
+      </c>
+      <c r="S40" s="12">
+        <v>0.03</v>
+      </c>
+      <c r="T40" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="U40" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="V40" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="W40" s="12">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="X40" s="12">
+        <v>0.08</v>
+      </c>
+      <c r="Y40" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z40" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="AA40" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="AB40">
+        <v>30</v>
+      </c>
+      <c r="AC40" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="AD40" s="19">
+        <v>0.75</v>
+      </c>
+      <c r="AE40">
         <v>200</v>
       </c>
-      <c r="B39" s="22" t="s">
-        <v>181</v>
-      </c>
-      <c r="C39" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="D39" t="s">
-        <v>109</v>
-      </c>
-      <c r="E39" t="s">
-        <v>109</v>
-      </c>
-      <c r="F39" t="s">
-        <v>109</v>
-      </c>
-      <c r="G39" t="s">
-        <v>109</v>
-      </c>
-      <c r="H39" t="s">
-        <v>149</v>
-      </c>
-      <c r="I39" t="s">
-        <v>171</v>
-      </c>
-      <c r="J39" s="12">
-        <v>0</v>
-      </c>
-      <c r="K39" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="L39" s="12">
-        <v>1.7999999999999999E-2</v>
-      </c>
-      <c r="M39">
-        <v>3</v>
-      </c>
-      <c r="N39">
-        <v>65</v>
-      </c>
-      <c r="O39">
-        <v>65</v>
-      </c>
-      <c r="P39" s="12">
-        <v>0.01</v>
-      </c>
-      <c r="Q39">
-        <v>10</v>
-      </c>
-      <c r="R39">
-        <v>10</v>
-      </c>
-      <c r="S39" s="12">
-        <v>0.03</v>
-      </c>
-      <c r="T39" s="12">
-        <v>0.01</v>
-      </c>
-      <c r="U39" s="12">
-        <v>6.4000000000000001E-2</v>
-      </c>
-      <c r="V39" s="12" t="s">
-        <v>158</v>
-      </c>
-      <c r="W39" s="12">
-        <v>6.4000000000000001E-2</v>
-      </c>
-      <c r="X39" s="12">
-        <v>0.08</v>
-      </c>
-      <c r="Y39" t="s">
-        <v>112</v>
-      </c>
-      <c r="Z39" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="AA39" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="AB39">
-        <v>15</v>
-      </c>
-      <c r="AC39" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="AD39" s="19">
-        <v>1</v>
-      </c>
-      <c r="AE39">
+      <c r="AF40" t="s">
+        <v>117</v>
+      </c>
+      <c r="AG40">
+        <v>5</v>
+      </c>
+      <c r="AH40">
         <v>200</v>
       </c>
-      <c r="AF39" t="s">
-        <v>117</v>
-      </c>
-      <c r="AG39">
-        <v>5</v>
-      </c>
-      <c r="AH39">
-        <v>200</v>
-      </c>
-      <c r="AI39" s="2" t="s">
+      <c r="AI40" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="AJ39">
-        <v>1</v>
-      </c>
-      <c r="AK39" s="2" t="s">
+      <c r="AJ40">
+        <v>1</v>
+      </c>
+      <c r="AK40" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="AL39" s="14">
+      <c r="AL40" s="14">
         <v>0.25</v>
       </c>
-      <c r="AM39" s="14">
+      <c r="AM40" s="14">
         <v>0.14499999999999999</v>
       </c>
-      <c r="AN39" s="14">
+      <c r="AN40" s="14">
         <v>0.05</v>
       </c>
-      <c r="AO39" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="AP39" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="AQ39" s="21" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:43" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AO40" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP40" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="AQ40" s="21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B41" s="22" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C41" s="11" t="b">
         <v>1</v>
@@ -5700,10 +5839,10 @@
         <v>158</v>
       </c>
       <c r="W41" s="12">
-        <v>8.2199999999999995E-2</v>
+        <v>6.4000000000000001E-2</v>
       </c>
       <c r="X41" s="12">
-        <v>0.12</v>
+        <v>0.08</v>
       </c>
       <c r="Y41" t="s">
         <v>112</v>
@@ -5715,7 +5854,7 @@
         <v>161</v>
       </c>
       <c r="AB41">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="AC41" s="2" t="s">
         <v>169</v>
@@ -5765,10 +5904,10 @@
     </row>
     <row r="42" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B42" s="22" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C42" s="11" t="b">
         <v>1</v>
@@ -5825,16 +5964,16 @@
         <v>0.01</v>
       </c>
       <c r="U42" s="12">
-        <v>7.4999999999999997E-2</v>
+        <v>6.4000000000000001E-2</v>
       </c>
       <c r="V42" s="12" t="s">
         <v>158</v>
       </c>
       <c r="W42" s="12">
-        <v>8.2199999999999995E-2</v>
+        <v>6.4000000000000001E-2</v>
       </c>
       <c r="X42" s="12">
-        <v>0.12</v>
+        <v>0.08</v>
       </c>
       <c r="Y42" t="s">
         <v>112</v>
@@ -5891,929 +6030,6 @@
         <v>1</v>
       </c>
       <c r="AQ42" s="21" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>210</v>
-      </c>
-      <c r="B43" s="22" t="s">
-        <v>181</v>
-      </c>
-      <c r="C43" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="D43" t="s">
-        <v>109</v>
-      </c>
-      <c r="E43" t="s">
-        <v>109</v>
-      </c>
-      <c r="F43" t="s">
-        <v>109</v>
-      </c>
-      <c r="G43" t="s">
-        <v>109</v>
-      </c>
-      <c r="H43" t="s">
-        <v>149</v>
-      </c>
-      <c r="I43" t="s">
-        <v>171</v>
-      </c>
-      <c r="J43" s="12">
-        <v>0</v>
-      </c>
-      <c r="K43" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="L43" s="12">
-        <v>1.7999999999999999E-2</v>
-      </c>
-      <c r="M43">
-        <v>3</v>
-      </c>
-      <c r="N43">
-        <v>65</v>
-      </c>
-      <c r="O43">
-        <v>65</v>
-      </c>
-      <c r="P43" s="12">
-        <v>0.01</v>
-      </c>
-      <c r="Q43">
-        <v>10</v>
-      </c>
-      <c r="R43">
-        <v>10</v>
-      </c>
-      <c r="S43" s="12">
-        <v>0.03</v>
-      </c>
-      <c r="T43" s="12">
-        <v>0.01</v>
-      </c>
-      <c r="U43" s="12">
-        <v>6.4000000000000001E-2</v>
-      </c>
-      <c r="V43" s="12" t="s">
-        <v>158</v>
-      </c>
-      <c r="W43" s="12">
-        <v>8.2199999999999995E-2</v>
-      </c>
-      <c r="X43" s="12">
-        <v>0.12</v>
-      </c>
-      <c r="Y43" t="s">
-        <v>112</v>
-      </c>
-      <c r="Z43" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="AA43" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="AB43">
-        <v>15</v>
-      </c>
-      <c r="AC43" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="AD43" s="19">
-        <v>0.75</v>
-      </c>
-      <c r="AE43">
-        <v>200</v>
-      </c>
-      <c r="AF43" t="s">
-        <v>117</v>
-      </c>
-      <c r="AG43">
-        <v>5</v>
-      </c>
-      <c r="AH43">
-        <v>200</v>
-      </c>
-      <c r="AI43" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="AJ43">
-        <v>1</v>
-      </c>
-      <c r="AK43" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="AL43" s="14">
-        <v>0.25</v>
-      </c>
-      <c r="AM43" s="14">
-        <v>0.14499999999999999</v>
-      </c>
-      <c r="AN43" s="14">
-        <v>0.05</v>
-      </c>
-      <c r="AO43" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="AP43" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="AQ43" s="21" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="AD44" s="19"/>
-    </row>
-    <row r="45" spans="1:43" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>211</v>
-      </c>
-      <c r="B45" s="22" t="s">
-        <v>180</v>
-      </c>
-      <c r="C45" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="D45" t="s">
-        <v>109</v>
-      </c>
-      <c r="E45" t="s">
-        <v>109</v>
-      </c>
-      <c r="F45" t="s">
-        <v>109</v>
-      </c>
-      <c r="G45" t="s">
-        <v>109</v>
-      </c>
-      <c r="H45" t="s">
-        <v>149</v>
-      </c>
-      <c r="I45" t="s">
-        <v>171</v>
-      </c>
-      <c r="J45" s="12">
-        <v>0</v>
-      </c>
-      <c r="K45" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="L45" s="12">
-        <v>1.7999999999999999E-2</v>
-      </c>
-      <c r="M45">
-        <v>3</v>
-      </c>
-      <c r="N45">
-        <v>65</v>
-      </c>
-      <c r="O45">
-        <v>65</v>
-      </c>
-      <c r="P45" s="12">
-        <v>0.01</v>
-      </c>
-      <c r="Q45">
-        <v>10</v>
-      </c>
-      <c r="R45">
-        <v>10</v>
-      </c>
-      <c r="S45" s="12">
-        <v>0.03</v>
-      </c>
-      <c r="T45" s="12">
-        <v>0.01</v>
-      </c>
-      <c r="U45" s="12">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="V45" s="12" t="s">
-        <v>158</v>
-      </c>
-      <c r="W45" s="12">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="X45" s="12">
-        <v>0.12</v>
-      </c>
-      <c r="Y45" t="s">
-        <v>112</v>
-      </c>
-      <c r="Z45" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="AA45" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="AB45">
-        <v>30</v>
-      </c>
-      <c r="AC45" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="AD45" s="19">
-        <v>0.75</v>
-      </c>
-      <c r="AE45">
-        <v>200</v>
-      </c>
-      <c r="AF45" t="s">
-        <v>117</v>
-      </c>
-      <c r="AG45">
-        <v>5</v>
-      </c>
-      <c r="AH45">
-        <v>200</v>
-      </c>
-      <c r="AI45" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="AJ45">
-        <v>1</v>
-      </c>
-      <c r="AK45" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="AL45" s="14">
-        <v>0.25</v>
-      </c>
-      <c r="AM45" s="14">
-        <v>0.14499999999999999</v>
-      </c>
-      <c r="AN45" s="14">
-        <v>0.05</v>
-      </c>
-      <c r="AO45" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="AP45" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="AQ45" s="21" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>212</v>
-      </c>
-      <c r="B46" s="22" t="s">
-        <v>179</v>
-      </c>
-      <c r="C46" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="D46" t="s">
-        <v>109</v>
-      </c>
-      <c r="E46" t="s">
-        <v>109</v>
-      </c>
-      <c r="F46" t="s">
-        <v>109</v>
-      </c>
-      <c r="G46" t="s">
-        <v>109</v>
-      </c>
-      <c r="H46" t="s">
-        <v>149</v>
-      </c>
-      <c r="I46" t="s">
-        <v>171</v>
-      </c>
-      <c r="J46" s="12">
-        <v>0</v>
-      </c>
-      <c r="K46" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="L46" s="12">
-        <v>1.7999999999999999E-2</v>
-      </c>
-      <c r="M46">
-        <v>3</v>
-      </c>
-      <c r="N46">
-        <v>65</v>
-      </c>
-      <c r="O46">
-        <v>65</v>
-      </c>
-      <c r="P46" s="12">
-        <v>0.01</v>
-      </c>
-      <c r="Q46">
-        <v>10</v>
-      </c>
-      <c r="R46">
-        <v>10</v>
-      </c>
-      <c r="S46" s="12">
-        <v>0.03</v>
-      </c>
-      <c r="T46" s="12">
-        <v>0.01</v>
-      </c>
-      <c r="U46" s="12">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="V46" s="12" t="s">
-        <v>158</v>
-      </c>
-      <c r="W46" s="12">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="X46" s="12">
-        <v>0.12</v>
-      </c>
-      <c r="Y46" t="s">
-        <v>112</v>
-      </c>
-      <c r="Z46" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="AA46" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="AB46">
-        <v>15</v>
-      </c>
-      <c r="AC46" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="AD46" s="19">
-        <v>0.75</v>
-      </c>
-      <c r="AE46">
-        <v>200</v>
-      </c>
-      <c r="AF46" t="s">
-        <v>117</v>
-      </c>
-      <c r="AG46">
-        <v>5</v>
-      </c>
-      <c r="AH46">
-        <v>200</v>
-      </c>
-      <c r="AI46" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="AJ46">
-        <v>1</v>
-      </c>
-      <c r="AK46" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="AL46" s="14">
-        <v>0.25</v>
-      </c>
-      <c r="AM46" s="14">
-        <v>0.14499999999999999</v>
-      </c>
-      <c r="AN46" s="14">
-        <v>0.05</v>
-      </c>
-      <c r="AO46" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="AP46" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="AQ46" s="21" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>213</v>
-      </c>
-      <c r="B47" s="22" t="s">
-        <v>181</v>
-      </c>
-      <c r="C47" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="D47" t="s">
-        <v>109</v>
-      </c>
-      <c r="E47" t="s">
-        <v>109</v>
-      </c>
-      <c r="F47" t="s">
-        <v>109</v>
-      </c>
-      <c r="G47" t="s">
-        <v>109</v>
-      </c>
-      <c r="H47" t="s">
-        <v>149</v>
-      </c>
-      <c r="I47" t="s">
-        <v>171</v>
-      </c>
-      <c r="J47" s="12">
-        <v>0</v>
-      </c>
-      <c r="K47" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="L47" s="12">
-        <v>1.7999999999999999E-2</v>
-      </c>
-      <c r="M47">
-        <v>3</v>
-      </c>
-      <c r="N47">
-        <v>65</v>
-      </c>
-      <c r="O47">
-        <v>65</v>
-      </c>
-      <c r="P47" s="12">
-        <v>0.01</v>
-      </c>
-      <c r="Q47">
-        <v>10</v>
-      </c>
-      <c r="R47">
-        <v>10</v>
-      </c>
-      <c r="S47" s="12">
-        <v>0.03</v>
-      </c>
-      <c r="T47" s="12">
-        <v>0.01</v>
-      </c>
-      <c r="U47" s="12">
-        <v>6.4000000000000001E-2</v>
-      </c>
-      <c r="V47" s="12" t="s">
-        <v>158</v>
-      </c>
-      <c r="W47" s="12">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="X47" s="12">
-        <v>0.12</v>
-      </c>
-      <c r="Y47" t="s">
-        <v>112</v>
-      </c>
-      <c r="Z47" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="AA47" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="AB47">
-        <v>15</v>
-      </c>
-      <c r="AC47" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="AD47" s="19">
-        <v>0.75</v>
-      </c>
-      <c r="AE47">
-        <v>200</v>
-      </c>
-      <c r="AF47" t="s">
-        <v>117</v>
-      </c>
-      <c r="AG47">
-        <v>5</v>
-      </c>
-      <c r="AH47">
-        <v>200</v>
-      </c>
-      <c r="AI47" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="AJ47">
-        <v>1</v>
-      </c>
-      <c r="AK47" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="AL47" s="14">
-        <v>0.25</v>
-      </c>
-      <c r="AM47" s="14">
-        <v>0.14499999999999999</v>
-      </c>
-      <c r="AN47" s="14">
-        <v>0.05</v>
-      </c>
-      <c r="AO47" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="AP47" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="AQ47" s="21" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="AD48" s="19"/>
-    </row>
-    <row r="49" spans="1:43" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>214</v>
-      </c>
-      <c r="B49" s="22" t="s">
-        <v>180</v>
-      </c>
-      <c r="C49" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="D49" t="s">
-        <v>109</v>
-      </c>
-      <c r="E49" t="s">
-        <v>109</v>
-      </c>
-      <c r="F49" t="s">
-        <v>109</v>
-      </c>
-      <c r="G49" t="s">
-        <v>109</v>
-      </c>
-      <c r="H49" t="s">
-        <v>149</v>
-      </c>
-      <c r="I49" t="s">
-        <v>171</v>
-      </c>
-      <c r="J49" s="12">
-        <v>0</v>
-      </c>
-      <c r="K49" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="L49" s="12">
-        <v>1.7999999999999999E-2</v>
-      </c>
-      <c r="M49">
-        <v>3</v>
-      </c>
-      <c r="N49">
-        <v>65</v>
-      </c>
-      <c r="O49">
-        <v>65</v>
-      </c>
-      <c r="P49" s="12">
-        <v>0.01</v>
-      </c>
-      <c r="Q49">
-        <v>10</v>
-      </c>
-      <c r="R49">
-        <v>10</v>
-      </c>
-      <c r="S49" s="12">
-        <v>0.03</v>
-      </c>
-      <c r="T49" s="12">
-        <v>0.01</v>
-      </c>
-      <c r="U49" s="12">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="V49" s="12" t="s">
-        <v>158</v>
-      </c>
-      <c r="W49" s="12">
-        <v>6.4000000000000001E-2</v>
-      </c>
-      <c r="X49" s="12">
-        <v>0.08</v>
-      </c>
-      <c r="Y49" t="s">
-        <v>112</v>
-      </c>
-      <c r="Z49" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="AA49" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="AB49">
-        <v>30</v>
-      </c>
-      <c r="AC49" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="AD49" s="19">
-        <v>0.75</v>
-      </c>
-      <c r="AE49">
-        <v>200</v>
-      </c>
-      <c r="AF49" t="s">
-        <v>117</v>
-      </c>
-      <c r="AG49">
-        <v>5</v>
-      </c>
-      <c r="AH49">
-        <v>200</v>
-      </c>
-      <c r="AI49" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="AJ49">
-        <v>1</v>
-      </c>
-      <c r="AK49" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="AL49" s="14">
-        <v>0.25</v>
-      </c>
-      <c r="AM49" s="14">
-        <v>0.14499999999999999</v>
-      </c>
-      <c r="AN49" s="14">
-        <v>0.05</v>
-      </c>
-      <c r="AO49" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="AP49" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="AQ49" s="21" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>215</v>
-      </c>
-      <c r="B50" s="22" t="s">
-        <v>179</v>
-      </c>
-      <c r="C50" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="D50" t="s">
-        <v>109</v>
-      </c>
-      <c r="E50" t="s">
-        <v>109</v>
-      </c>
-      <c r="F50" t="s">
-        <v>109</v>
-      </c>
-      <c r="G50" t="s">
-        <v>109</v>
-      </c>
-      <c r="H50" t="s">
-        <v>149</v>
-      </c>
-      <c r="I50" t="s">
-        <v>171</v>
-      </c>
-      <c r="J50" s="12">
-        <v>0</v>
-      </c>
-      <c r="K50" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="L50" s="12">
-        <v>1.7999999999999999E-2</v>
-      </c>
-      <c r="M50">
-        <v>3</v>
-      </c>
-      <c r="N50">
-        <v>65</v>
-      </c>
-      <c r="O50">
-        <v>65</v>
-      </c>
-      <c r="P50" s="12">
-        <v>0.01</v>
-      </c>
-      <c r="Q50">
-        <v>10</v>
-      </c>
-      <c r="R50">
-        <v>10</v>
-      </c>
-      <c r="S50" s="12">
-        <v>0.03</v>
-      </c>
-      <c r="T50" s="12">
-        <v>0.01</v>
-      </c>
-      <c r="U50" s="12">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="V50" s="12" t="s">
-        <v>158</v>
-      </c>
-      <c r="W50" s="12">
-        <v>6.4000000000000001E-2</v>
-      </c>
-      <c r="X50" s="12">
-        <v>0.08</v>
-      </c>
-      <c r="Y50" t="s">
-        <v>112</v>
-      </c>
-      <c r="Z50" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="AA50" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="AB50">
-        <v>15</v>
-      </c>
-      <c r="AC50" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="AD50" s="19">
-        <v>0.75</v>
-      </c>
-      <c r="AE50">
-        <v>200</v>
-      </c>
-      <c r="AF50" t="s">
-        <v>117</v>
-      </c>
-      <c r="AG50">
-        <v>5</v>
-      </c>
-      <c r="AH50">
-        <v>200</v>
-      </c>
-      <c r="AI50" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="AJ50">
-        <v>1</v>
-      </c>
-      <c r="AK50" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="AL50" s="14">
-        <v>0.25</v>
-      </c>
-      <c r="AM50" s="14">
-        <v>0.14499999999999999</v>
-      </c>
-      <c r="AN50" s="14">
-        <v>0.05</v>
-      </c>
-      <c r="AO50" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="AP50" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="AQ50" s="21" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>216</v>
-      </c>
-      <c r="B51" s="22" t="s">
-        <v>181</v>
-      </c>
-      <c r="C51" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="D51" t="s">
-        <v>109</v>
-      </c>
-      <c r="E51" t="s">
-        <v>109</v>
-      </c>
-      <c r="F51" t="s">
-        <v>109</v>
-      </c>
-      <c r="G51" t="s">
-        <v>109</v>
-      </c>
-      <c r="H51" t="s">
-        <v>149</v>
-      </c>
-      <c r="I51" t="s">
-        <v>171</v>
-      </c>
-      <c r="J51" s="12">
-        <v>0</v>
-      </c>
-      <c r="K51" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="L51" s="12">
-        <v>1.7999999999999999E-2</v>
-      </c>
-      <c r="M51">
-        <v>3</v>
-      </c>
-      <c r="N51">
-        <v>65</v>
-      </c>
-      <c r="O51">
-        <v>65</v>
-      </c>
-      <c r="P51" s="12">
-        <v>0.01</v>
-      </c>
-      <c r="Q51">
-        <v>10</v>
-      </c>
-      <c r="R51">
-        <v>10</v>
-      </c>
-      <c r="S51" s="12">
-        <v>0.03</v>
-      </c>
-      <c r="T51" s="12">
-        <v>0.01</v>
-      </c>
-      <c r="U51" s="12">
-        <v>6.4000000000000001E-2</v>
-      </c>
-      <c r="V51" s="12" t="s">
-        <v>158</v>
-      </c>
-      <c r="W51" s="12">
-        <v>6.4000000000000001E-2</v>
-      </c>
-      <c r="X51" s="12">
-        <v>0.08</v>
-      </c>
-      <c r="Y51" t="s">
-        <v>112</v>
-      </c>
-      <c r="Z51" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="AA51" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="AB51">
-        <v>15</v>
-      </c>
-      <c r="AC51" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="AD51" s="19">
-        <v>0.75</v>
-      </c>
-      <c r="AE51">
-        <v>200</v>
-      </c>
-      <c r="AF51" t="s">
-        <v>117</v>
-      </c>
-      <c r="AG51">
-        <v>5</v>
-      </c>
-      <c r="AH51">
-        <v>200</v>
-      </c>
-      <c r="AI51" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="AJ51">
-        <v>1</v>
-      </c>
-      <c r="AK51" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="AL51" s="14">
-        <v>0.25</v>
-      </c>
-      <c r="AM51" s="14">
-        <v>0.14499999999999999</v>
-      </c>
-      <c r="AN51" s="14">
-        <v>0.05</v>
-      </c>
-      <c r="AO51" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="AP51" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="AQ51" s="21" t="b">
         <v>0</v>
       </c>
     </row>
@@ -6832,78 +6048,78 @@
     <mergeCell ref="V4:X4"/>
   </mergeCells>
   <dataValidations count="20">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AI49:AI51 AI6:AI15 AI33:AI35 AI37:AI39 AI41:AI43 AI45:AI47 AI17:AI31">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AI6:AI16 AI18:AI35 AI37:AI42">
       <formula1>"MA,EAA"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA49:AA51 AA6:AA15 AA33:AA35 AA37:AA39 AA41:AA43 AA45:AA47 AA17:AA31">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA6:AA16 AA18:AA35 AA37:AA42">
       <formula1>"cd,cp,sl"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z49:Z51 Z6:Z15 Z33:Z35 Z37:Z39 Z41:Z43 Z45:Z47 Z17:Z31">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z6:Z16 Z18:Z35 Z37:Z42">
       <formula1>"open,closed"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AK49:AK51 AK6:AK15 AK33:AK35 AK37:AK39 AK41:AK43 AK45:AK47 AK17:AK31">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AK6:AK16 AK18:AK35 AK37:AK42">
       <formula1>ConPolicy</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C45:C47 K17:K31 C6:C15 K33:K35 C17:C31 K37:K39 C33:C35 K41:K43 C37:C39 K45:K47 C41:C43 K49:K51 K6:K15 C49:C51">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K6:K16 C6:C16 C18:C35 K18:K35 K37:K42 C37:C42">
       <formula1>"TRUE,FALSE"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer 55 to 65, please" sqref="N49:N51 N6:N15 N33:N35 N37:N39 N41:N43 N45:N47 N17:N31">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer 55 to 65, please" sqref="N6:N16 N18:N35 N37:N42">
       <formula1>55</formula1>
       <formula2>65</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-10% please" sqref="P49:P51 P17:P31 P6:P15 T33:T35 P33:P35 T37:T39 P37:P39 T41:T43 P41:P43 T45:T47 P45:P47 T49:T51 T6:T15 T17:T31">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-10% please" sqref="T6:T16 P6:P16 P18:P35 T18:T35 T37:T42 P37:P42">
       <formula1>0</formula1>
       <formula2>0.1</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 0-15" sqref="Q49:R51 Q6:R15 Q33:R35 Q37:R39 Q41:R43 Q45:R47 Q17:R31">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 0-15" sqref="Q6:R16 Q18:R35 Q37:R42">
       <formula1>0</formula1>
       <formula2>15</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="U45:U47 S17:S31 U17:U31 U6:U15 S33:S35 W17:W31 W33:W35 S37:S39 U33:U35 W49:W51 S41:S43 S6:S15 U37:U39 S45:S47 W6:W15 U41:U43 S49:S51 W37:W39 W41:W43 W45:W47 U49:U51">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="S6:S16 U6:U16 W6:W16 S18:S35 U18:U35 W18:W35 S37:S42 W37:W42 U37:U42">
       <formula1>0</formula1>
       <formula2>0.2</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 0 to 30, please" sqref="AB6:AB15 AB17:AB31 AB33:AB35 AB37:AB39 AB41:AB43 AB45:AB47 AB49:AB51">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 0 to 30, please" sqref="AB6:AB16 AB18:AB35 AB37:AB42">
       <formula1>0</formula1>
       <formula2>30</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-75%" sqref="AL49:AM51 AL6:AM15 AL33:AM35 AL37:AM39 AL41:AM43 AL45:AM47 AL17:AM31">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-75%" sqref="AL6:AM16 AL18:AM35 AL37:AM42">
       <formula1>0</formula1>
       <formula2>0.75</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-30%" sqref="AN49:AN51 AN6:AN15 AN33:AN35 AN37:AN39 AN41:AN43 AN45:AN47 AN17:AN31">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-30%" sqref="AN6:AN16 AN18:AN35 AN37:AN42">
       <formula1>0</formula1>
       <formula2>0.3</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-75% please" sqref="X37:X39 X6:X15 X33:X35 X17:X31 X49:X51 X45:X47 X41:X43">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-75% please" sqref="X6:X16 X18:X35 X37:X42">
       <formula1>0</formula1>
       <formula2>0.75</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 1 to 30" sqref="AG49:AG51 AG6:AG15 AG33:AG35 AG37:AG39 AG41:AG43 AG45:AG47 AG17:AG31">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 1 to 30" sqref="AG6:AG16 AG18:AG35 AG37:AG42">
       <formula1>1</formula1>
       <formula2>30</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AH49:AH51 AH6:AH15 AH33:AH35 AH37:AH39 AH41:AH43 AH45:AH47 AH17:AH31">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AH6:AH16 AH18:AH35 AH37:AH42">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AJ49:AJ51 AJ6:AJ15 AJ33:AJ35 AJ37:AJ39 AJ41:AJ43 AJ45:AJ47 AJ17:AJ31">
+    <dataValidation type="decimal" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AJ6:AJ16 AJ18:AJ35 AJ37:AJ42">
       <formula1>1</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="V49:V51 V6:V15 V33:V35 V37:V39 V41:V43 V45:V47 V17:V31"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AO49:AQ51 AO33:AQ35 AO37:AQ39 AO41:AQ43 AO45:AQ47 AO6:AQ31">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="V6:V16 V18:V35 V37:V42"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AO6:AQ35 AO37:AQ42">
       <formula1>"TRUE, FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AC49:AC51 AC33:AC35 AC37:AC39 AC41:AC43 AC45:AC47 AC6:AC31">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AC6:AC35 AC37:AC42">
       <formula1>"MA,AL,AL_pct"</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AD41:AD51 AD33:AD35 AD37:AD39 AD6:AD31">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AD6:AD35 AD37:AD42">
       <formula1>0</formula1>
       <formula2>1.5</formula2>
     </dataValidation>
@@ -6917,13 +6133,13 @@
           <x14:formula1>
             <xm:f>DropDowns!$A$37:$A$41</xm:f>
           </x14:formula1>
-          <xm:sqref>H49:H51 H33:H35 H37:H39 H41:H43 H45:H47 H6:H31</xm:sqref>
+          <xm:sqref>H6:H35 H37:H42</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DropDowns!$A$44:$A$46</xm:f>
           </x14:formula1>
-          <xm:sqref>I49:I51 I33:I35 I37:I39 I41:I43 I45:I47 I6:I31</xm:sqref>
+          <xm:sqref>I6:I35 I37:I42</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -7055,7 +6271,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7093,13 +6309,13 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="B3">
         <v>1000</v>
       </c>
       <c r="C3">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D3">
         <v>20</v>

</xml_diff>

<commit_message>
changes for M1 and M2.1
</commit_message>
<xml_diff>
--- a/IO_M1/RunControl_M1.xlsx
+++ b/IO_M1/RunControl_M1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19164" windowHeight="7164" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TOC" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="908" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1036" uniqueCount="273">
   <si>
     <t>Sheet #</t>
   </si>
@@ -772,9 +772,6 @@
     <t>75% initial Funding; BRP: open 30-year cp; 5-year asset smoothing, DR 6.4%, ir 7.5%, sd 12%</t>
   </si>
   <si>
-    <t>75% initial Funding; Open 10-year cd; no asset smoothing</t>
-  </si>
-  <si>
     <t>75% initial Funding; Open 30-year cd; no asset smoothing</t>
   </si>
   <si>
@@ -790,9 +787,6 @@
     <t>75% initial Funding; Closed 30-year cp; no asset smoothing</t>
   </si>
   <si>
-    <t>100% initial Funding; Open 10-year cd; no asset smoothing</t>
-  </si>
-  <si>
     <t>100% initial Funding; Open 30-year cd; no asset smoothing</t>
   </si>
   <si>
@@ -818,6 +812,45 @@
   </si>
   <si>
     <t>75% initial Funding; No amort No Smoothing; no non-negative restriction</t>
+  </si>
+  <si>
+    <t>B2F100_2a</t>
+  </si>
+  <si>
+    <t>B2F100_3a</t>
+  </si>
+  <si>
+    <t>Comparable initial Funding; BRP: open 15-year cp; 5-year asset smoothing, DR 6.4%, ir 6.4%, sd 8%</t>
+  </si>
+  <si>
+    <t>Comparable initial Funding; BRP: open 30-year cp; 5-year asset smoothing, DR 6.4%, ir 7.5%, sd 12%</t>
+  </si>
+  <si>
+    <t>B2F075_2a</t>
+  </si>
+  <si>
+    <t>B2F075_3a</t>
+  </si>
+  <si>
+    <t>100% initial Funding; Open 15-year cd; no asset smoothing</t>
+  </si>
+  <si>
+    <t>75% initial Funding; Open 15-year cd; no asset smoothing</t>
+  </si>
+  <si>
+    <t>100% initial Funding; Open 15-year cp; no asset smoothing</t>
+  </si>
+  <si>
+    <t>A1F100_1cp</t>
+  </si>
+  <si>
+    <t>A1F100_2cp</t>
+  </si>
+  <si>
+    <t>A1F075_1cp</t>
+  </si>
+  <si>
+    <t>A1F075_2cp</t>
   </si>
 </sst>
 </file>
@@ -1002,13 +1035,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1017,10 +1044,16 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1124,13 +1157,13 @@
       <sheetName val="DropDowns"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1549,13 +1582,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AQ55"/>
+  <dimension ref="A1:AQ63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="B34" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="5" topLeftCell="B54" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="U1" sqref="U1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="C15" sqref="C15"/>
+      <selection pane="bottomRight" activeCell="C23" sqref="C23:C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1725,59 +1758,59 @@
       </c>
     </row>
     <row r="4" spans="1:43" s="8" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="29" t="s">
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="E4" s="29"/>
-      <c r="F4" s="30" t="s">
+      <c r="E4" s="33"/>
+      <c r="F4" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="G4" s="30"/>
-      <c r="H4" s="31" t="s">
+      <c r="G4" s="34"/>
+      <c r="H4" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="I4" s="31"/>
-      <c r="J4" s="32" t="s">
+      <c r="I4" s="29"/>
+      <c r="J4" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="K4" s="32"/>
-      <c r="L4" s="31" t="s">
+      <c r="K4" s="30"/>
+      <c r="L4" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="M4" s="31"/>
-      <c r="N4" s="31"/>
-      <c r="O4" s="31"/>
-      <c r="P4" s="31"/>
-      <c r="Q4" s="31"/>
-      <c r="R4" s="31"/>
-      <c r="S4" s="32" t="s">
+      <c r="M4" s="29"/>
+      <c r="N4" s="29"/>
+      <c r="O4" s="29"/>
+      <c r="P4" s="29"/>
+      <c r="Q4" s="29"/>
+      <c r="R4" s="29"/>
+      <c r="S4" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="T4" s="32"/>
-      <c r="U4" s="32"/>
-      <c r="V4" s="33" t="s">
-        <v>65</v>
-      </c>
-      <c r="W4" s="33"/>
-      <c r="X4" s="33"/>
+      <c r="T4" s="30"/>
+      <c r="U4" s="30"/>
+      <c r="V4" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="W4" s="28"/>
+      <c r="X4" s="28"/>
       <c r="Y4" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="Z4" s="28" t="s">
+      <c r="Z4" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="AA4" s="28"/>
-      <c r="AB4" s="28"/>
-      <c r="AC4" s="33" t="s">
+      <c r="AA4" s="31"/>
+      <c r="AB4" s="31"/>
+      <c r="AC4" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="AD4" s="33"/>
-      <c r="AE4" s="33"/>
+      <c r="AD4" s="28"/>
+      <c r="AE4" s="28"/>
       <c r="AF4" s="24" t="s">
         <v>70</v>
       </c>
@@ -1785,12 +1818,12 @@
       <c r="AH4" s="24"/>
       <c r="AI4" s="24"/>
       <c r="AJ4" s="24"/>
-      <c r="AK4" s="34" t="s">
+      <c r="AK4" s="32" t="s">
         <v>68</v>
       </c>
-      <c r="AL4" s="34"/>
-      <c r="AM4" s="34"/>
-      <c r="AN4" s="34"/>
+      <c r="AL4" s="32"/>
+      <c r="AM4" s="32"/>
+      <c r="AN4" s="32"/>
       <c r="AO4" s="17"/>
       <c r="AP4" s="26"/>
       <c r="AQ4" s="23"/>
@@ -1931,7 +1964,7 @@
         <v>180</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C6" s="11" t="b">
         <v>0</v>
@@ -2062,7 +2095,7 @@
         <v>181</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C7" s="11" t="b">
         <v>0</v>
@@ -2193,7 +2226,7 @@
         <v>182</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>252</v>
+        <v>266</v>
       </c>
       <c r="C8" s="11" t="b">
         <v>0</v>
@@ -2324,7 +2357,7 @@
         <v>183</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C9" s="11" t="b">
         <v>0</v>
@@ -2455,7 +2488,7 @@
         <v>184</v>
       </c>
       <c r="B10" s="22" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C10" s="11" t="b">
         <v>0</v>
@@ -2586,7 +2619,7 @@
         <v>185</v>
       </c>
       <c r="B11" s="22" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C11" s="11" t="b">
         <v>0</v>
@@ -2717,7 +2750,7 @@
         <v>186</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C12" s="11" t="b">
         <v>0</v>
@@ -2848,7 +2881,7 @@
         <v>187</v>
       </c>
       <c r="B13" s="22" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C13" s="11" t="b">
         <v>0</v>
@@ -3761,23 +3794,142 @@
       </c>
     </row>
     <row r="20" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="B20" s="22"/>
+      <c r="A20" t="s">
+        <v>269</v>
+      </c>
+      <c r="B20" s="22" t="s">
+        <v>268</v>
+      </c>
       <c r="C20" s="11" t="b">
         <v>0</v>
       </c>
-      <c r="L20" s="27"/>
-      <c r="AC20" s="2"/>
-      <c r="AD20" s="19"/>
-      <c r="AN20" s="25"/>
-      <c r="AP20" s="21"/>
-      <c r="AQ20" s="21"/>
+      <c r="D20" t="s">
+        <v>109</v>
+      </c>
+      <c r="E20" t="s">
+        <v>109</v>
+      </c>
+      <c r="F20" t="s">
+        <v>109</v>
+      </c>
+      <c r="G20" t="s">
+        <v>109</v>
+      </c>
+      <c r="H20" t="s">
+        <v>149</v>
+      </c>
+      <c r="I20" t="s">
+        <v>171</v>
+      </c>
+      <c r="J20" s="12">
+        <v>0</v>
+      </c>
+      <c r="K20" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="L20" s="12">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="M20">
+        <v>3</v>
+      </c>
+      <c r="N20">
+        <v>65</v>
+      </c>
+      <c r="O20">
+        <v>65</v>
+      </c>
+      <c r="P20" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="Q20">
+        <v>10</v>
+      </c>
+      <c r="R20">
+        <v>10</v>
+      </c>
+      <c r="S20" s="12">
+        <v>0.03</v>
+      </c>
+      <c r="T20" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="U20" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="V20" t="s">
+        <v>158</v>
+      </c>
+      <c r="W20" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="X20" s="12">
+        <v>0.12</v>
+      </c>
+      <c r="Y20" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z20" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="AA20" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="AB20">
+        <v>15</v>
+      </c>
+      <c r="AC20" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="AD20" s="19">
+        <v>1</v>
+      </c>
+      <c r="AE20">
+        <v>200</v>
+      </c>
+      <c r="AF20" t="s">
+        <v>144</v>
+      </c>
+      <c r="AG20">
+        <v>5</v>
+      </c>
+      <c r="AH20">
+        <v>200</v>
+      </c>
+      <c r="AI20" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="AJ20">
+        <v>1</v>
+      </c>
+      <c r="AK20" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="AL20" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="AM20" s="14">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AN20" s="14">
+        <v>0.05</v>
+      </c>
+      <c r="AO20" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP20" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="AQ20" s="21" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="21" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>194</v>
+        <v>270</v>
       </c>
       <c r="B21" s="22" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="C21" s="11" t="b">
         <v>0</v>
@@ -3852,16 +4004,16 @@
         <v>160</v>
       </c>
       <c r="AA21" s="2" t="s">
-        <v>114</v>
+        <v>161</v>
       </c>
       <c r="AB21">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="AC21" s="2" t="s">
         <v>169</v>
       </c>
       <c r="AD21" s="19">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="AE21">
         <v>200</v>
@@ -3897,149 +4049,28 @@
         <v>0</v>
       </c>
       <c r="AP21" s="21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ21" s="21" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>195</v>
-      </c>
-      <c r="B22" s="22" t="s">
-        <v>260</v>
-      </c>
-      <c r="C22" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="D22" t="s">
-        <v>109</v>
-      </c>
-      <c r="E22" t="s">
-        <v>109</v>
-      </c>
-      <c r="F22" t="s">
-        <v>109</v>
-      </c>
-      <c r="G22" t="s">
-        <v>109</v>
-      </c>
-      <c r="H22" t="s">
-        <v>149</v>
-      </c>
-      <c r="I22" t="s">
-        <v>171</v>
-      </c>
-      <c r="J22" s="12">
-        <v>0</v>
-      </c>
-      <c r="K22" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="L22" s="12">
-        <v>1.7999999999999999E-2</v>
-      </c>
-      <c r="M22">
-        <v>3</v>
-      </c>
-      <c r="N22">
-        <v>65</v>
-      </c>
-      <c r="O22">
-        <v>65</v>
-      </c>
-      <c r="P22" s="12">
-        <v>0.01</v>
-      </c>
-      <c r="Q22">
-        <v>10</v>
-      </c>
-      <c r="R22">
-        <v>10</v>
-      </c>
-      <c r="S22" s="12">
-        <v>0.03</v>
-      </c>
-      <c r="T22" s="12">
-        <v>0.01</v>
-      </c>
-      <c r="U22" s="12">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="V22" s="12" t="s">
-        <v>158</v>
-      </c>
-      <c r="W22" s="12">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="X22" s="12">
-        <v>0.12</v>
-      </c>
-      <c r="Y22" t="s">
-        <v>112</v>
-      </c>
-      <c r="Z22" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="AA22" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="AB22">
-        <v>1</v>
-      </c>
-      <c r="AC22" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="AD22" s="19">
-        <v>0.75</v>
-      </c>
-      <c r="AE22">
-        <v>200</v>
-      </c>
-      <c r="AF22" t="s">
-        <v>144</v>
-      </c>
-      <c r="AG22">
-        <v>5</v>
-      </c>
-      <c r="AH22">
-        <v>200</v>
-      </c>
-      <c r="AI22" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="AJ22">
-        <v>1</v>
-      </c>
-      <c r="AK22" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="AL22" s="14">
-        <v>0.25</v>
-      </c>
-      <c r="AM22" s="14">
-        <v>0.14499999999999999</v>
-      </c>
-      <c r="AN22" s="14">
-        <v>0.05</v>
-      </c>
-      <c r="AO22" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="AP22" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="AQ22" s="21" t="b">
-        <v>0</v>
-      </c>
+      <c r="B22" s="22"/>
+      <c r="C22" s="11"/>
+      <c r="L22" s="27"/>
+      <c r="AC22" s="2"/>
+      <c r="AD22" s="19"/>
+      <c r="AN22" s="25"/>
+      <c r="AP22" s="21"/>
+      <c r="AQ22" s="21"/>
     </row>
     <row r="23" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B23" s="22" t="s">
-        <v>246</v>
+        <v>259</v>
       </c>
       <c r="C23" s="11" t="b">
         <v>0</v>
@@ -4098,7 +4129,7 @@
       <c r="U23" s="12">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="V23" t="s">
+      <c r="V23" s="12" t="s">
         <v>158</v>
       </c>
       <c r="W23" s="12">
@@ -4117,7 +4148,7 @@
         <v>114</v>
       </c>
       <c r="AB23">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="AC23" s="2" t="s">
         <v>169</v>
@@ -4159,7 +4190,7 @@
         <v>0</v>
       </c>
       <c r="AP23" s="21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AQ23" s="21" t="b">
         <v>0</v>
@@ -4167,10 +4198,10 @@
     </row>
     <row r="24" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B24" s="22" t="s">
-        <v>247</v>
+        <v>258</v>
       </c>
       <c r="C24" s="11" t="b">
         <v>0</v>
@@ -4248,7 +4279,7 @@
         <v>114</v>
       </c>
       <c r="AB24">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="AC24" s="2" t="s">
         <v>169</v>
@@ -4298,10 +4329,10 @@
     </row>
     <row r="25" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B25" s="22" t="s">
-        <v>248</v>
+        <v>267</v>
       </c>
       <c r="C25" s="11" t="b">
         <v>0</v>
@@ -4360,7 +4391,7 @@
       <c r="U25" s="12">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="V25" s="12" t="s">
+      <c r="V25" t="s">
         <v>158</v>
       </c>
       <c r="W25" s="12">
@@ -4376,10 +4407,10 @@
         <v>160</v>
       </c>
       <c r="AA25" s="2" t="s">
-        <v>161</v>
+        <v>114</v>
       </c>
       <c r="AB25">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="AC25" s="2" t="s">
         <v>169</v>
@@ -4429,10 +4460,10 @@
     </row>
     <row r="26" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B26" s="22" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C26" s="11" t="b">
         <v>0</v>
@@ -4491,7 +4522,7 @@
       <c r="U26" s="12">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="V26" t="s">
+      <c r="V26" s="12" t="s">
         <v>158</v>
       </c>
       <c r="W26" s="12">
@@ -4504,13 +4535,13 @@
         <v>112</v>
       </c>
       <c r="Z26" s="2" t="s">
-        <v>113</v>
+        <v>160</v>
       </c>
       <c r="AA26" s="2" t="s">
         <v>114</v>
       </c>
       <c r="AB26">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="AC26" s="2" t="s">
         <v>169</v>
@@ -4560,10 +4591,10 @@
     </row>
     <row r="27" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B27" s="22" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="C27" s="11" t="b">
         <v>0</v>
@@ -4635,10 +4666,10 @@
         <v>112</v>
       </c>
       <c r="Z27" s="2" t="s">
-        <v>113</v>
+        <v>160</v>
       </c>
       <c r="AA27" s="2" t="s">
-        <v>114</v>
+        <v>161</v>
       </c>
       <c r="AB27">
         <v>30</v>
@@ -4691,10 +4722,10 @@
     </row>
     <row r="28" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B28" s="22" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="C28" s="11" t="b">
         <v>0</v>
@@ -4753,7 +4784,7 @@
       <c r="U28" s="12">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="V28" s="12" t="s">
+      <c r="V28" t="s">
         <v>158</v>
       </c>
       <c r="W28" s="12">
@@ -4769,10 +4800,10 @@
         <v>113</v>
       </c>
       <c r="AA28" s="2" t="s">
-        <v>161</v>
+        <v>114</v>
       </c>
       <c r="AB28">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="AC28" s="2" t="s">
         <v>169</v>
@@ -4822,10 +4853,10 @@
     </row>
     <row r="29" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B29" s="22" t="s">
-        <v>228</v>
+        <v>249</v>
       </c>
       <c r="C29" s="11" t="b">
         <v>0</v>
@@ -4897,13 +4928,13 @@
         <v>112</v>
       </c>
       <c r="Z29" s="2" t="s">
-        <v>160</v>
+        <v>113</v>
       </c>
       <c r="AA29" s="2" t="s">
         <v>114</v>
       </c>
       <c r="AB29">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="AC29" s="2" t="s">
         <v>169</v>
@@ -4915,7 +4946,7 @@
         <v>200</v>
       </c>
       <c r="AF29" t="s">
-        <v>117</v>
+        <v>144</v>
       </c>
       <c r="AG29">
         <v>5</v>
@@ -4953,10 +4984,10 @@
     </row>
     <row r="30" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B30" s="22" t="s">
-        <v>229</v>
+        <v>250</v>
       </c>
       <c r="C30" s="11" t="b">
         <v>0</v>
@@ -5028,13 +5059,13 @@
         <v>112</v>
       </c>
       <c r="Z30" s="2" t="s">
-        <v>160</v>
+        <v>113</v>
       </c>
       <c r="AA30" s="2" t="s">
-        <v>114</v>
+        <v>161</v>
       </c>
       <c r="AB30">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="AC30" s="2" t="s">
         <v>169</v>
@@ -5046,10 +5077,10 @@
         <v>200</v>
       </c>
       <c r="AF30" t="s">
-        <v>117</v>
+        <v>144</v>
       </c>
       <c r="AG30">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="AH30">
         <v>200</v>
@@ -5084,10 +5115,10 @@
     </row>
     <row r="31" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B31" s="22" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C31" s="11" t="b">
         <v>0</v>
@@ -5162,10 +5193,10 @@
         <v>160</v>
       </c>
       <c r="AA31" s="2" t="s">
-        <v>161</v>
+        <v>114</v>
       </c>
       <c r="AB31">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="AC31" s="2" t="s">
         <v>169</v>
@@ -5215,10 +5246,10 @@
     </row>
     <row r="32" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B32" s="22" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C32" s="11" t="b">
         <v>0</v>
@@ -5293,10 +5324,10 @@
         <v>160</v>
       </c>
       <c r="AA32" s="2" t="s">
-        <v>161</v>
+        <v>114</v>
       </c>
       <c r="AB32">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="AC32" s="2" t="s">
         <v>169</v>
@@ -5346,13 +5377,13 @@
     </row>
     <row r="33" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B33" s="22" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C33" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D33" t="s">
         <v>109</v>
@@ -5409,7 +5440,7 @@
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="V33" s="12" t="s">
-        <v>177</v>
+        <v>158</v>
       </c>
       <c r="W33" s="12">
         <v>7.4999999999999997E-2</v>
@@ -5424,22 +5455,22 @@
         <v>160</v>
       </c>
       <c r="AA33" s="2" t="s">
-        <v>114</v>
+        <v>161</v>
       </c>
       <c r="AB33">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="AC33" s="2" t="s">
         <v>169</v>
       </c>
       <c r="AD33" s="19">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="AE33">
         <v>200</v>
       </c>
       <c r="AF33" t="s">
-        <v>144</v>
+        <v>117</v>
       </c>
       <c r="AG33">
         <v>5</v>
@@ -5477,13 +5508,13 @@
     </row>
     <row r="34" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B34" s="22" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C34" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D34" t="s">
         <v>109</v>
@@ -5540,7 +5571,7 @@
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="V34" s="12" t="s">
-        <v>177</v>
+        <v>158</v>
       </c>
       <c r="W34" s="12">
         <v>7.4999999999999997E-2</v>
@@ -5564,16 +5595,16 @@
         <v>169</v>
       </c>
       <c r="AD34" s="19">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="AE34">
         <v>200</v>
       </c>
       <c r="AF34" t="s">
-        <v>144</v>
+        <v>117</v>
       </c>
       <c r="AG34">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="AH34">
         <v>200</v>
@@ -5608,13 +5639,13 @@
     </row>
     <row r="35" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B35" s="22" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C35" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D35" t="s">
         <v>109</v>
@@ -5701,7 +5732,7 @@
         <v>200</v>
       </c>
       <c r="AF35" t="s">
-        <v>117</v>
+        <v>144</v>
       </c>
       <c r="AG35">
         <v>5</v>
@@ -5739,13 +5770,13 @@
     </row>
     <row r="36" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B36" s="22" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C36" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D36" t="s">
         <v>109</v>
@@ -5817,10 +5848,10 @@
         <v>160</v>
       </c>
       <c r="AA36" s="2" t="s">
-        <v>114</v>
+        <v>161</v>
       </c>
       <c r="AB36">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="AC36" s="2" t="s">
         <v>169</v>
@@ -5832,10 +5863,10 @@
         <v>200</v>
       </c>
       <c r="AF36" t="s">
-        <v>117</v>
+        <v>144</v>
       </c>
       <c r="AG36">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="AH36">
         <v>200</v>
@@ -5870,13 +5901,13 @@
     </row>
     <row r="37" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B37" s="22" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C37" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D37" t="s">
         <v>109</v>
@@ -5948,10 +5979,10 @@
         <v>160</v>
       </c>
       <c r="AA37" s="2" t="s">
-        <v>161</v>
+        <v>114</v>
       </c>
       <c r="AB37">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="AC37" s="2" t="s">
         <v>169</v>
@@ -6001,13 +6032,13 @@
     </row>
     <row r="38" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B38" s="22" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C38" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D38" t="s">
         <v>109</v>
@@ -6079,10 +6110,10 @@
         <v>160</v>
       </c>
       <c r="AA38" s="2" t="s">
-        <v>161</v>
+        <v>114</v>
       </c>
       <c r="AB38">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="AC38" s="2" t="s">
         <v>169</v>
@@ -6131,66 +6162,276 @@
       </c>
     </row>
     <row r="39" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="B39" s="22"/>
-      <c r="C39" s="11"/>
-      <c r="J39" s="12"/>
-      <c r="K39" s="21"/>
-      <c r="L39" s="12"/>
-      <c r="P39" s="12"/>
-      <c r="S39" s="12"/>
-      <c r="T39" s="12"/>
-      <c r="U39" s="12"/>
-      <c r="V39" s="12"/>
-      <c r="W39" s="12"/>
-      <c r="X39" s="12"/>
-      <c r="Z39" s="2"/>
-      <c r="AA39" s="2"/>
-      <c r="AC39" s="2"/>
-      <c r="AD39" s="19"/>
-      <c r="AI39" s="2"/>
-      <c r="AK39" s="2"/>
-      <c r="AL39" s="14"/>
-      <c r="AM39" s="14"/>
-      <c r="AN39" s="14"/>
-      <c r="AO39" s="21"/>
-      <c r="AP39" s="21"/>
-      <c r="AQ39" s="21"/>
+      <c r="A39" t="s">
+        <v>210</v>
+      </c>
+      <c r="B39" s="22" t="s">
+        <v>236</v>
+      </c>
+      <c r="C39" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D39" t="s">
+        <v>109</v>
+      </c>
+      <c r="E39" t="s">
+        <v>109</v>
+      </c>
+      <c r="F39" t="s">
+        <v>109</v>
+      </c>
+      <c r="G39" t="s">
+        <v>109</v>
+      </c>
+      <c r="H39" t="s">
+        <v>149</v>
+      </c>
+      <c r="I39" t="s">
+        <v>171</v>
+      </c>
+      <c r="J39" s="12">
+        <v>0</v>
+      </c>
+      <c r="K39" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="L39" s="12">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="M39">
+        <v>3</v>
+      </c>
+      <c r="N39">
+        <v>65</v>
+      </c>
+      <c r="O39">
+        <v>65</v>
+      </c>
+      <c r="P39" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="Q39">
+        <v>10</v>
+      </c>
+      <c r="R39">
+        <v>10</v>
+      </c>
+      <c r="S39" s="12">
+        <v>0.03</v>
+      </c>
+      <c r="T39" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="U39" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="V39" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="W39" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="X39" s="12">
+        <v>0.12</v>
+      </c>
+      <c r="Y39" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z39" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="AA39" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="AB39">
+        <v>30</v>
+      </c>
+      <c r="AC39" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="AD39" s="19">
+        <v>1</v>
+      </c>
+      <c r="AE39">
+        <v>200</v>
+      </c>
+      <c r="AF39" t="s">
+        <v>117</v>
+      </c>
+      <c r="AG39">
+        <v>5</v>
+      </c>
+      <c r="AH39">
+        <v>200</v>
+      </c>
+      <c r="AI39" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="AJ39">
+        <v>1</v>
+      </c>
+      <c r="AK39" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="AL39" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="AM39" s="14">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AN39" s="14">
+        <v>0.05</v>
+      </c>
+      <c r="AO39" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP39" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="AQ39" s="21" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="40" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="B40" s="22"/>
-      <c r="C40" s="11"/>
-      <c r="J40" s="12"/>
-      <c r="K40" s="21"/>
-      <c r="L40" s="12"/>
-      <c r="P40" s="12"/>
-      <c r="S40" s="12"/>
-      <c r="T40" s="12"/>
-      <c r="U40" s="12"/>
-      <c r="V40" s="12"/>
-      <c r="W40" s="12"/>
-      <c r="X40" s="12"/>
-      <c r="Z40" s="2"/>
-      <c r="AA40" s="2"/>
-      <c r="AC40" s="2"/>
-      <c r="AD40" s="19"/>
-      <c r="AI40" s="2"/>
-      <c r="AK40" s="2"/>
-      <c r="AL40" s="14"/>
-      <c r="AM40" s="14"/>
-      <c r="AN40" s="14"/>
-      <c r="AO40" s="21"/>
-      <c r="AP40" s="21"/>
-      <c r="AQ40" s="21"/>
-    </row>
-    <row r="41" spans="1:43" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>211</v>
+      </c>
+      <c r="B40" s="22" t="s">
+        <v>237</v>
+      </c>
+      <c r="C40" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D40" t="s">
+        <v>109</v>
+      </c>
+      <c r="E40" t="s">
+        <v>109</v>
+      </c>
+      <c r="F40" t="s">
+        <v>109</v>
+      </c>
+      <c r="G40" t="s">
+        <v>109</v>
+      </c>
+      <c r="H40" t="s">
+        <v>149</v>
+      </c>
+      <c r="I40" t="s">
+        <v>171</v>
+      </c>
+      <c r="J40" s="12">
+        <v>0</v>
+      </c>
+      <c r="K40" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="L40" s="12">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="M40">
+        <v>3</v>
+      </c>
+      <c r="N40">
+        <v>65</v>
+      </c>
+      <c r="O40">
+        <v>65</v>
+      </c>
+      <c r="P40" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="Q40">
+        <v>10</v>
+      </c>
+      <c r="R40">
+        <v>10</v>
+      </c>
+      <c r="S40" s="12">
+        <v>0.03</v>
+      </c>
+      <c r="T40" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="U40" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="V40" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="W40" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="X40" s="12">
+        <v>0.12</v>
+      </c>
+      <c r="Y40" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z40" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="AA40" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="AB40">
+        <v>30</v>
+      </c>
+      <c r="AC40" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="AD40" s="19">
+        <v>1</v>
+      </c>
+      <c r="AE40">
+        <v>200</v>
+      </c>
+      <c r="AF40" t="s">
+        <v>117</v>
+      </c>
+      <c r="AG40">
+        <v>10</v>
+      </c>
+      <c r="AH40">
+        <v>200</v>
+      </c>
+      <c r="AI40" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="AJ40">
+        <v>1</v>
+      </c>
+      <c r="AK40" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="AL40" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="AM40" s="14">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AN40" s="14">
+        <v>0.05</v>
+      </c>
+      <c r="AO40" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP40" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="AQ40" s="21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>212</v>
+        <v>271</v>
       </c>
       <c r="B41" s="22" t="s">
-        <v>173</v>
+        <v>267</v>
       </c>
       <c r="C41" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D41" t="s">
         <v>109</v>
@@ -6246,7 +6487,7 @@
       <c r="U41" s="12">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="V41" s="12" t="s">
+      <c r="V41" t="s">
         <v>158</v>
       </c>
       <c r="W41" s="12">
@@ -6265,19 +6506,19 @@
         <v>161</v>
       </c>
       <c r="AB41">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="AC41" s="2" t="s">
         <v>169</v>
       </c>
       <c r="AD41" s="19">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="AE41">
         <v>200</v>
       </c>
       <c r="AF41" t="s">
-        <v>117</v>
+        <v>144</v>
       </c>
       <c r="AG41">
         <v>5</v>
@@ -6315,13 +6556,13 @@
     </row>
     <row r="42" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>213</v>
+        <v>272</v>
       </c>
       <c r="B42" s="22" t="s">
-        <v>174</v>
+        <v>246</v>
       </c>
       <c r="C42" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D42" t="s">
         <v>109</v>
@@ -6381,7 +6622,7 @@
         <v>158</v>
       </c>
       <c r="W42" s="12">
-        <v>8.2199999999999995E-2</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="X42" s="12">
         <v>0.12</v>
@@ -6402,13 +6643,13 @@
         <v>169</v>
       </c>
       <c r="AD42" s="19">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="AE42">
         <v>200</v>
       </c>
       <c r="AF42" t="s">
-        <v>117</v>
+        <v>144</v>
       </c>
       <c r="AG42">
         <v>5</v>
@@ -6470,146 +6711,41 @@
       <c r="AP43" s="21"/>
       <c r="AQ43" s="21"/>
     </row>
-    <row r="44" spans="1:43" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>214</v>
-      </c>
-      <c r="B44" s="22" t="s">
-        <v>238</v>
-      </c>
-      <c r="C44" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="D44" t="s">
-        <v>109</v>
-      </c>
-      <c r="E44" t="s">
-        <v>109</v>
-      </c>
-      <c r="F44" t="s">
-        <v>109</v>
-      </c>
-      <c r="G44" t="s">
-        <v>109</v>
-      </c>
-      <c r="H44" t="s">
-        <v>149</v>
-      </c>
-      <c r="I44" t="s">
-        <v>171</v>
-      </c>
-      <c r="J44" s="12">
-        <v>0</v>
-      </c>
-      <c r="K44" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="L44" s="12">
-        <v>1.7999999999999999E-2</v>
-      </c>
-      <c r="M44">
-        <v>3</v>
-      </c>
-      <c r="N44">
-        <v>65</v>
-      </c>
-      <c r="O44">
-        <v>65</v>
-      </c>
-      <c r="P44" s="12">
-        <v>0.01</v>
-      </c>
-      <c r="Q44">
-        <v>10</v>
-      </c>
-      <c r="R44">
-        <v>10</v>
-      </c>
-      <c r="S44" s="12">
-        <v>0.03</v>
-      </c>
-      <c r="T44" s="12">
-        <v>0.01</v>
-      </c>
-      <c r="U44" s="12">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="V44" s="12" t="s">
-        <v>158</v>
-      </c>
-      <c r="W44" s="12">
-        <v>6.4000000000000001E-2</v>
-      </c>
-      <c r="X44" s="12">
-        <v>0.08</v>
-      </c>
-      <c r="Y44" t="s">
-        <v>112</v>
-      </c>
-      <c r="Z44" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="AA44" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="AB44">
-        <v>30</v>
-      </c>
-      <c r="AC44" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="AD44" s="19">
-        <v>1</v>
-      </c>
-      <c r="AE44">
-        <v>200</v>
-      </c>
-      <c r="AF44" t="s">
-        <v>117</v>
-      </c>
-      <c r="AG44">
-        <v>5</v>
-      </c>
-      <c r="AH44">
-        <v>200</v>
-      </c>
-      <c r="AI44" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="AJ44">
-        <v>1</v>
-      </c>
-      <c r="AK44" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="AL44" s="14">
-        <v>0.25</v>
-      </c>
-      <c r="AM44" s="14">
-        <v>0.14499999999999999</v>
-      </c>
-      <c r="AN44" s="14">
-        <v>0.05</v>
-      </c>
-      <c r="AO44" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="AP44" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="AQ44" s="21" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="B44" s="22"/>
+      <c r="C44" s="11"/>
+      <c r="J44" s="12"/>
+      <c r="K44" s="21"/>
+      <c r="L44" s="12"/>
+      <c r="P44" s="12"/>
+      <c r="S44" s="12"/>
+      <c r="T44" s="12"/>
+      <c r="U44" s="12"/>
+      <c r="V44" s="12"/>
+      <c r="W44" s="12"/>
+      <c r="X44" s="12"/>
+      <c r="Z44" s="2"/>
+      <c r="AA44" s="2"/>
+      <c r="AC44" s="2"/>
+      <c r="AD44" s="19"/>
+      <c r="AI44" s="2"/>
+      <c r="AK44" s="2"/>
+      <c r="AL44" s="14"/>
+      <c r="AM44" s="14"/>
+      <c r="AN44" s="14"/>
+      <c r="AO44" s="21"/>
+      <c r="AP44" s="21"/>
+      <c r="AQ44" s="21"/>
+    </row>
+    <row r="45" spans="1:43" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B45" s="22" t="s">
-        <v>239</v>
+        <v>173</v>
       </c>
       <c r="C45" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D45" t="s">
         <v>109</v>
@@ -6669,10 +6805,10 @@
         <v>158</v>
       </c>
       <c r="W45" s="12">
-        <v>6.4000000000000001E-2</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="X45" s="12">
-        <v>0.08</v>
+        <v>0.12</v>
       </c>
       <c r="Y45" t="s">
         <v>112</v>
@@ -6684,7 +6820,7 @@
         <v>161</v>
       </c>
       <c r="AB45">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="AC45" s="2" t="s">
         <v>169</v>
@@ -6734,13 +6870,13 @@
     </row>
     <row r="46" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B46" s="22" t="s">
-        <v>240</v>
+        <v>174</v>
       </c>
       <c r="C46" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D46" t="s">
         <v>109</v>
@@ -6794,16 +6930,16 @@
         <v>0.01</v>
       </c>
       <c r="U46" s="12">
-        <v>6.4000000000000001E-2</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="V46" s="12" t="s">
         <v>158</v>
       </c>
       <c r="W46" s="12">
-        <v>6.4000000000000001E-2</v>
+        <v>8.2199999999999995E-2</v>
       </c>
       <c r="X46" s="12">
-        <v>0.08</v>
+        <v>0.12</v>
       </c>
       <c r="Y46" t="s">
         <v>112</v>
@@ -6815,7 +6951,7 @@
         <v>161</v>
       </c>
       <c r="AB46">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="AC46" s="2" t="s">
         <v>169</v>
@@ -6864,148 +7000,171 @@
       </c>
     </row>
     <row r="47" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>217</v>
-      </c>
-      <c r="B47" s="22" t="s">
-        <v>241</v>
-      </c>
-      <c r="C47" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="D47" t="s">
-        <v>109</v>
-      </c>
-      <c r="E47" t="s">
-        <v>109</v>
-      </c>
-      <c r="F47" t="s">
-        <v>109</v>
-      </c>
-      <c r="G47" t="s">
-        <v>109</v>
-      </c>
-      <c r="H47" t="s">
+      <c r="B47" s="22"/>
+      <c r="C47" s="11"/>
+      <c r="J47" s="12"/>
+      <c r="K47" s="21"/>
+      <c r="L47" s="12"/>
+      <c r="P47" s="12"/>
+      <c r="S47" s="12"/>
+      <c r="T47" s="12"/>
+      <c r="U47" s="12"/>
+      <c r="V47" s="12"/>
+      <c r="W47" s="12"/>
+      <c r="X47" s="12"/>
+      <c r="Z47" s="2"/>
+      <c r="AA47" s="2"/>
+      <c r="AC47" s="2"/>
+      <c r="AD47" s="19"/>
+      <c r="AI47" s="2"/>
+      <c r="AK47" s="2"/>
+      <c r="AL47" s="14"/>
+      <c r="AM47" s="14"/>
+      <c r="AN47" s="14"/>
+      <c r="AO47" s="21"/>
+      <c r="AP47" s="21"/>
+      <c r="AQ47" s="21"/>
+    </row>
+    <row r="48" spans="1:43" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>214</v>
+      </c>
+      <c r="B48" s="22" t="s">
+        <v>238</v>
+      </c>
+      <c r="C48" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D48" t="s">
+        <v>109</v>
+      </c>
+      <c r="E48" t="s">
+        <v>109</v>
+      </c>
+      <c r="F48" t="s">
+        <v>109</v>
+      </c>
+      <c r="G48" t="s">
+        <v>109</v>
+      </c>
+      <c r="H48" t="s">
         <v>149</v>
       </c>
-      <c r="I47" t="s">
+      <c r="I48" t="s">
         <v>171</v>
       </c>
-      <c r="J47" s="12">
-        <v>0</v>
-      </c>
-      <c r="K47" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="L47" s="12">
+      <c r="J48" s="12">
+        <v>0</v>
+      </c>
+      <c r="K48" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="L48" s="12">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="M47">
+      <c r="M48">
         <v>3</v>
       </c>
-      <c r="N47">
-        <v>65</v>
-      </c>
-      <c r="O47">
-        <v>65</v>
-      </c>
-      <c r="P47" s="12">
-        <v>0.01</v>
-      </c>
-      <c r="Q47">
-        <v>10</v>
-      </c>
-      <c r="R47">
-        <v>10</v>
-      </c>
-      <c r="S47" s="12">
+      <c r="N48">
+        <v>65</v>
+      </c>
+      <c r="O48">
+        <v>65</v>
+      </c>
+      <c r="P48" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="Q48">
+        <v>10</v>
+      </c>
+      <c r="R48">
+        <v>10</v>
+      </c>
+      <c r="S48" s="12">
         <v>0.03</v>
       </c>
-      <c r="T47" s="12">
-        <v>0.01</v>
-      </c>
-      <c r="U47" s="12">
+      <c r="T48" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="U48" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="V48" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="W48" s="12">
         <v>6.4000000000000001E-2</v>
       </c>
-      <c r="V47" s="12" t="s">
-        <v>158</v>
-      </c>
-      <c r="W47" s="12">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="X47" s="12">
-        <v>0.12</v>
-      </c>
-      <c r="Y47" t="s">
+      <c r="X48" s="12">
+        <v>0.08</v>
+      </c>
+      <c r="Y48" t="s">
         <v>112</v>
       </c>
-      <c r="Z47" s="2" t="s">
+      <c r="Z48" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="AA47" s="2" t="s">
+      <c r="AA48" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="AB47">
-        <v>15</v>
-      </c>
-      <c r="AC47" s="2" t="s">
+      <c r="AB48">
+        <v>30</v>
+      </c>
+      <c r="AC48" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="AD47" s="19">
-        <v>1</v>
-      </c>
-      <c r="AE47">
-        <v>200</v>
-      </c>
-      <c r="AF47" t="s">
+      <c r="AD48" s="19">
+        <v>1</v>
+      </c>
+      <c r="AE48">
+        <v>200</v>
+      </c>
+      <c r="AF48" t="s">
         <v>117</v>
       </c>
-      <c r="AG47">
+      <c r="AG48">
         <v>5</v>
       </c>
-      <c r="AH47">
-        <v>200</v>
-      </c>
-      <c r="AI47" s="2" t="s">
+      <c r="AH48">
+        <v>200</v>
+      </c>
+      <c r="AI48" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="AJ47">
-        <v>1</v>
-      </c>
-      <c r="AK47" s="2" t="s">
+      <c r="AJ48">
+        <v>1</v>
+      </c>
+      <c r="AK48" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="AL47" s="14">
+      <c r="AL48" s="14">
         <v>0.25</v>
       </c>
-      <c r="AM47" s="14">
+      <c r="AM48" s="14">
         <v>0.14499999999999999</v>
       </c>
-      <c r="AN47" s="14">
+      <c r="AN48" s="14">
         <v>0.05</v>
       </c>
-      <c r="AO47" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="AP47" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="AQ47" s="21" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="C48" s="11"/>
-    </row>
-    <row r="49" spans="1:43" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AO48" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP48" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="AQ48" s="21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B49" s="22" t="s">
-        <v>175</v>
+        <v>239</v>
       </c>
       <c r="C49" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D49" t="s">
         <v>109</v>
@@ -7065,10 +7224,10 @@
         <v>158</v>
       </c>
       <c r="W49" s="12">
-        <v>7.4999999999999997E-2</v>
+        <v>6.4000000000000001E-2</v>
       </c>
       <c r="X49" s="12">
-        <v>0.12</v>
+        <v>0.08</v>
       </c>
       <c r="Y49" t="s">
         <v>112</v>
@@ -7080,13 +7239,13 @@
         <v>161</v>
       </c>
       <c r="AB49">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="AC49" s="2" t="s">
         <v>169</v>
       </c>
       <c r="AD49" s="19">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="AE49">
         <v>200</v>
@@ -7130,13 +7289,13 @@
     </row>
     <row r="50" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B50" s="22" t="s">
-        <v>176</v>
+        <v>240</v>
       </c>
       <c r="C50" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D50" t="s">
         <v>109</v>
@@ -7190,16 +7349,16 @@
         <v>0.01</v>
       </c>
       <c r="U50" s="12">
-        <v>7.4999999999999997E-2</v>
+        <v>6.4000000000000001E-2</v>
       </c>
       <c r="V50" s="12" t="s">
         <v>158</v>
       </c>
       <c r="W50" s="12">
-        <v>8.2199999999999995E-2</v>
+        <v>6.4000000000000001E-2</v>
       </c>
       <c r="X50" s="12">
-        <v>0.12</v>
+        <v>0.08</v>
       </c>
       <c r="Y50" t="s">
         <v>112</v>
@@ -7211,13 +7370,13 @@
         <v>161</v>
       </c>
       <c r="AB50">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="AC50" s="2" t="s">
         <v>169</v>
       </c>
       <c r="AD50" s="19">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="AE50">
         <v>200</v>
@@ -7260,40 +7419,145 @@
       </c>
     </row>
     <row r="51" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="B51" s="22"/>
-      <c r="C51" s="11"/>
-      <c r="J51" s="12"/>
-      <c r="K51" s="21"/>
-      <c r="L51" s="12"/>
-      <c r="P51" s="12"/>
-      <c r="S51" s="12"/>
-      <c r="T51" s="12"/>
-      <c r="U51" s="12"/>
-      <c r="V51" s="12"/>
-      <c r="W51" s="12"/>
-      <c r="X51" s="12"/>
-      <c r="Z51" s="2"/>
-      <c r="AA51" s="2"/>
-      <c r="AC51" s="2"/>
-      <c r="AD51" s="19"/>
-      <c r="AI51" s="2"/>
-      <c r="AK51" s="2"/>
-      <c r="AL51" s="14"/>
-      <c r="AM51" s="14"/>
-      <c r="AN51" s="14"/>
-      <c r="AO51" s="21"/>
-      <c r="AP51" s="21"/>
-      <c r="AQ51" s="21"/>
-    </row>
-    <row r="52" spans="1:43" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>217</v>
+      </c>
+      <c r="B51" s="22" t="s">
+        <v>241</v>
+      </c>
+      <c r="C51" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D51" t="s">
+        <v>109</v>
+      </c>
+      <c r="E51" t="s">
+        <v>109</v>
+      </c>
+      <c r="F51" t="s">
+        <v>109</v>
+      </c>
+      <c r="G51" t="s">
+        <v>109</v>
+      </c>
+      <c r="H51" t="s">
+        <v>149</v>
+      </c>
+      <c r="I51" t="s">
+        <v>171</v>
+      </c>
+      <c r="J51" s="12">
+        <v>0</v>
+      </c>
+      <c r="K51" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="L51" s="12">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="M51">
+        <v>3</v>
+      </c>
+      <c r="N51">
+        <v>65</v>
+      </c>
+      <c r="O51">
+        <v>65</v>
+      </c>
+      <c r="P51" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="Q51">
+        <v>10</v>
+      </c>
+      <c r="R51">
+        <v>10</v>
+      </c>
+      <c r="S51" s="12">
+        <v>0.03</v>
+      </c>
+      <c r="T51" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="U51" s="12">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="V51" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="W51" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="X51" s="12">
+        <v>0.12</v>
+      </c>
+      <c r="Y51" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z51" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="AA51" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="AB51">
+        <v>15</v>
+      </c>
+      <c r="AC51" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="AD51" s="19">
+        <v>1</v>
+      </c>
+      <c r="AE51">
+        <v>200</v>
+      </c>
+      <c r="AF51" t="s">
+        <v>117</v>
+      </c>
+      <c r="AG51">
+        <v>5</v>
+      </c>
+      <c r="AH51">
+        <v>200</v>
+      </c>
+      <c r="AI51" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="AJ51">
+        <v>1</v>
+      </c>
+      <c r="AK51" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="AL51" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="AM51" s="14">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AN51" s="14">
+        <v>0.05</v>
+      </c>
+      <c r="AO51" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP51" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="AQ51" s="21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>220</v>
+        <v>260</v>
       </c>
       <c r="B52" s="22" t="s">
-        <v>242</v>
+        <v>262</v>
       </c>
       <c r="C52" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D52" t="s">
         <v>109</v>
@@ -7347,7 +7611,7 @@
         <v>0.01</v>
       </c>
       <c r="U52" s="12">
-        <v>7.4999999999999997E-2</v>
+        <v>6.4000000000000001E-2</v>
       </c>
       <c r="V52" s="12" t="s">
         <v>158</v>
@@ -7368,16 +7632,16 @@
         <v>161</v>
       </c>
       <c r="AB52">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="AC52" s="2" t="s">
-        <v>169</v>
+        <v>116</v>
       </c>
       <c r="AD52" s="19">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="AE52">
-        <v>200</v>
+        <v>143423401</v>
       </c>
       <c r="AF52" t="s">
         <v>117</v>
@@ -7418,13 +7682,13 @@
     </row>
     <row r="53" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>221</v>
+        <v>261</v>
       </c>
       <c r="B53" s="22" t="s">
-        <v>243</v>
+        <v>263</v>
       </c>
       <c r="C53" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D53" t="s">
         <v>109</v>
@@ -7478,16 +7742,16 @@
         <v>0.01</v>
       </c>
       <c r="U53" s="12">
-        <v>7.4999999999999997E-2</v>
+        <v>6.4000000000000001E-2</v>
       </c>
       <c r="V53" s="12" t="s">
         <v>158</v>
       </c>
       <c r="W53" s="12">
-        <v>6.4000000000000001E-2</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="X53" s="12">
-        <v>0.08</v>
+        <v>0.12</v>
       </c>
       <c r="Y53" t="s">
         <v>112</v>
@@ -7502,13 +7766,13 @@
         <v>15</v>
       </c>
       <c r="AC53" s="2" t="s">
-        <v>169</v>
+        <v>116</v>
       </c>
       <c r="AD53" s="19">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="AE53">
-        <v>200</v>
+        <v>143423401</v>
       </c>
       <c r="AF53" t="s">
         <v>117</v>
@@ -7548,145 +7812,17 @@
       </c>
     </row>
     <row r="54" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
-        <v>222</v>
-      </c>
-      <c r="B54" s="22" t="s">
-        <v>244</v>
-      </c>
-      <c r="C54" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="D54" t="s">
-        <v>109</v>
-      </c>
-      <c r="E54" t="s">
-        <v>109</v>
-      </c>
-      <c r="F54" t="s">
-        <v>109</v>
-      </c>
-      <c r="G54" t="s">
-        <v>109</v>
-      </c>
-      <c r="H54" t="s">
-        <v>149</v>
-      </c>
-      <c r="I54" t="s">
-        <v>171</v>
-      </c>
-      <c r="J54" s="12">
-        <v>0</v>
-      </c>
-      <c r="K54" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="L54" s="12">
-        <v>1.7999999999999999E-2</v>
-      </c>
-      <c r="M54">
-        <v>3</v>
-      </c>
-      <c r="N54">
-        <v>65</v>
-      </c>
-      <c r="O54">
-        <v>65</v>
-      </c>
-      <c r="P54" s="12">
-        <v>0.01</v>
-      </c>
-      <c r="Q54">
-        <v>10</v>
-      </c>
-      <c r="R54">
-        <v>10</v>
-      </c>
-      <c r="S54" s="12">
-        <v>0.03</v>
-      </c>
-      <c r="T54" s="12">
-        <v>0.01</v>
-      </c>
-      <c r="U54" s="12">
-        <v>6.4000000000000001E-2</v>
-      </c>
-      <c r="V54" s="12" t="s">
-        <v>158</v>
-      </c>
-      <c r="W54" s="12">
-        <v>6.4000000000000001E-2</v>
-      </c>
-      <c r="X54" s="12">
-        <v>0.08</v>
-      </c>
-      <c r="Y54" t="s">
-        <v>112</v>
-      </c>
-      <c r="Z54" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="AA54" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="AB54">
-        <v>15</v>
-      </c>
-      <c r="AC54" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="AD54" s="19">
-        <v>0.75</v>
-      </c>
-      <c r="AE54">
-        <v>200</v>
-      </c>
-      <c r="AF54" t="s">
-        <v>117</v>
-      </c>
-      <c r="AG54">
-        <v>5</v>
-      </c>
-      <c r="AH54">
-        <v>200</v>
-      </c>
-      <c r="AI54" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="AJ54">
-        <v>1</v>
-      </c>
-      <c r="AK54" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="AL54" s="14">
-        <v>0.25</v>
-      </c>
-      <c r="AM54" s="14">
-        <v>0.14499999999999999</v>
-      </c>
-      <c r="AN54" s="14">
-        <v>0.05</v>
-      </c>
-      <c r="AO54" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="AP54" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="AQ54" s="21" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="C54" s="11"/>
+    </row>
+    <row r="55" spans="1:43" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="B55" s="22" t="s">
-        <v>245</v>
+        <v>175</v>
       </c>
       <c r="C55" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D55" t="s">
         <v>109</v>
@@ -7740,7 +7876,7 @@
         <v>0.01</v>
       </c>
       <c r="U55" s="12">
-        <v>6.4000000000000001E-2</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="V55" s="12" t="s">
         <v>158</v>
@@ -7761,7 +7897,7 @@
         <v>161</v>
       </c>
       <c r="AB55">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="AC55" s="2" t="s">
         <v>169</v>
@@ -7809,93 +7945,1036 @@
         <v>0</v>
       </c>
     </row>
+    <row r="56" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>219</v>
+      </c>
+      <c r="B56" s="22" t="s">
+        <v>176</v>
+      </c>
+      <c r="C56" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D56" t="s">
+        <v>109</v>
+      </c>
+      <c r="E56" t="s">
+        <v>109</v>
+      </c>
+      <c r="F56" t="s">
+        <v>109</v>
+      </c>
+      <c r="G56" t="s">
+        <v>109</v>
+      </c>
+      <c r="H56" t="s">
+        <v>149</v>
+      </c>
+      <c r="I56" t="s">
+        <v>171</v>
+      </c>
+      <c r="J56" s="12">
+        <v>0</v>
+      </c>
+      <c r="K56" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="L56" s="12">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="M56">
+        <v>3</v>
+      </c>
+      <c r="N56">
+        <v>65</v>
+      </c>
+      <c r="O56">
+        <v>65</v>
+      </c>
+      <c r="P56" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="Q56">
+        <v>10</v>
+      </c>
+      <c r="R56">
+        <v>10</v>
+      </c>
+      <c r="S56" s="12">
+        <v>0.03</v>
+      </c>
+      <c r="T56" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="U56" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="V56" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="W56" s="12">
+        <v>8.2199999999999995E-2</v>
+      </c>
+      <c r="X56" s="12">
+        <v>0.12</v>
+      </c>
+      <c r="Y56" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z56" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="AA56" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="AB56">
+        <v>30</v>
+      </c>
+      <c r="AC56" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="AD56" s="19">
+        <v>0.75</v>
+      </c>
+      <c r="AE56">
+        <v>200</v>
+      </c>
+      <c r="AF56" t="s">
+        <v>117</v>
+      </c>
+      <c r="AG56">
+        <v>5</v>
+      </c>
+      <c r="AH56">
+        <v>200</v>
+      </c>
+      <c r="AI56" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="AJ56">
+        <v>1</v>
+      </c>
+      <c r="AK56" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="AL56" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="AM56" s="14">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AN56" s="14">
+        <v>0.05</v>
+      </c>
+      <c r="AO56" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP56" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="AQ56" s="21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="B57" s="22"/>
+      <c r="C57" s="11"/>
+      <c r="J57" s="12"/>
+      <c r="K57" s="21"/>
+      <c r="L57" s="12"/>
+      <c r="P57" s="12"/>
+      <c r="S57" s="12"/>
+      <c r="T57" s="12"/>
+      <c r="U57" s="12"/>
+      <c r="V57" s="12"/>
+      <c r="W57" s="12"/>
+      <c r="X57" s="12"/>
+      <c r="Z57" s="2"/>
+      <c r="AA57" s="2"/>
+      <c r="AC57" s="2"/>
+      <c r="AD57" s="19"/>
+      <c r="AI57" s="2"/>
+      <c r="AK57" s="2"/>
+      <c r="AL57" s="14"/>
+      <c r="AM57" s="14"/>
+      <c r="AN57" s="14"/>
+      <c r="AO57" s="21"/>
+      <c r="AP57" s="21"/>
+      <c r="AQ57" s="21"/>
+    </row>
+    <row r="58" spans="1:43" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>220</v>
+      </c>
+      <c r="B58" s="22" t="s">
+        <v>242</v>
+      </c>
+      <c r="C58" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D58" t="s">
+        <v>109</v>
+      </c>
+      <c r="E58" t="s">
+        <v>109</v>
+      </c>
+      <c r="F58" t="s">
+        <v>109</v>
+      </c>
+      <c r="G58" t="s">
+        <v>109</v>
+      </c>
+      <c r="H58" t="s">
+        <v>149</v>
+      </c>
+      <c r="I58" t="s">
+        <v>171</v>
+      </c>
+      <c r="J58" s="12">
+        <v>0</v>
+      </c>
+      <c r="K58" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="L58" s="12">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="M58">
+        <v>3</v>
+      </c>
+      <c r="N58">
+        <v>65</v>
+      </c>
+      <c r="O58">
+        <v>65</v>
+      </c>
+      <c r="P58" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="Q58">
+        <v>10</v>
+      </c>
+      <c r="R58">
+        <v>10</v>
+      </c>
+      <c r="S58" s="12">
+        <v>0.03</v>
+      </c>
+      <c r="T58" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="U58" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="V58" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="W58" s="12">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="X58" s="12">
+        <v>0.08</v>
+      </c>
+      <c r="Y58" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z58" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="AA58" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="AB58">
+        <v>30</v>
+      </c>
+      <c r="AC58" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="AD58" s="19">
+        <v>0.75</v>
+      </c>
+      <c r="AE58">
+        <v>200</v>
+      </c>
+      <c r="AF58" t="s">
+        <v>117</v>
+      </c>
+      <c r="AG58">
+        <v>5</v>
+      </c>
+      <c r="AH58">
+        <v>200</v>
+      </c>
+      <c r="AI58" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="AJ58">
+        <v>1</v>
+      </c>
+      <c r="AK58" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="AL58" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="AM58" s="14">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AN58" s="14">
+        <v>0.05</v>
+      </c>
+      <c r="AO58" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP58" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="AQ58" s="21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>221</v>
+      </c>
+      <c r="B59" s="22" t="s">
+        <v>243</v>
+      </c>
+      <c r="C59" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D59" t="s">
+        <v>109</v>
+      </c>
+      <c r="E59" t="s">
+        <v>109</v>
+      </c>
+      <c r="F59" t="s">
+        <v>109</v>
+      </c>
+      <c r="G59" t="s">
+        <v>109</v>
+      </c>
+      <c r="H59" t="s">
+        <v>149</v>
+      </c>
+      <c r="I59" t="s">
+        <v>171</v>
+      </c>
+      <c r="J59" s="12">
+        <v>0</v>
+      </c>
+      <c r="K59" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="L59" s="12">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="M59">
+        <v>3</v>
+      </c>
+      <c r="N59">
+        <v>65</v>
+      </c>
+      <c r="O59">
+        <v>65</v>
+      </c>
+      <c r="P59" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="Q59">
+        <v>10</v>
+      </c>
+      <c r="R59">
+        <v>10</v>
+      </c>
+      <c r="S59" s="12">
+        <v>0.03</v>
+      </c>
+      <c r="T59" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="U59" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="V59" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="W59" s="12">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="X59" s="12">
+        <v>0.08</v>
+      </c>
+      <c r="Y59" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z59" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="AA59" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="AB59">
+        <v>15</v>
+      </c>
+      <c r="AC59" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="AD59" s="19">
+        <v>0.75</v>
+      </c>
+      <c r="AE59">
+        <v>200</v>
+      </c>
+      <c r="AF59" t="s">
+        <v>117</v>
+      </c>
+      <c r="AG59">
+        <v>5</v>
+      </c>
+      <c r="AH59">
+        <v>200</v>
+      </c>
+      <c r="AI59" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="AJ59">
+        <v>1</v>
+      </c>
+      <c r="AK59" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="AL59" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="AM59" s="14">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AN59" s="14">
+        <v>0.05</v>
+      </c>
+      <c r="AO59" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP59" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="AQ59" s="21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>222</v>
+      </c>
+      <c r="B60" s="22" t="s">
+        <v>244</v>
+      </c>
+      <c r="C60" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D60" t="s">
+        <v>109</v>
+      </c>
+      <c r="E60" t="s">
+        <v>109</v>
+      </c>
+      <c r="F60" t="s">
+        <v>109</v>
+      </c>
+      <c r="G60" t="s">
+        <v>109</v>
+      </c>
+      <c r="H60" t="s">
+        <v>149</v>
+      </c>
+      <c r="I60" t="s">
+        <v>171</v>
+      </c>
+      <c r="J60" s="12">
+        <v>0</v>
+      </c>
+      <c r="K60" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="L60" s="12">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="M60">
+        <v>3</v>
+      </c>
+      <c r="N60">
+        <v>65</v>
+      </c>
+      <c r="O60">
+        <v>65</v>
+      </c>
+      <c r="P60" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="Q60">
+        <v>10</v>
+      </c>
+      <c r="R60">
+        <v>10</v>
+      </c>
+      <c r="S60" s="12">
+        <v>0.03</v>
+      </c>
+      <c r="T60" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="U60" s="12">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="V60" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="W60" s="12">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="X60" s="12">
+        <v>0.08</v>
+      </c>
+      <c r="Y60" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z60" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="AA60" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="AB60">
+        <v>15</v>
+      </c>
+      <c r="AC60" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="AD60" s="19">
+        <v>0.75</v>
+      </c>
+      <c r="AE60">
+        <v>200</v>
+      </c>
+      <c r="AF60" t="s">
+        <v>117</v>
+      </c>
+      <c r="AG60">
+        <v>5</v>
+      </c>
+      <c r="AH60">
+        <v>200</v>
+      </c>
+      <c r="AI60" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="AJ60">
+        <v>1</v>
+      </c>
+      <c r="AK60" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="AL60" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="AM60" s="14">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AN60" s="14">
+        <v>0.05</v>
+      </c>
+      <c r="AO60" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP60" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="AQ60" s="21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>223</v>
+      </c>
+      <c r="B61" s="22" t="s">
+        <v>245</v>
+      </c>
+      <c r="C61" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D61" t="s">
+        <v>109</v>
+      </c>
+      <c r="E61" t="s">
+        <v>109</v>
+      </c>
+      <c r="F61" t="s">
+        <v>109</v>
+      </c>
+      <c r="G61" t="s">
+        <v>109</v>
+      </c>
+      <c r="H61" t="s">
+        <v>149</v>
+      </c>
+      <c r="I61" t="s">
+        <v>171</v>
+      </c>
+      <c r="J61" s="12">
+        <v>0</v>
+      </c>
+      <c r="K61" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="L61" s="12">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="M61">
+        <v>3</v>
+      </c>
+      <c r="N61">
+        <v>65</v>
+      </c>
+      <c r="O61">
+        <v>65</v>
+      </c>
+      <c r="P61" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="Q61">
+        <v>10</v>
+      </c>
+      <c r="R61">
+        <v>10</v>
+      </c>
+      <c r="S61" s="12">
+        <v>0.03</v>
+      </c>
+      <c r="T61" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="U61" s="12">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="V61" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="W61" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="X61" s="12">
+        <v>0.12</v>
+      </c>
+      <c r="Y61" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z61" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="AA61" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="AB61">
+        <v>15</v>
+      </c>
+      <c r="AC61" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="AD61" s="19">
+        <v>0.75</v>
+      </c>
+      <c r="AE61">
+        <v>200</v>
+      </c>
+      <c r="AF61" t="s">
+        <v>117</v>
+      </c>
+      <c r="AG61">
+        <v>5</v>
+      </c>
+      <c r="AH61">
+        <v>200</v>
+      </c>
+      <c r="AI61" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="AJ61">
+        <v>1</v>
+      </c>
+      <c r="AK61" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="AL61" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="AM61" s="14">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AN61" s="14">
+        <v>0.05</v>
+      </c>
+      <c r="AO61" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP61" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="AQ61" s="21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>264</v>
+      </c>
+      <c r="B62" s="22" t="s">
+        <v>262</v>
+      </c>
+      <c r="C62" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="D62" t="s">
+        <v>109</v>
+      </c>
+      <c r="E62" t="s">
+        <v>109</v>
+      </c>
+      <c r="F62" t="s">
+        <v>109</v>
+      </c>
+      <c r="G62" t="s">
+        <v>109</v>
+      </c>
+      <c r="H62" t="s">
+        <v>149</v>
+      </c>
+      <c r="I62" t="s">
+        <v>171</v>
+      </c>
+      <c r="J62" s="12">
+        <v>0</v>
+      </c>
+      <c r="K62" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="L62" s="12">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="M62">
+        <v>3</v>
+      </c>
+      <c r="N62">
+        <v>65</v>
+      </c>
+      <c r="O62">
+        <v>65</v>
+      </c>
+      <c r="P62" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="Q62">
+        <v>10</v>
+      </c>
+      <c r="R62">
+        <v>10</v>
+      </c>
+      <c r="S62" s="12">
+        <v>0.03</v>
+      </c>
+      <c r="T62" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="U62" s="12">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="V62" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="W62" s="12">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="X62" s="12">
+        <v>0.08</v>
+      </c>
+      <c r="Y62" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z62" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="AA62" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="AB62">
+        <v>15</v>
+      </c>
+      <c r="AC62" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="AD62" s="19">
+        <v>0.75</v>
+      </c>
+      <c r="AE62">
+        <v>107567551</v>
+      </c>
+      <c r="AF62" t="s">
+        <v>117</v>
+      </c>
+      <c r="AG62">
+        <v>5</v>
+      </c>
+      <c r="AH62">
+        <v>200</v>
+      </c>
+      <c r="AI62" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="AJ62">
+        <v>1</v>
+      </c>
+      <c r="AK62" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="AL62" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="AM62" s="14">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AN62" s="14">
+        <v>0.05</v>
+      </c>
+      <c r="AO62" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP62" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="AQ62" s="21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>265</v>
+      </c>
+      <c r="B63" s="22" t="s">
+        <v>263</v>
+      </c>
+      <c r="C63" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="D63" t="s">
+        <v>109</v>
+      </c>
+      <c r="E63" t="s">
+        <v>109</v>
+      </c>
+      <c r="F63" t="s">
+        <v>109</v>
+      </c>
+      <c r="G63" t="s">
+        <v>109</v>
+      </c>
+      <c r="H63" t="s">
+        <v>149</v>
+      </c>
+      <c r="I63" t="s">
+        <v>171</v>
+      </c>
+      <c r="J63" s="12">
+        <v>0</v>
+      </c>
+      <c r="K63" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="L63" s="12">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="M63">
+        <v>3</v>
+      </c>
+      <c r="N63">
+        <v>65</v>
+      </c>
+      <c r="O63">
+        <v>65</v>
+      </c>
+      <c r="P63" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="Q63">
+        <v>10</v>
+      </c>
+      <c r="R63">
+        <v>10</v>
+      </c>
+      <c r="S63" s="12">
+        <v>0.03</v>
+      </c>
+      <c r="T63" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="U63" s="12">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="V63" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="W63" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="X63" s="12">
+        <v>0.12</v>
+      </c>
+      <c r="Y63" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z63" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="AA63" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="AB63">
+        <v>15</v>
+      </c>
+      <c r="AC63" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="AD63" s="19">
+        <v>0.75</v>
+      </c>
+      <c r="AE63">
+        <v>107567551</v>
+      </c>
+      <c r="AF63" t="s">
+        <v>117</v>
+      </c>
+      <c r="AG63">
+        <v>5</v>
+      </c>
+      <c r="AH63">
+        <v>200</v>
+      </c>
+      <c r="AI63" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="AJ63">
+        <v>1</v>
+      </c>
+      <c r="AK63" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="AL63" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="AM63" s="14">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AN63" s="14">
+        <v>0.05</v>
+      </c>
+      <c r="AO63" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP63" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="AQ63" s="21" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="J4:K4"/>
     <mergeCell ref="AC4:AE4"/>
     <mergeCell ref="L4:R4"/>
     <mergeCell ref="S4:U4"/>
     <mergeCell ref="Z4:AB4"/>
     <mergeCell ref="AK4:AN4"/>
     <mergeCell ref="V4:X4"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="J4:K4"/>
   </mergeCells>
   <dataValidations count="20">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AI21:AI47 AI49:AI55 AI6:AI19">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AI6:AI21 AI55:AI63 AI23:AI53">
       <formula1>"MA,EAA"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA21:AA47 AA49:AA55 AA6:AA19">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA6:AA21 AA55:AA63 AA23:AA53">
       <formula1>"cd,cp,sl"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z21:Z47 Z49:Z55 Z6:Z19">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z6:Z21 Z55:Z63 Z23:Z53">
       <formula1>"open,closed"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AK21:AK47 AK49:AK55 AK6:AK19">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AK6:AK21 AK55:AK63 AK23:AK53">
       <formula1>ConPolicy</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K21:K47 K49:K55 K6:K19 C6:C55">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K55:K63 K6:K21 K23:K53 C6:C63">
       <formula1>"TRUE,FALSE"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer 55 to 65, please" sqref="N21:N47 N49:N55 N6:N19">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer 55 to 65, please" sqref="N6:N21 N55:N63 N23:N53">
       <formula1>55</formula1>
       <formula2>65</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-10% please" sqref="T6:T19 P21:P47 P49:P55 T49:T55 T21:T47 P6:P19">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-10% please" sqref="P6:P21 P55:P63 T55:T63 T6:T21 P23:P53 T23:T53">
       <formula1>0</formula1>
       <formula2>0.1</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 0-15" sqref="Q21:R47 Q49:R55 Q6:R19">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 0-15" sqref="Q6:R21 Q55:R63 Q23:R53">
       <formula1>0</formula1>
       <formula2>15</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="W6:W19 S6:S19 S21:S47 U49:U55 W49:W55 S49:S55 U21:U47 W21:W47 U6:U19">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="S6:S21 U6:U21 U55:U63 W55:W63 S55:S63 W6:W21 S23:S53 W23:W53 U23:U53">
       <formula1>0</formula1>
       <formula2>0.2</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 0 to 30, please" sqref="AB21:AB47 AB49:AB55 AB6:AB19">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 0 to 30, please" sqref="AB6:AB21 AB55:AB63 AB23:AB53">
       <formula1>0</formula1>
       <formula2>30</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-75%" sqref="AL21:AM47 AL49:AM55 AL6:AM19">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-75%" sqref="AL6:AM21 AL55:AM63 AL23:AM53">
       <formula1>0</formula1>
       <formula2>0.75</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-30%" sqref="AN21:AN47 AN49:AN55 AN6:AN19">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-30%" sqref="AN6:AN21 AN55:AN63 AN23:AN53">
       <formula1>0</formula1>
       <formula2>0.3</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-75% please" sqref="X21:X47 X49:X55 X6:X19">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-75% please" sqref="X6:X21 X55:X63 X23:X53">
       <formula1>0</formula1>
       <formula2>0.75</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 1 to 30" sqref="AG21:AG47 AG49:AG55 AG6:AG19">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 1 to 30" sqref="AG6:AG21 AG55:AG63 AG23:AG53">
       <formula1>1</formula1>
       <formula2>30</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AH21:AH47 AH49:AH55 AH6:AH19">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AH6:AH21 AH55:AH63 AH23:AH53">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AJ21:AJ47 AJ49:AJ55 AJ6:AJ19">
+    <dataValidation type="decimal" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AJ6:AJ21 AJ55:AJ63 AJ23:AJ53">
       <formula1>1</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="V21:V47 V49:V55 V6:V19"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AO49:AQ55 AO6:AQ47">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="V6:V21 V55:V63 V23:V53"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AO55:AQ63 AO6:AQ53">
       <formula1>"TRUE, FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AC49:AC55 AC6:AC47">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AC55:AC63 AC6:AC53">
       <formula1>"MA,AL,AL_pct"</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AD49:AD55 AD6:AD47">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AD55:AD63 AD6:AD53">
       <formula1>0</formula1>
       <formula2>1.5</formula2>
     </dataValidation>
@@ -7904,30 +8983,24 @@
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DropDowns!$A$37:$A$41</xm:f>
           </x14:formula1>
-          <xm:sqref>H49:H55 H6:H17 H20:H47</xm:sqref>
+          <xm:sqref>H55:H63 H6:H17 H20:H53</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DropDowns!$A$44:$A$46</xm:f>
           </x14:formula1>
-          <xm:sqref>I49:I55 I6:I17 I20:I47</xm:sqref>
+          <xm:sqref>I55:I63 I6:I17 I20:I53</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>[1]DropDowns!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>I18:I19</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>[1]DropDowns!#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>H18:H19</xm:sqref>
+          <xm:sqref>H18:I19</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
New runs for M1
</commit_message>
<xml_diff>
--- a/IO_M1/RunControl_M1.xlsx
+++ b/IO_M1/RunControl_M1.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1036" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1262" uniqueCount="290">
   <si>
     <t>Sheet #</t>
   </si>
@@ -851,6 +851,57 @@
   </si>
   <si>
     <t>A1F075_2cp</t>
+  </si>
+  <si>
+    <t>75% initial Funding; Open 30-year cp, 5-year smoothing; Deterministic return</t>
+  </si>
+  <si>
+    <t>C1F075_u</t>
+  </si>
+  <si>
+    <t>C1F075_0</t>
+  </si>
+  <si>
+    <t>C1F075_3</t>
+  </si>
+  <si>
+    <t>C1F075_1c</t>
+  </si>
+  <si>
+    <t>C1F075_2c</t>
+  </si>
+  <si>
+    <t>C1F075_3c</t>
+  </si>
+  <si>
+    <t>C1F075_6</t>
+  </si>
+  <si>
+    <t>C1F075_6d</t>
+  </si>
+  <si>
+    <t>C1F075_1</t>
+  </si>
+  <si>
+    <t>C1F075_4</t>
+  </si>
+  <si>
+    <t>C1F100_6</t>
+  </si>
+  <si>
+    <t>C1F075_6a</t>
+  </si>
+  <si>
+    <t>75% initial Funding; SOA smoothing: open 15-year cp; 5-year asset smoothing, DR 6.4%, ir 7.5%, sd 12%</t>
+  </si>
+  <si>
+    <t>75% initial Funding; SOA smoothing: open 15-year cp; 5-year asset smoothing, DR 7.5%, ir 7.5%, sd 12%</t>
+  </si>
+  <si>
+    <t>C1F075_soa1</t>
+  </si>
+  <si>
+    <t>C1F075_soa2</t>
   </si>
 </sst>
 </file>
@@ -1035,13 +1086,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1050,10 +1095,16 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1155,6 +1206,7 @@
       <sheetName val="Contributions"/>
       <sheetName val="GlobalParams"/>
       <sheetName val="DropDowns"/>
+      <sheetName val="Sheet1"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0"/>
@@ -1164,6 +1216,7 @@
       <sheetData sheetId="4"/>
       <sheetData sheetId="5"/>
       <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1582,19 +1635,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AQ63"/>
+  <dimension ref="A1:AQ81"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="5" topLeftCell="V62" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="U1" sqref="U1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="C23" sqref="C23:C25"/>
+      <selection pane="bottomRight" activeCell="X84" sqref="X84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.85546875" customWidth="1"/>
-    <col min="2" max="2" width="73.42578125" customWidth="1"/>
+    <col min="2" max="2" width="90.5703125" customWidth="1"/>
     <col min="3" max="3" width="18.85546875" customWidth="1"/>
     <col min="4" max="7" width="16" customWidth="1"/>
     <col min="8" max="8" width="24.42578125"/>
@@ -1758,59 +1811,59 @@
       </c>
     </row>
     <row r="4" spans="1:43" s="8" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="29" t="s">
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="E4" s="29"/>
-      <c r="F4" s="30" t="s">
+      <c r="E4" s="33"/>
+      <c r="F4" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="G4" s="30"/>
-      <c r="H4" s="31" t="s">
+      <c r="G4" s="34"/>
+      <c r="H4" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="I4" s="31"/>
-      <c r="J4" s="32" t="s">
+      <c r="I4" s="29"/>
+      <c r="J4" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="K4" s="32"/>
-      <c r="L4" s="31" t="s">
+      <c r="K4" s="30"/>
+      <c r="L4" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="M4" s="31"/>
-      <c r="N4" s="31"/>
-      <c r="O4" s="31"/>
-      <c r="P4" s="31"/>
-      <c r="Q4" s="31"/>
-      <c r="R4" s="31"/>
-      <c r="S4" s="32" t="s">
+      <c r="M4" s="29"/>
+      <c r="N4" s="29"/>
+      <c r="O4" s="29"/>
+      <c r="P4" s="29"/>
+      <c r="Q4" s="29"/>
+      <c r="R4" s="29"/>
+      <c r="S4" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="T4" s="32"/>
-      <c r="U4" s="32"/>
-      <c r="V4" s="33" t="s">
+      <c r="T4" s="30"/>
+      <c r="U4" s="30"/>
+      <c r="V4" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="W4" s="33"/>
-      <c r="X4" s="33"/>
+      <c r="W4" s="28"/>
+      <c r="X4" s="28"/>
       <c r="Y4" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="Z4" s="28" t="s">
+      <c r="Z4" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="AA4" s="28"/>
-      <c r="AB4" s="28"/>
-      <c r="AC4" s="33" t="s">
+      <c r="AA4" s="31"/>
+      <c r="AB4" s="31"/>
+      <c r="AC4" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="AD4" s="33"/>
-      <c r="AE4" s="33"/>
+      <c r="AD4" s="28"/>
+      <c r="AE4" s="28"/>
       <c r="AF4" s="24" t="s">
         <v>70</v>
       </c>
@@ -1818,12 +1871,12 @@
       <c r="AH4" s="24"/>
       <c r="AI4" s="24"/>
       <c r="AJ4" s="24"/>
-      <c r="AK4" s="34" t="s">
+      <c r="AK4" s="32" t="s">
         <v>68</v>
       </c>
-      <c r="AL4" s="34"/>
-      <c r="AM4" s="34"/>
-      <c r="AN4" s="34"/>
+      <c r="AL4" s="32"/>
+      <c r="AM4" s="32"/>
+      <c r="AN4" s="32"/>
       <c r="AO4" s="17"/>
       <c r="AP4" s="26"/>
       <c r="AQ4" s="23"/>
@@ -8634,7 +8687,7 @@
         <v>262</v>
       </c>
       <c r="C62" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D62" t="s">
         <v>109</v>
@@ -8765,7 +8818,7 @@
         <v>263</v>
       </c>
       <c r="C63" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D63" t="s">
         <v>109</v>
@@ -8888,93 +8941,1932 @@
         <v>0</v>
       </c>
     </row>
+    <row r="66" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>284</v>
+      </c>
+      <c r="B66" s="22" t="s">
+        <v>178</v>
+      </c>
+      <c r="C66" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D66" t="s">
+        <v>109</v>
+      </c>
+      <c r="E66" t="s">
+        <v>109</v>
+      </c>
+      <c r="F66" t="s">
+        <v>109</v>
+      </c>
+      <c r="G66" t="s">
+        <v>109</v>
+      </c>
+      <c r="H66" t="s">
+        <v>170</v>
+      </c>
+      <c r="I66" t="s">
+        <v>171</v>
+      </c>
+      <c r="J66" s="12">
+        <v>0</v>
+      </c>
+      <c r="K66" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="L66" s="12">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="M66">
+        <v>3</v>
+      </c>
+      <c r="N66">
+        <v>60</v>
+      </c>
+      <c r="O66">
+        <v>60</v>
+      </c>
+      <c r="P66" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="Q66">
+        <v>10</v>
+      </c>
+      <c r="R66">
+        <v>10</v>
+      </c>
+      <c r="S66" s="12">
+        <v>0.03</v>
+      </c>
+      <c r="T66" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="U66" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="V66" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="W66" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="X66" s="12">
+        <v>0.12</v>
+      </c>
+      <c r="Y66" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z66" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="AA66" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="AB66">
+        <v>30</v>
+      </c>
+      <c r="AC66" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="AD66" s="19">
+        <v>1</v>
+      </c>
+      <c r="AE66">
+        <v>200</v>
+      </c>
+      <c r="AF66" t="s">
+        <v>117</v>
+      </c>
+      <c r="AG66">
+        <v>5</v>
+      </c>
+      <c r="AH66">
+        <v>200</v>
+      </c>
+      <c r="AI66" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="AJ66">
+        <v>1</v>
+      </c>
+      <c r="AK66" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="AL66" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="AM66" s="14">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AN66" s="14">
+        <v>0.05</v>
+      </c>
+      <c r="AO66" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP66" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="AQ66" s="21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>274</v>
+      </c>
+      <c r="B67" s="22" t="s">
+        <v>259</v>
+      </c>
+      <c r="C67" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D67" t="s">
+        <v>109</v>
+      </c>
+      <c r="E67" t="s">
+        <v>109</v>
+      </c>
+      <c r="F67" t="s">
+        <v>109</v>
+      </c>
+      <c r="G67" t="s">
+        <v>109</v>
+      </c>
+      <c r="H67" t="s">
+        <v>170</v>
+      </c>
+      <c r="I67" t="s">
+        <v>171</v>
+      </c>
+      <c r="J67" s="12">
+        <v>0</v>
+      </c>
+      <c r="K67" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="L67" s="12">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="M67">
+        <v>3</v>
+      </c>
+      <c r="N67">
+        <v>60</v>
+      </c>
+      <c r="O67">
+        <v>60</v>
+      </c>
+      <c r="P67" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="Q67">
+        <v>10</v>
+      </c>
+      <c r="R67">
+        <v>10</v>
+      </c>
+      <c r="S67" s="12">
+        <v>0.03</v>
+      </c>
+      <c r="T67" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="U67" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="V67" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="W67" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="X67" s="12">
+        <v>0.12</v>
+      </c>
+      <c r="Y67" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z67" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="AA67" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AB67">
+        <v>1</v>
+      </c>
+      <c r="AC67" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="AD67" s="19">
+        <v>0.75</v>
+      </c>
+      <c r="AE67">
+        <v>200</v>
+      </c>
+      <c r="AF67" t="s">
+        <v>144</v>
+      </c>
+      <c r="AG67">
+        <v>5</v>
+      </c>
+      <c r="AH67">
+        <v>200</v>
+      </c>
+      <c r="AI67" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="AJ67">
+        <v>1</v>
+      </c>
+      <c r="AK67" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="AL67" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="AM67" s="14">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AN67" s="14">
+        <v>0.05</v>
+      </c>
+      <c r="AO67" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP67" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="AQ67" s="21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>275</v>
+      </c>
+      <c r="B68" s="22" t="s">
+        <v>258</v>
+      </c>
+      <c r="C68" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D68" t="s">
+        <v>109</v>
+      </c>
+      <c r="E68" t="s">
+        <v>109</v>
+      </c>
+      <c r="F68" t="s">
+        <v>109</v>
+      </c>
+      <c r="G68" t="s">
+        <v>109</v>
+      </c>
+      <c r="H68" t="s">
+        <v>170</v>
+      </c>
+      <c r="I68" t="s">
+        <v>171</v>
+      </c>
+      <c r="J68" s="12">
+        <v>0</v>
+      </c>
+      <c r="K68" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="L68" s="12">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="M68">
+        <v>3</v>
+      </c>
+      <c r="N68">
+        <v>60</v>
+      </c>
+      <c r="O68">
+        <v>60</v>
+      </c>
+      <c r="P68" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="Q68">
+        <v>10</v>
+      </c>
+      <c r="R68">
+        <v>10</v>
+      </c>
+      <c r="S68" s="12">
+        <v>0.03</v>
+      </c>
+      <c r="T68" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="U68" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="V68" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="W68" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="X68" s="12">
+        <v>0.12</v>
+      </c>
+      <c r="Y68" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z68" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="AA68" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AB68">
+        <v>1</v>
+      </c>
+      <c r="AC68" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="AD68" s="19">
+        <v>0.75</v>
+      </c>
+      <c r="AE68">
+        <v>200</v>
+      </c>
+      <c r="AF68" t="s">
+        <v>144</v>
+      </c>
+      <c r="AG68">
+        <v>5</v>
+      </c>
+      <c r="AH68">
+        <v>200</v>
+      </c>
+      <c r="AI68" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="AJ68">
+        <v>1</v>
+      </c>
+      <c r="AK68" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="AL68" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="AM68" s="14">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AN68" s="14">
+        <v>0.05</v>
+      </c>
+      <c r="AO68" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP68" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="AQ68" s="21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>276</v>
+      </c>
+      <c r="B69" s="22" t="s">
+        <v>247</v>
+      </c>
+      <c r="C69" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D69" t="s">
+        <v>109</v>
+      </c>
+      <c r="E69" t="s">
+        <v>109</v>
+      </c>
+      <c r="F69" t="s">
+        <v>109</v>
+      </c>
+      <c r="G69" t="s">
+        <v>109</v>
+      </c>
+      <c r="H69" t="s">
+        <v>170</v>
+      </c>
+      <c r="I69" t="s">
+        <v>171</v>
+      </c>
+      <c r="J69" s="12">
+        <v>0</v>
+      </c>
+      <c r="K69" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="L69" s="12">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="M69">
+        <v>3</v>
+      </c>
+      <c r="N69">
+        <v>60</v>
+      </c>
+      <c r="O69">
+        <v>60</v>
+      </c>
+      <c r="P69" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="Q69">
+        <v>10</v>
+      </c>
+      <c r="R69">
+        <v>10</v>
+      </c>
+      <c r="S69" s="12">
+        <v>0.03</v>
+      </c>
+      <c r="T69" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="U69" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="V69" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="W69" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="X69" s="12">
+        <v>0.12</v>
+      </c>
+      <c r="Y69" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z69" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="AA69" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="AB69">
+        <v>30</v>
+      </c>
+      <c r="AC69" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="AD69" s="19">
+        <v>0.75</v>
+      </c>
+      <c r="AE69">
+        <v>200</v>
+      </c>
+      <c r="AF69" t="s">
+        <v>144</v>
+      </c>
+      <c r="AG69">
+        <v>5</v>
+      </c>
+      <c r="AH69">
+        <v>200</v>
+      </c>
+      <c r="AI69" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="AJ69">
+        <v>1</v>
+      </c>
+      <c r="AK69" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="AL69" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="AM69" s="14">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AN69" s="14">
+        <v>0.05</v>
+      </c>
+      <c r="AO69" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP69" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="AQ69" s="21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>277</v>
+      </c>
+      <c r="B70" s="22" t="s">
+        <v>248</v>
+      </c>
+      <c r="C70" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D70" t="s">
+        <v>109</v>
+      </c>
+      <c r="E70" t="s">
+        <v>109</v>
+      </c>
+      <c r="F70" t="s">
+        <v>109</v>
+      </c>
+      <c r="G70" t="s">
+        <v>109</v>
+      </c>
+      <c r="H70" t="s">
+        <v>170</v>
+      </c>
+      <c r="I70" t="s">
+        <v>171</v>
+      </c>
+      <c r="J70" s="12">
+        <v>0</v>
+      </c>
+      <c r="K70" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="L70" s="12">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="M70">
+        <v>3</v>
+      </c>
+      <c r="N70">
+        <v>60</v>
+      </c>
+      <c r="O70">
+        <v>60</v>
+      </c>
+      <c r="P70" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="Q70">
+        <v>10</v>
+      </c>
+      <c r="R70">
+        <v>10</v>
+      </c>
+      <c r="S70" s="12">
+        <v>0.03</v>
+      </c>
+      <c r="T70" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="U70" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="V70" t="s">
+        <v>158</v>
+      </c>
+      <c r="W70" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="X70" s="12">
+        <v>0.12</v>
+      </c>
+      <c r="Y70" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z70" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AA70" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AB70">
+        <v>15</v>
+      </c>
+      <c r="AC70" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="AD70" s="19">
+        <v>0.75</v>
+      </c>
+      <c r="AE70">
+        <v>200</v>
+      </c>
+      <c r="AF70" t="s">
+        <v>144</v>
+      </c>
+      <c r="AG70">
+        <v>5</v>
+      </c>
+      <c r="AH70">
+        <v>200</v>
+      </c>
+      <c r="AI70" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="AJ70">
+        <v>1</v>
+      </c>
+      <c r="AK70" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="AL70" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="AM70" s="14">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AN70" s="14">
+        <v>0.05</v>
+      </c>
+      <c r="AO70" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP70" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="AQ70" s="21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>278</v>
+      </c>
+      <c r="B71" s="22" t="s">
+        <v>249</v>
+      </c>
+      <c r="C71" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D71" t="s">
+        <v>109</v>
+      </c>
+      <c r="E71" t="s">
+        <v>109</v>
+      </c>
+      <c r="F71" t="s">
+        <v>109</v>
+      </c>
+      <c r="G71" t="s">
+        <v>109</v>
+      </c>
+      <c r="H71" t="s">
+        <v>170</v>
+      </c>
+      <c r="I71" t="s">
+        <v>171</v>
+      </c>
+      <c r="J71" s="12">
+        <v>0</v>
+      </c>
+      <c r="K71" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="L71" s="12">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="M71">
+        <v>3</v>
+      </c>
+      <c r="N71">
+        <v>60</v>
+      </c>
+      <c r="O71">
+        <v>60</v>
+      </c>
+      <c r="P71" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="Q71">
+        <v>10</v>
+      </c>
+      <c r="R71">
+        <v>10</v>
+      </c>
+      <c r="S71" s="12">
+        <v>0.03</v>
+      </c>
+      <c r="T71" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="U71" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="V71" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="W71" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="X71" s="12">
+        <v>0.12</v>
+      </c>
+      <c r="Y71" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z71" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AA71" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AB71">
+        <v>30</v>
+      </c>
+      <c r="AC71" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="AD71" s="19">
+        <v>0.75</v>
+      </c>
+      <c r="AE71">
+        <v>200</v>
+      </c>
+      <c r="AF71" t="s">
+        <v>144</v>
+      </c>
+      <c r="AG71">
+        <v>5</v>
+      </c>
+      <c r="AH71">
+        <v>200</v>
+      </c>
+      <c r="AI71" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="AJ71">
+        <v>1</v>
+      </c>
+      <c r="AK71" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="AL71" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="AM71" s="14">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AN71" s="14">
+        <v>0.05</v>
+      </c>
+      <c r="AO71" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP71" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="AQ71" s="21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>279</v>
+      </c>
+      <c r="B72" s="22" t="s">
+        <v>250</v>
+      </c>
+      <c r="C72" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D72" t="s">
+        <v>109</v>
+      </c>
+      <c r="E72" t="s">
+        <v>109</v>
+      </c>
+      <c r="F72" t="s">
+        <v>109</v>
+      </c>
+      <c r="G72" t="s">
+        <v>109</v>
+      </c>
+      <c r="H72" t="s">
+        <v>170</v>
+      </c>
+      <c r="I72" t="s">
+        <v>171</v>
+      </c>
+      <c r="J72" s="12">
+        <v>0</v>
+      </c>
+      <c r="K72" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="L72" s="12">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="M72">
+        <v>3</v>
+      </c>
+      <c r="N72">
+        <v>60</v>
+      </c>
+      <c r="O72">
+        <v>60</v>
+      </c>
+      <c r="P72" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="Q72">
+        <v>10</v>
+      </c>
+      <c r="R72">
+        <v>10</v>
+      </c>
+      <c r="S72" s="12">
+        <v>0.03</v>
+      </c>
+      <c r="T72" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="U72" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="V72" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="W72" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="X72" s="12">
+        <v>0.12</v>
+      </c>
+      <c r="Y72" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z72" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AA72" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="AB72">
+        <v>30</v>
+      </c>
+      <c r="AC72" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="AD72" s="19">
+        <v>0.75</v>
+      </c>
+      <c r="AE72">
+        <v>200</v>
+      </c>
+      <c r="AF72" t="s">
+        <v>144</v>
+      </c>
+      <c r="AG72">
+        <v>5</v>
+      </c>
+      <c r="AH72">
+        <v>200</v>
+      </c>
+      <c r="AI72" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="AJ72">
+        <v>1</v>
+      </c>
+      <c r="AK72" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="AL72" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="AM72" s="14">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AN72" s="14">
+        <v>0.05</v>
+      </c>
+      <c r="AO72" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP72" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="AQ72" s="21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>280</v>
+      </c>
+      <c r="B73" s="22" t="s">
+        <v>230</v>
+      </c>
+      <c r="C73" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D73" t="s">
+        <v>109</v>
+      </c>
+      <c r="E73" t="s">
+        <v>109</v>
+      </c>
+      <c r="F73" t="s">
+        <v>109</v>
+      </c>
+      <c r="G73" t="s">
+        <v>109</v>
+      </c>
+      <c r="H73" t="s">
+        <v>170</v>
+      </c>
+      <c r="I73" t="s">
+        <v>171</v>
+      </c>
+      <c r="J73" s="12">
+        <v>0</v>
+      </c>
+      <c r="K73" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="L73" s="12">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="M73">
+        <v>3</v>
+      </c>
+      <c r="N73">
+        <v>60</v>
+      </c>
+      <c r="O73">
+        <v>60</v>
+      </c>
+      <c r="P73" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="Q73">
+        <v>10</v>
+      </c>
+      <c r="R73">
+        <v>10</v>
+      </c>
+      <c r="S73" s="12">
+        <v>0.03</v>
+      </c>
+      <c r="T73" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="U73" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="V73" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="W73" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="X73" s="12">
+        <v>0.12</v>
+      </c>
+      <c r="Y73" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z73" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="AA73" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="AB73">
+        <v>30</v>
+      </c>
+      <c r="AC73" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="AD73" s="19">
+        <v>0.75</v>
+      </c>
+      <c r="AE73">
+        <v>200</v>
+      </c>
+      <c r="AF73" t="s">
+        <v>117</v>
+      </c>
+      <c r="AG73">
+        <v>5</v>
+      </c>
+      <c r="AH73">
+        <v>200</v>
+      </c>
+      <c r="AI73" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="AJ73">
+        <v>1</v>
+      </c>
+      <c r="AK73" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="AL73" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="AM73" s="14">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AN73" s="14">
+        <v>0.05</v>
+      </c>
+      <c r="AO73" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP73" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="AQ73" s="21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>285</v>
+      </c>
+      <c r="B74" s="22" t="s">
+        <v>236</v>
+      </c>
+      <c r="C74" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D74" t="s">
+        <v>109</v>
+      </c>
+      <c r="E74" t="s">
+        <v>109</v>
+      </c>
+      <c r="F74" t="s">
+        <v>109</v>
+      </c>
+      <c r="G74" t="s">
+        <v>109</v>
+      </c>
+      <c r="H74" t="s">
+        <v>170</v>
+      </c>
+      <c r="I74" t="s">
+        <v>171</v>
+      </c>
+      <c r="J74" s="12">
+        <v>0</v>
+      </c>
+      <c r="K74" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="L74" s="12">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="M74">
+        <v>3</v>
+      </c>
+      <c r="N74">
+        <v>60</v>
+      </c>
+      <c r="O74">
+        <v>60</v>
+      </c>
+      <c r="P74" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="Q74">
+        <v>10</v>
+      </c>
+      <c r="R74">
+        <v>10</v>
+      </c>
+      <c r="S74" s="12">
+        <v>0.03</v>
+      </c>
+      <c r="T74" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="U74" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="V74" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="W74" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="X74" s="12">
+        <v>0.12</v>
+      </c>
+      <c r="Y74" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z74" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="AA74" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="AB74">
+        <v>30</v>
+      </c>
+      <c r="AC74" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="AD74" s="19">
+        <v>1</v>
+      </c>
+      <c r="AE74">
+        <v>200</v>
+      </c>
+      <c r="AF74" t="s">
+        <v>117</v>
+      </c>
+      <c r="AG74">
+        <v>5</v>
+      </c>
+      <c r="AH74">
+        <v>200</v>
+      </c>
+      <c r="AI74" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="AJ74">
+        <v>1</v>
+      </c>
+      <c r="AK74" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="AL74" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="AM74" s="14">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AN74" s="14">
+        <v>0.05</v>
+      </c>
+      <c r="AO74" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP74" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="AQ74" s="21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>281</v>
+      </c>
+      <c r="B75" s="22" t="s">
+        <v>273</v>
+      </c>
+      <c r="C75" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D75" t="s">
+        <v>109</v>
+      </c>
+      <c r="E75" t="s">
+        <v>109</v>
+      </c>
+      <c r="F75" t="s">
+        <v>109</v>
+      </c>
+      <c r="G75" t="s">
+        <v>109</v>
+      </c>
+      <c r="H75" t="s">
+        <v>170</v>
+      </c>
+      <c r="I75" t="s">
+        <v>171</v>
+      </c>
+      <c r="J75" s="12">
+        <v>0</v>
+      </c>
+      <c r="K75" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="L75" s="12">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="M75">
+        <v>3</v>
+      </c>
+      <c r="N75">
+        <v>60</v>
+      </c>
+      <c r="O75">
+        <v>60</v>
+      </c>
+      <c r="P75" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="Q75">
+        <v>10</v>
+      </c>
+      <c r="R75">
+        <v>10</v>
+      </c>
+      <c r="S75" s="12">
+        <v>0.03</v>
+      </c>
+      <c r="T75" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="U75" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="V75" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="W75" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="X75" s="12">
+        <v>0</v>
+      </c>
+      <c r="Y75" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z75" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="AA75" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="AB75">
+        <v>30</v>
+      </c>
+      <c r="AC75" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="AD75" s="19">
+        <v>0.75</v>
+      </c>
+      <c r="AE75">
+        <v>200</v>
+      </c>
+      <c r="AF75" t="s">
+        <v>117</v>
+      </c>
+      <c r="AG75">
+        <v>5</v>
+      </c>
+      <c r="AH75">
+        <v>200</v>
+      </c>
+      <c r="AI75" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="AJ75">
+        <v>1</v>
+      </c>
+      <c r="AK75" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="AL75" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="AM75" s="14">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AN75" s="14">
+        <v>0.05</v>
+      </c>
+      <c r="AO75" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP75" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="AQ75" s="21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="C76" s="11"/>
+      <c r="L76" s="12"/>
+      <c r="P76" s="12"/>
+    </row>
+    <row r="77" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>282</v>
+      </c>
+      <c r="B77" s="22" t="s">
+        <v>267</v>
+      </c>
+      <c r="C77" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D77" t="s">
+        <v>109</v>
+      </c>
+      <c r="E77" t="s">
+        <v>109</v>
+      </c>
+      <c r="F77" t="s">
+        <v>109</v>
+      </c>
+      <c r="G77" t="s">
+        <v>109</v>
+      </c>
+      <c r="H77" t="s">
+        <v>170</v>
+      </c>
+      <c r="I77" t="s">
+        <v>171</v>
+      </c>
+      <c r="J77" s="12">
+        <v>0</v>
+      </c>
+      <c r="K77" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="L77" s="12">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="M77">
+        <v>3</v>
+      </c>
+      <c r="N77">
+        <v>60</v>
+      </c>
+      <c r="O77">
+        <v>60</v>
+      </c>
+      <c r="P77" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="Q77">
+        <v>10</v>
+      </c>
+      <c r="R77">
+        <v>10</v>
+      </c>
+      <c r="S77" s="12">
+        <v>0.03</v>
+      </c>
+      <c r="T77" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="U77" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="V77" t="s">
+        <v>158</v>
+      </c>
+      <c r="W77" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="X77" s="12">
+        <v>0.12</v>
+      </c>
+      <c r="Y77" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z77" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="AA77" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AB77">
+        <v>15</v>
+      </c>
+      <c r="AC77" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="AD77" s="19">
+        <v>0.75</v>
+      </c>
+      <c r="AE77">
+        <v>200</v>
+      </c>
+      <c r="AF77" t="s">
+        <v>144</v>
+      </c>
+      <c r="AG77">
+        <v>5</v>
+      </c>
+      <c r="AH77">
+        <v>200</v>
+      </c>
+      <c r="AI77" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="AJ77">
+        <v>1</v>
+      </c>
+      <c r="AK77" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="AL77" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="AM77" s="14">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AN77" s="14">
+        <v>0.05</v>
+      </c>
+      <c r="AO77" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP77" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="AQ77" s="21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>283</v>
+      </c>
+      <c r="B78" s="22" t="s">
+        <v>228</v>
+      </c>
+      <c r="C78" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D78" t="s">
+        <v>109</v>
+      </c>
+      <c r="E78" t="s">
+        <v>109</v>
+      </c>
+      <c r="F78" t="s">
+        <v>109</v>
+      </c>
+      <c r="G78" t="s">
+        <v>109</v>
+      </c>
+      <c r="H78" t="s">
+        <v>170</v>
+      </c>
+      <c r="I78" t="s">
+        <v>171</v>
+      </c>
+      <c r="J78" s="12">
+        <v>0</v>
+      </c>
+      <c r="K78" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="L78" s="12">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="M78">
+        <v>3</v>
+      </c>
+      <c r="N78">
+        <v>60</v>
+      </c>
+      <c r="O78">
+        <v>60</v>
+      </c>
+      <c r="P78" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="Q78">
+        <v>10</v>
+      </c>
+      <c r="R78">
+        <v>10</v>
+      </c>
+      <c r="S78" s="12">
+        <v>0.03</v>
+      </c>
+      <c r="T78" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="U78" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="V78" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="W78" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="X78" s="12">
+        <v>0.12</v>
+      </c>
+      <c r="Y78" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z78" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="AA78" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AB78">
+        <v>1</v>
+      </c>
+      <c r="AC78" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="AD78" s="19">
+        <v>0.75</v>
+      </c>
+      <c r="AE78">
+        <v>200</v>
+      </c>
+      <c r="AF78" t="s">
+        <v>117</v>
+      </c>
+      <c r="AG78">
+        <v>5</v>
+      </c>
+      <c r="AH78">
+        <v>200</v>
+      </c>
+      <c r="AI78" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="AJ78">
+        <v>1</v>
+      </c>
+      <c r="AK78" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="AL78" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="AM78" s="14">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AN78" s="14">
+        <v>0.05</v>
+      </c>
+      <c r="AO78" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP78" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="AQ78" s="21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>288</v>
+      </c>
+      <c r="B80" s="22" t="s">
+        <v>286</v>
+      </c>
+      <c r="C80" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="D80" t="s">
+        <v>109</v>
+      </c>
+      <c r="E80" t="s">
+        <v>109</v>
+      </c>
+      <c r="F80" t="s">
+        <v>109</v>
+      </c>
+      <c r="G80" t="s">
+        <v>109</v>
+      </c>
+      <c r="H80" t="s">
+        <v>170</v>
+      </c>
+      <c r="I80" t="s">
+        <v>171</v>
+      </c>
+      <c r="J80" s="12">
+        <v>0</v>
+      </c>
+      <c r="K80" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="L80" s="12">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="M80">
+        <v>3</v>
+      </c>
+      <c r="N80">
+        <v>60</v>
+      </c>
+      <c r="O80">
+        <v>60</v>
+      </c>
+      <c r="P80" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="Q80">
+        <v>10</v>
+      </c>
+      <c r="R80">
+        <v>10</v>
+      </c>
+      <c r="S80" s="12">
+        <v>0.03</v>
+      </c>
+      <c r="T80" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="U80" s="12">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="V80" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="W80" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="X80" s="12">
+        <v>0.12</v>
+      </c>
+      <c r="Y80" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z80" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="AA80" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="AB80">
+        <v>15</v>
+      </c>
+      <c r="AC80" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="AD80" s="19">
+        <v>0.75</v>
+      </c>
+      <c r="AE80">
+        <v>200</v>
+      </c>
+      <c r="AF80" t="s">
+        <v>117</v>
+      </c>
+      <c r="AG80">
+        <v>5</v>
+      </c>
+      <c r="AH80">
+        <v>200</v>
+      </c>
+      <c r="AI80" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="AJ80">
+        <v>1</v>
+      </c>
+      <c r="AK80" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="AL80" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="AM80" s="14">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AN80" s="14">
+        <v>0.05</v>
+      </c>
+      <c r="AO80" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP80" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="AQ80" s="21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>289</v>
+      </c>
+      <c r="B81" s="22" t="s">
+        <v>287</v>
+      </c>
+      <c r="C81" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="D81" t="s">
+        <v>109</v>
+      </c>
+      <c r="E81" t="s">
+        <v>109</v>
+      </c>
+      <c r="F81" t="s">
+        <v>109</v>
+      </c>
+      <c r="G81" t="s">
+        <v>109</v>
+      </c>
+      <c r="H81" t="s">
+        <v>170</v>
+      </c>
+      <c r="I81" t="s">
+        <v>171</v>
+      </c>
+      <c r="J81" s="12">
+        <v>0</v>
+      </c>
+      <c r="K81" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="L81" s="12">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="M81">
+        <v>3</v>
+      </c>
+      <c r="N81">
+        <v>60</v>
+      </c>
+      <c r="O81">
+        <v>60</v>
+      </c>
+      <c r="P81" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="Q81">
+        <v>10</v>
+      </c>
+      <c r="R81">
+        <v>10</v>
+      </c>
+      <c r="S81" s="12">
+        <v>0.03</v>
+      </c>
+      <c r="T81" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="U81" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="V81" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="W81" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="X81" s="12">
+        <v>0.12</v>
+      </c>
+      <c r="Y81" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z81" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="AA81" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="AB81">
+        <v>15</v>
+      </c>
+      <c r="AC81" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="AD81" s="19">
+        <v>0.75</v>
+      </c>
+      <c r="AE81">
+        <v>200</v>
+      </c>
+      <c r="AF81" t="s">
+        <v>117</v>
+      </c>
+      <c r="AG81">
+        <v>5</v>
+      </c>
+      <c r="AH81">
+        <v>200</v>
+      </c>
+      <c r="AI81" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="AJ81">
+        <v>1</v>
+      </c>
+      <c r="AK81" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="AL81" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="AM81" s="14">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AN81" s="14">
+        <v>0.05</v>
+      </c>
+      <c r="AO81" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP81" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="AQ81" s="21" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="J4:K4"/>
     <mergeCell ref="AC4:AE4"/>
     <mergeCell ref="L4:R4"/>
     <mergeCell ref="S4:U4"/>
     <mergeCell ref="Z4:AB4"/>
     <mergeCell ref="AK4:AN4"/>
     <mergeCell ref="V4:X4"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="J4:K4"/>
   </mergeCells>
   <dataValidations count="20">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AI6:AI21 AI55:AI63 AI23:AI53">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AI6:AI21 AI55:AI63 AI23:AI53 AI66:AI75 AI77:AI78 AI80:AI81">
       <formula1>"MA,EAA"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA6:AA21 AA55:AA63 AA23:AA53">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA6:AA21 AA55:AA63 AA23:AA53 AA66:AA75 AA77:AA78 AA80:AA81">
       <formula1>"cd,cp,sl"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z6:Z21 Z55:Z63 Z23:Z53">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z6:Z21 Z55:Z63 Z23:Z53 Z66:Z75 Z77:Z78 Z80:Z81">
       <formula1>"open,closed"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AK6:AK21 AK55:AK63 AK23:AK53">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AK6:AK21 AK55:AK63 AK23:AK53 AK66:AK75 AK77:AK78 AK80:AK81">
       <formula1>ConPolicy</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K55:K63 K6:K21 K23:K53 C6:C63">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K55:K63 K6:K21 K23:K53 C80:C81 K66:K75 C6:C63 K77:K78 K80:K81 C66:C78">
       <formula1>"TRUE,FALSE"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer 55 to 65, please" sqref="N6:N21 N55:N63 N23:N53">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer 55 to 65, please" sqref="N6:N21 N55:N63 N23:N53 N66:O78 N80:N81">
       <formula1>55</formula1>
       <formula2>65</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-10% please" sqref="P6:P21 P55:P63 T55:T63 T6:T21 P23:P53 T23:T53">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-10% please" sqref="P6:P21 P55:P63 T55:T63 T6:T21 P23:P53 T23:T53 T77:T78 T66:T75 P66:P78 P80:P81 T80:T81">
       <formula1>0</formula1>
       <formula2>0.1</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 0-15" sqref="Q6:R21 Q55:R63 Q23:R53">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 0-15" sqref="Q6:R21 Q55:R63 Q23:R53 Q66:R75 Q77:R78 Q80:R81">
       <formula1>0</formula1>
       <formula2>15</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="S6:S21 U6:U21 U55:U63 W55:W63 S55:S63 W6:W21 S23:S53 W23:W53 U23:U53">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="S6:S21 U6:U21 U55:U63 W55:W63 S55:S63 W6:W21 S23:S53 W23:W53 U23:U53 S66:S75 U66:U75 W66:W75 S77:S78 W77:W78 U77:U78 U80:U81 W80:W81 S80:S81">
       <formula1>0</formula1>
       <formula2>0.2</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 0 to 30, please" sqref="AB6:AB21 AB55:AB63 AB23:AB53">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 0 to 30, please" sqref="AB6:AB21 AB55:AB63 AB23:AB53 AB66:AB75 AB77:AB78 AB80:AB81">
       <formula1>0</formula1>
       <formula2>30</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-75%" sqref="AL6:AM21 AL55:AM63 AL23:AM53">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-75%" sqref="AL6:AM21 AL55:AM63 AL23:AM53 AL66:AM75 AL77:AM78 AL80:AM81">
       <formula1>0</formula1>
       <formula2>0.75</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-30%" sqref="AN6:AN21 AN55:AN63 AN23:AN53">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-30%" sqref="AN6:AN21 AN55:AN63 AN23:AN53 AN66:AN75 AN77:AN78 AN80:AN81">
       <formula1>0</formula1>
       <formula2>0.3</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-75% please" sqref="X6:X21 X55:X63 X23:X53">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-75% please" sqref="X6:X21 X55:X63 X23:X53 X66:X75 X77:X78 X80:X81">
       <formula1>0</formula1>
       <formula2>0.75</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 1 to 30" sqref="AG6:AG21 AG55:AG63 AG23:AG53">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 1 to 30" sqref="AG6:AG21 AG55:AG63 AG23:AG53 AG66:AG75 AG77:AG78 AG80:AG81">
       <formula1>1</formula1>
       <formula2>30</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AH6:AH21 AH55:AH63 AH23:AH53">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AH6:AH21 AH55:AH63 AH23:AH53 AH66:AH75 AH77:AH78 AH80:AH81">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AJ6:AJ21 AJ55:AJ63 AJ23:AJ53">
+    <dataValidation type="decimal" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AJ6:AJ21 AJ55:AJ63 AJ23:AJ53 AJ66:AJ75 AJ77:AJ78 AJ80:AJ81">
       <formula1>1</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="V6:V21 V55:V63 V23:V53"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AO55:AQ63 AO6:AQ53">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="V6:V21 V55:V63 V23:V53 V66:V75 V77:V78 V80:V81"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AO55:AQ63 AO6:AQ53 AO66:AQ75 AO77:AQ78 AO80:AQ81">
       <formula1>"TRUE, FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AC55:AC63 AC6:AC53">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AC55:AC63 AC6:AC53 AC66:AC75 AC77:AC78 AC80:AC81">
       <formula1>"MA,AL,AL_pct"</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AD55:AD63 AD6:AD53">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AD55:AD63 AD6:AD53 AD66:AD75 AD77:AD78 AD80:AD81">
       <formula1>0</formula1>
       <formula2>1.5</formula2>
     </dataValidation>
@@ -8988,13 +10880,13 @@
           <x14:formula1>
             <xm:f>DropDowns!$A$37:$A$41</xm:f>
           </x14:formula1>
-          <xm:sqref>H55:H63 H6:H17 H20:H53</xm:sqref>
+          <xm:sqref>H55:H63 H6:H17 H20:H53 H66:H78 H80:H81</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DropDowns!$A$44:$A$46</xm:f>
           </x14:formula1>
-          <xm:sqref>I55:I63 I6:I17 I20:I53</xm:sqref>
+          <xm:sqref>I55:I63 I6:I17 I20:I53 I66:I75 I77:I78 I80:I81</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
@@ -9013,7 +10905,7 @@
   <dimension ref="A3:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9204,20 +11096,40 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>285</v>
+      </c>
+      <c r="B16" s="12">
+        <v>-0.25</v>
+      </c>
+      <c r="C16" s="12">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>285</v>
+      </c>
+      <c r="B17" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="C17" s="12">
+        <v>0.12</v>
+      </c>
+      <c r="D17">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B18" s="12"/>
       <c r="C18" s="12"/>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="B16:B18">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="B18">
       <formula1>0</formula1>
       <formula2>0.2</formula2>
     </dataValidation>
@@ -9225,7 +11137,7 @@
       <formula1>0</formula1>
       <formula2>0.75</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="B4:B15">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="B4:B17">
       <formula1>-1</formula1>
       <formula2>0.5</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
More runs for M2.1
</commit_message>
<xml_diff>
--- a/IO_M1/RunControl_M1.xlsx
+++ b/IO_M1/RunControl_M1.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1262" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1278" uniqueCount="291">
   <si>
     <t>Sheet #</t>
   </si>
@@ -902,6 +902,9 @@
   </si>
   <si>
     <t>C1F075_soa2</t>
+  </si>
+  <si>
+    <t>C1F075_soa3</t>
   </si>
 </sst>
 </file>
@@ -1635,13 +1638,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AQ81"/>
+  <dimension ref="A1:AQ82"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="V62" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="5" topLeftCell="B66" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="U1" sqref="U1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="X84" sqref="X84"/>
+      <selection pane="bottomRight" activeCell="C86" sqref="C86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1662,8 +1665,9 @@
     <col min="29" max="30" width="11.7109375" customWidth="1"/>
     <col min="31" max="31" width="13.140625" customWidth="1"/>
     <col min="32" max="32" width="11.85546875" customWidth="1"/>
+    <col min="34" max="34" width="9.140625" customWidth="1"/>
     <col min="37" max="40" width="12.7109375"/>
-    <col min="43" max="43" width="9" customWidth="1"/>
+    <col min="43" max="43" width="10.42578125" customWidth="1"/>
     <col min="44" max="1030" width="8.5703125"/>
   </cols>
   <sheetData>
@@ -10526,7 +10530,7 @@
         <v>286</v>
       </c>
       <c r="C80" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D80" t="s">
         <v>109</v>
@@ -10657,7 +10661,7 @@
         <v>287</v>
       </c>
       <c r="C81" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D81" t="s">
         <v>109</v>
@@ -10777,6 +10781,137 @@
         <v>1</v>
       </c>
       <c r="AQ81" s="21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>290</v>
+      </c>
+      <c r="B82" s="22" t="s">
+        <v>286</v>
+      </c>
+      <c r="C82" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="D82" t="s">
+        <v>109</v>
+      </c>
+      <c r="E82" t="s">
+        <v>109</v>
+      </c>
+      <c r="F82" t="s">
+        <v>109</v>
+      </c>
+      <c r="G82" t="s">
+        <v>109</v>
+      </c>
+      <c r="H82" t="s">
+        <v>170</v>
+      </c>
+      <c r="I82" t="s">
+        <v>171</v>
+      </c>
+      <c r="J82" s="12">
+        <v>0</v>
+      </c>
+      <c r="K82" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="L82" s="12">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="M82">
+        <v>3</v>
+      </c>
+      <c r="N82">
+        <v>60</v>
+      </c>
+      <c r="O82">
+        <v>60</v>
+      </c>
+      <c r="P82" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="Q82">
+        <v>10</v>
+      </c>
+      <c r="R82">
+        <v>10</v>
+      </c>
+      <c r="S82" s="12">
+        <v>0.03</v>
+      </c>
+      <c r="T82" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="U82" s="12">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="V82" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="W82" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="X82" s="12">
+        <v>0.12</v>
+      </c>
+      <c r="Y82" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z82" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="AA82" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="AB82">
+        <v>15</v>
+      </c>
+      <c r="AC82" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="AD82" s="19">
+        <v>0.75</v>
+      </c>
+      <c r="AE82">
+        <v>137995080</v>
+      </c>
+      <c r="AF82" t="s">
+        <v>117</v>
+      </c>
+      <c r="AG82">
+        <v>5</v>
+      </c>
+      <c r="AH82">
+        <v>137995080</v>
+      </c>
+      <c r="AI82" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="AJ82">
+        <v>1</v>
+      </c>
+      <c r="AK82" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="AL82" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="AM82" s="14">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AN82" s="14">
+        <v>0.05</v>
+      </c>
+      <c r="AO82" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP82" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="AQ82" s="21" t="b">
         <v>0</v>
       </c>
     </row>
@@ -10795,78 +10930,78 @@
     <mergeCell ref="V4:X4"/>
   </mergeCells>
   <dataValidations count="20">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AI6:AI21 AI55:AI63 AI23:AI53 AI66:AI75 AI77:AI78 AI80:AI81">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AI6:AI21 AI55:AI63 AI23:AI53 AI66:AI75 AI77:AI78 AI80:AI82">
       <formula1>"MA,EAA"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA6:AA21 AA55:AA63 AA23:AA53 AA66:AA75 AA77:AA78 AA80:AA81">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA6:AA21 AA55:AA63 AA23:AA53 AA66:AA75 AA77:AA78 AA80:AA82">
       <formula1>"cd,cp,sl"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z6:Z21 Z55:Z63 Z23:Z53 Z66:Z75 Z77:Z78 Z80:Z81">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z6:Z21 Z55:Z63 Z23:Z53 Z66:Z75 Z77:Z78 Z80:Z82">
       <formula1>"open,closed"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AK6:AK21 AK55:AK63 AK23:AK53 AK66:AK75 AK77:AK78 AK80:AK81">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AK6:AK21 AK55:AK63 AK23:AK53 AK66:AK75 AK77:AK78 AK80:AK82">
       <formula1>ConPolicy</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K55:K63 K6:K21 K23:K53 C80:C81 K66:K75 C6:C63 K77:K78 K80:K81 C66:C78">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K55:K63 K6:K21 K23:K53 C80:C82 K66:K75 C6:C63 K77:K78 K80:K82 C66:C78">
       <formula1>"TRUE,FALSE"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer 55 to 65, please" sqref="N6:N21 N55:N63 N23:N53 N66:O78 N80:N81">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer 55 to 65, please" sqref="N6:N21 N55:N63 N23:N53 N66:O78 N80:N82">
       <formula1>55</formula1>
       <formula2>65</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-10% please" sqref="P6:P21 P55:P63 T55:T63 T6:T21 P23:P53 T23:T53 T77:T78 T66:T75 P66:P78 P80:P81 T80:T81">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-10% please" sqref="P6:P21 P55:P63 T55:T63 T6:T21 P23:P53 T23:T53 T77:T78 T66:T75 P66:P78 P80:P82 T80:T82">
       <formula1>0</formula1>
       <formula2>0.1</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 0-15" sqref="Q6:R21 Q55:R63 Q23:R53 Q66:R75 Q77:R78 Q80:R81">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 0-15" sqref="Q6:R21 Q55:R63 Q23:R53 Q66:R75 Q77:R78 Q80:R82">
       <formula1>0</formula1>
       <formula2>15</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="S6:S21 U6:U21 U55:U63 W55:W63 S55:S63 W6:W21 S23:S53 W23:W53 U23:U53 S66:S75 U66:U75 W66:W75 S77:S78 W77:W78 U77:U78 U80:U81 W80:W81 S80:S81">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="S6:S21 U6:U21 U55:U63 W55:W63 S55:S63 W6:W21 S23:S53 W23:W53 U23:U53 S66:S75 U66:U75 W66:W75 S77:S78 W77:W78 U77:U78 U80:U82 W80:W82 S80:S82">
       <formula1>0</formula1>
       <formula2>0.2</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 0 to 30, please" sqref="AB6:AB21 AB55:AB63 AB23:AB53 AB66:AB75 AB77:AB78 AB80:AB81">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 0 to 30, please" sqref="AB6:AB21 AB55:AB63 AB23:AB53 AB66:AB75 AB77:AB78 AB80:AB82">
       <formula1>0</formula1>
       <formula2>30</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-75%" sqref="AL6:AM21 AL55:AM63 AL23:AM53 AL66:AM75 AL77:AM78 AL80:AM81">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-75%" sqref="AL6:AM21 AL55:AM63 AL23:AM53 AL66:AM75 AL77:AM78 AL80:AM82">
       <formula1>0</formula1>
       <formula2>0.75</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-30%" sqref="AN6:AN21 AN55:AN63 AN23:AN53 AN66:AN75 AN77:AN78 AN80:AN81">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-30%" sqref="AN6:AN21 AN55:AN63 AN23:AN53 AN66:AN75 AN77:AN78 AN80:AN82">
       <formula1>0</formula1>
       <formula2>0.3</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-75% please" sqref="X6:X21 X55:X63 X23:X53 X66:X75 X77:X78 X80:X81">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-75% please" sqref="X6:X21 X55:X63 X23:X53 X66:X75 X77:X78 X80:X82">
       <formula1>0</formula1>
       <formula2>0.75</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 1 to 30" sqref="AG6:AG21 AG55:AG63 AG23:AG53 AG66:AG75 AG77:AG78 AG80:AG81">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 1 to 30" sqref="AG6:AG21 AG55:AG63 AG23:AG53 AG66:AG75 AG77:AG78 AG80:AG82">
       <formula1>1</formula1>
       <formula2>30</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AH6:AH21 AH55:AH63 AH23:AH53 AH66:AH75 AH77:AH78 AH80:AH81">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AH6:AH21 AH55:AH63 AH23:AH53 AH66:AH75 AH77:AH78 AH80:AH82">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AJ6:AJ21 AJ55:AJ63 AJ23:AJ53 AJ66:AJ75 AJ77:AJ78 AJ80:AJ81">
+    <dataValidation type="decimal" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AJ6:AJ21 AJ55:AJ63 AJ23:AJ53 AJ66:AJ75 AJ77:AJ78 AJ80:AJ82">
       <formula1>1</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="V6:V21 V55:V63 V23:V53 V66:V75 V77:V78 V80:V81"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AO55:AQ63 AO6:AQ53 AO66:AQ75 AO77:AQ78 AO80:AQ81">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="V6:V21 V55:V63 V23:V53 V66:V75 V77:V78 V80:V82"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AO55:AQ63 AO6:AQ53 AO66:AQ75 AO77:AQ78 AO80:AQ82">
       <formula1>"TRUE, FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AC55:AC63 AC6:AC53 AC66:AC75 AC77:AC78 AC80:AC81">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AC55:AC63 AC6:AC53 AC66:AC75 AC77:AC78 AC80:AC82">
       <formula1>"MA,AL,AL_pct"</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AD55:AD63 AD6:AD53 AD66:AD75 AD77:AD78 AD80:AD81">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AD55:AD63 AD6:AD53 AD66:AD75 AD77:AD78 AD80:AD82">
       <formula1>0</formula1>
       <formula2>1.5</formula2>
     </dataValidation>
@@ -10880,13 +11015,13 @@
           <x14:formula1>
             <xm:f>DropDowns!$A$37:$A$41</xm:f>
           </x14:formula1>
-          <xm:sqref>H55:H63 H6:H17 H20:H53 H66:H78 H80:H81</xm:sqref>
+          <xm:sqref>H55:H63 H6:H17 H20:H53 H66:H78 H80:H82</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DropDowns!$A$44:$A$46</xm:f>
           </x14:formula1>
-          <xm:sqref>I55:I63 I6:I17 I20:I53 I66:I75 I77:I78 I80:I81</xm:sqref>
+          <xm:sqref>I55:I63 I6:I17 I20:I53 I66:I75 I77:I78 I80:I82</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>

</xml_diff>

<commit_message>
fix small bug in investment return
</commit_message>
<xml_diff>
--- a/IO_M1/RunControl_M1.xlsx
+++ b/IO_M1/RunControl_M1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19164" windowHeight="7164" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="7170" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="TOC" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Returns!$A$3:$D$12</definedName>
     <definedName name="ConPolicy">DropDowns!$A$12:$A$14</definedName>
   </definedNames>
-  <calcPr calcId="152511" iterateDelta="1E-4"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -856,7 +856,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* \-??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
@@ -1035,7 +1035,13 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1044,16 +1050,10 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1155,6 +1155,7 @@
       <sheetName val="Contributions"/>
       <sheetName val="GlobalParams"/>
       <sheetName val="DropDowns"/>
+      <sheetName val="Sheet1"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0"/>
@@ -1164,6 +1165,7 @@
       <sheetData sheetId="4"/>
       <sheetData sheetId="5"/>
       <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1441,14 +1443,14 @@
       <selection pane="bottomRight" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.5546875"/>
-    <col min="2" max="2" width="16.6640625"/>
-    <col min="3" max="1025" width="8.5546875"/>
+    <col min="1" max="1" width="7.5703125"/>
+    <col min="2" max="2" width="16.7109375"/>
+    <col min="3" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1456,7 +1458,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1464,7 +1466,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -1472,7 +1474,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -1499,77 +1501,77 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1025" width="8.5546875"/>
+    <col min="1" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>21</v>
       </c>
@@ -1584,37 +1586,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AQ63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="B54" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="5" topLeftCell="B38" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="U1" sqref="U1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="C23" sqref="C23:C25"/>
+      <selection pane="bottomRight" activeCell="V41" sqref="V41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.88671875" customWidth="1"/>
-    <col min="2" max="2" width="73.44140625" customWidth="1"/>
-    <col min="3" max="3" width="18.88671875" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" customWidth="1"/>
+    <col min="2" max="2" width="95.42578125" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" customWidth="1"/>
     <col min="4" max="7" width="16" customWidth="1"/>
-    <col min="8" max="8" width="24.44140625"/>
-    <col min="9" max="9" width="13.44140625" customWidth="1"/>
-    <col min="10" max="11" width="13.109375" customWidth="1"/>
-    <col min="12" max="15" width="9.33203125" customWidth="1"/>
+    <col min="8" max="8" width="24.42578125"/>
+    <col min="9" max="9" width="13.42578125" customWidth="1"/>
+    <col min="10" max="11" width="13.140625" customWidth="1"/>
+    <col min="12" max="15" width="9.28515625" customWidth="1"/>
     <col min="16" max="16" width="16"/>
-    <col min="17" max="21" width="12.6640625"/>
-    <col min="22" max="22" width="11.109375" customWidth="1"/>
-    <col min="23" max="27" width="12.6640625"/>
-    <col min="28" max="28" width="12.6640625" customWidth="1"/>
-    <col min="29" max="30" width="11.6640625" customWidth="1"/>
-    <col min="31" max="31" width="13.109375" customWidth="1"/>
-    <col min="32" max="32" width="11.88671875" customWidth="1"/>
-    <col min="37" max="40" width="12.6640625"/>
+    <col min="17" max="21" width="12.7109375"/>
+    <col min="22" max="22" width="11.140625" customWidth="1"/>
+    <col min="23" max="27" width="12.7109375"/>
+    <col min="28" max="28" width="12.7109375" customWidth="1"/>
+    <col min="29" max="30" width="11.7109375" customWidth="1"/>
+    <col min="31" max="31" width="13.140625" customWidth="1"/>
+    <col min="32" max="32" width="11.85546875" customWidth="1"/>
+    <col min="37" max="40" width="12.7109375"/>
     <col min="43" max="43" width="9" customWidth="1"/>
-    <col min="44" max="1030" width="8.5546875"/>
+    <col min="44" max="1030" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:43" x14ac:dyDescent="0.25">
       <c r="AK1" s="1" t="s">
         <v>22</v>
       </c>
@@ -1625,7 +1627,7 @@
       <c r="AP1" s="1"/>
       <c r="AQ1" s="1"/>
     </row>
-    <row r="2" spans="1:43" s="4" customFormat="1" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:43" s="4" customFormat="1" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>23</v>
       </c>
@@ -1706,7 +1708,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="3" spans="1:43" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:43" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>43</v>
       </c>
@@ -1757,60 +1759,60 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:43" s="8" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="31" t="s">
+    <row r="4" spans="1:43" s="8" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="33" t="s">
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="E4" s="33"/>
-      <c r="F4" s="34" t="s">
+      <c r="E4" s="29"/>
+      <c r="F4" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="G4" s="34"/>
-      <c r="H4" s="29" t="s">
+      <c r="G4" s="30"/>
+      <c r="H4" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="I4" s="29"/>
-      <c r="J4" s="30" t="s">
+      <c r="I4" s="31"/>
+      <c r="J4" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="K4" s="30"/>
-      <c r="L4" s="29" t="s">
+      <c r="K4" s="32"/>
+      <c r="L4" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="M4" s="29"/>
-      <c r="N4" s="29"/>
-      <c r="O4" s="29"/>
-      <c r="P4" s="29"/>
-      <c r="Q4" s="29"/>
-      <c r="R4" s="29"/>
-      <c r="S4" s="30" t="s">
+      <c r="M4" s="31"/>
+      <c r="N4" s="31"/>
+      <c r="O4" s="31"/>
+      <c r="P4" s="31"/>
+      <c r="Q4" s="31"/>
+      <c r="R4" s="31"/>
+      <c r="S4" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="T4" s="30"/>
-      <c r="U4" s="30"/>
-      <c r="V4" s="28" t="s">
-        <v>65</v>
-      </c>
-      <c r="W4" s="28"/>
-      <c r="X4" s="28"/>
+      <c r="T4" s="32"/>
+      <c r="U4" s="32"/>
+      <c r="V4" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="W4" s="33"/>
+      <c r="X4" s="33"/>
       <c r="Y4" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="Z4" s="31" t="s">
+      <c r="Z4" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="AA4" s="31"/>
-      <c r="AB4" s="31"/>
-      <c r="AC4" s="28" t="s">
+      <c r="AA4" s="28"/>
+      <c r="AB4" s="28"/>
+      <c r="AC4" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="AD4" s="28"/>
-      <c r="AE4" s="28"/>
+      <c r="AD4" s="33"/>
+      <c r="AE4" s="33"/>
       <c r="AF4" s="24" t="s">
         <v>70</v>
       </c>
@@ -1818,17 +1820,17 @@
       <c r="AH4" s="24"/>
       <c r="AI4" s="24"/>
       <c r="AJ4" s="24"/>
-      <c r="AK4" s="32" t="s">
+      <c r="AK4" s="34" t="s">
         <v>68</v>
       </c>
-      <c r="AL4" s="32"/>
-      <c r="AM4" s="32"/>
-      <c r="AN4" s="32"/>
+      <c r="AL4" s="34"/>
+      <c r="AM4" s="34"/>
+      <c r="AN4" s="34"/>
       <c r="AO4" s="17"/>
       <c r="AP4" s="26"/>
       <c r="AQ4" s="23"/>
     </row>
-    <row r="5" spans="1:43" s="10" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:43" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>71</v>
       </c>
@@ -1959,7 +1961,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="6" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>180</v>
       </c>
@@ -2090,7 +2092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>181</v>
       </c>
@@ -2221,7 +2223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>182</v>
       </c>
@@ -2352,7 +2354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>183</v>
       </c>
@@ -2483,7 +2485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>184</v>
       </c>
@@ -2614,7 +2616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>185</v>
       </c>
@@ -2745,7 +2747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>186</v>
       </c>
@@ -2876,7 +2878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>187</v>
       </c>
@@ -3007,7 +3009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>188</v>
       </c>
@@ -3138,7 +3140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>189</v>
       </c>
@@ -3269,7 +3271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>190</v>
       </c>
@@ -3400,7 +3402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>191</v>
       </c>
@@ -3531,7 +3533,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>192</v>
       </c>
@@ -3662,7 +3664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>193</v>
       </c>
@@ -3793,7 +3795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>269</v>
       </c>
@@ -3924,7 +3926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>270</v>
       </c>
@@ -4055,7 +4057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:43" x14ac:dyDescent="0.25">
       <c r="B22" s="22"/>
       <c r="C22" s="11"/>
       <c r="L22" s="27"/>
@@ -4065,7 +4067,7 @@
       <c r="AP22" s="21"/>
       <c r="AQ22" s="21"/>
     </row>
-    <row r="23" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>194</v>
       </c>
@@ -4196,7 +4198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>195</v>
       </c>
@@ -4327,7 +4329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>196</v>
       </c>
@@ -4458,7 +4460,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>197</v>
       </c>
@@ -4589,7 +4591,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>198</v>
       </c>
@@ -4720,7 +4722,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>199</v>
       </c>
@@ -4851,7 +4853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>200</v>
       </c>
@@ -4982,7 +4984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>201</v>
       </c>
@@ -5113,7 +5115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>202</v>
       </c>
@@ -5244,7 +5246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>203</v>
       </c>
@@ -5375,7 +5377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>204</v>
       </c>
@@ -5506,7 +5508,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>205</v>
       </c>
@@ -5637,7 +5639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>206</v>
       </c>
@@ -5768,7 +5770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>207</v>
       </c>
@@ -5899,7 +5901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>208</v>
       </c>
@@ -6030,7 +6032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>209</v>
       </c>
@@ -6161,7 +6163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>210</v>
       </c>
@@ -6292,7 +6294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>211</v>
       </c>
@@ -6423,7 +6425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>271</v>
       </c>
@@ -6554,7 +6556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>272</v>
       </c>
@@ -6685,7 +6687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:43" x14ac:dyDescent="0.25">
       <c r="B43" s="22"/>
       <c r="C43" s="11"/>
       <c r="J43" s="12"/>
@@ -6711,7 +6713,7 @@
       <c r="AP43" s="21"/>
       <c r="AQ43" s="21"/>
     </row>
-    <row r="44" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:43" x14ac:dyDescent="0.25">
       <c r="B44" s="22"/>
       <c r="C44" s="11"/>
       <c r="J44" s="12"/>
@@ -6737,7 +6739,7 @@
       <c r="AP44" s="21"/>
       <c r="AQ44" s="21"/>
     </row>
-    <row r="45" spans="1:43" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:43" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>212</v>
       </c>
@@ -6868,7 +6870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>213</v>
       </c>
@@ -6999,7 +7001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:43" x14ac:dyDescent="0.25">
       <c r="B47" s="22"/>
       <c r="C47" s="11"/>
       <c r="J47" s="12"/>
@@ -7025,7 +7027,7 @@
       <c r="AP47" s="21"/>
       <c r="AQ47" s="21"/>
     </row>
-    <row r="48" spans="1:43" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:43" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>214</v>
       </c>
@@ -7156,7 +7158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>215</v>
       </c>
@@ -7287,7 +7289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>216</v>
       </c>
@@ -7418,7 +7420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>217</v>
       </c>
@@ -7549,7 +7551,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>260</v>
       </c>
@@ -7680,7 +7682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>261</v>
       </c>
@@ -7811,10 +7813,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:43" x14ac:dyDescent="0.25">
       <c r="C54" s="11"/>
     </row>
-    <row r="55" spans="1:43" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:43" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>218</v>
       </c>
@@ -7945,7 +7947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>219</v>
       </c>
@@ -8076,7 +8078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:43" x14ac:dyDescent="0.25">
       <c r="B57" s="22"/>
       <c r="C57" s="11"/>
       <c r="J57" s="12"/>
@@ -8102,7 +8104,7 @@
       <c r="AP57" s="21"/>
       <c r="AQ57" s="21"/>
     </row>
-    <row r="58" spans="1:43" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:43" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>220</v>
       </c>
@@ -8233,7 +8235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>221</v>
       </c>
@@ -8364,7 +8366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>222</v>
       </c>
@@ -8495,7 +8497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>223</v>
       </c>
@@ -8626,7 +8628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>264</v>
       </c>
@@ -8757,7 +8759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>265</v>
       </c>
@@ -8890,17 +8892,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="J4:K4"/>
     <mergeCell ref="AC4:AE4"/>
     <mergeCell ref="L4:R4"/>
     <mergeCell ref="S4:U4"/>
     <mergeCell ref="Z4:AB4"/>
     <mergeCell ref="AK4:AN4"/>
     <mergeCell ref="V4:X4"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="J4:K4"/>
   </mergeCells>
   <dataValidations count="20">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AI6:AI21 AI55:AI63 AI23:AI53">
@@ -8998,7 +9000,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>[1]DropDowns!#REF!</xm:f>
+            <xm:f>'E:\GitHub\PenSim-Projects\Model_Main\IO_M2.1\[RunControl_M2.1.xlsx]DropDowns'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>H18:I19</xm:sqref>
         </x14:dataValidation>
@@ -9012,16 +9014,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:D18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>71</v>
       </c>
@@ -9035,7 +9037,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>206</v>
       </c>
@@ -9049,7 +9051,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>206</v>
       </c>
@@ -9063,7 +9065,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>207</v>
       </c>
@@ -9077,7 +9079,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>207</v>
       </c>
@@ -9091,7 +9093,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>208</v>
       </c>
@@ -9105,7 +9107,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>208</v>
       </c>
@@ -9119,7 +9121,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>209</v>
       </c>
@@ -9133,7 +9135,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>209</v>
       </c>
@@ -9147,7 +9149,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>210</v>
       </c>
@@ -9161,7 +9163,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>210</v>
       </c>
@@ -9175,7 +9177,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>211</v>
       </c>
@@ -9189,7 +9191,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>211</v>
       </c>
@@ -9203,15 +9205,15 @@
         <v>79</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" s="12"/>
       <c r="C16" s="12"/>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="12"/>
       <c r="C17" s="12"/>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="12"/>
       <c r="C18" s="12"/>
     </row>
@@ -9242,9 +9244,9 @@
       <selection activeCell="A3" sqref="A3:D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>71</v>
       </c>
@@ -9258,17 +9260,17 @@
         <v>157</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" s="18"/>
       <c r="C3" s="18"/>
       <c r="D3" s="19"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" s="18"/>
       <c r="C4" s="18"/>
       <c r="D4" s="19"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" s="18"/>
       <c r="C5" s="18"/>
       <c r="D5" s="19"/>
@@ -9286,17 +9288,17 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1025" width="8.5546875"/>
+    <col min="1" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>120</v>
       </c>
@@ -9319,7 +9321,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>80</v>
       </c>
@@ -9356,30 +9358,30 @@
       <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.44140625"/>
+    <col min="1" max="1" width="23.42578125"/>
     <col min="2" max="2" width="5"/>
-    <col min="3" max="3" width="85.44140625"/>
-    <col min="4" max="1025" width="8.5546875"/>
+    <col min="3" max="3" width="85.42578125"/>
+    <col min="4" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>127</v>
       </c>
       <c r="B1" s="3"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>129</v>
       </c>
@@ -9387,12 +9389,12 @@
         <v>130</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>112</v>
       </c>
@@ -9400,7 +9402,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>118</v>
       </c>
@@ -9408,7 +9410,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>133</v>
       </c>
@@ -9416,12 +9418,12 @@
         <v>134</v>
       </c>
     </row>
-    <row r="11" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>115</v>
       </c>
@@ -9429,7 +9431,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>136</v>
       </c>
@@ -9437,7 +9439,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>138</v>
       </c>
@@ -9445,12 +9447,12 @@
         <v>139</v>
       </c>
     </row>
-    <row r="16" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>109</v>
       </c>
@@ -9458,7 +9460,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>141</v>
       </c>
@@ -9466,12 +9468,12 @@
         <v>142</v>
       </c>
     </row>
-    <row r="20" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>109</v>
       </c>
@@ -9479,7 +9481,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>141</v>
       </c>
@@ -9487,12 +9489,12 @@
         <v>142</v>
       </c>
     </row>
-    <row r="24" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="16" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>109</v>
       </c>
@@ -9500,7 +9502,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>141</v>
       </c>
@@ -9508,12 +9510,12 @@
         <v>142</v>
       </c>
     </row>
-    <row r="28" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="16" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>109</v>
       </c>
@@ -9521,7 +9523,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>141</v>
       </c>
@@ -9529,12 +9531,12 @@
         <v>142</v>
       </c>
     </row>
-    <row r="32" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="16" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>117</v>
       </c>
@@ -9542,7 +9544,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>144</v>
       </c>
@@ -9550,12 +9552,12 @@
         <v>145</v>
       </c>
     </row>
-    <row r="36" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="16" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>110</v>
       </c>
@@ -9563,7 +9565,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>147</v>
       </c>
@@ -9571,7 +9573,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>149</v>
       </c>
@@ -9579,7 +9581,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>151</v>
       </c>
@@ -9587,17 +9589,17 @@
         <v>152</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="43" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="16" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>111</v>
       </c>
@@ -9605,12 +9607,12 @@
         <v>153</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>172</v>
       </c>

</xml_diff>